<commit_message>
back: atualizando caminho da api de iniciar o front
</commit_message>
<xml_diff>
--- a/syspzl-api/templates/modelo-auto-de-infracao.xlsx
+++ b/syspzl-api/templates/modelo-auto-de-infracao.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\fiscais_vd\THIAGO_SOUSA\INFRACOES\FLAGRANTE\A-FAZER\0000-MODELO\AUTO\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\sistema_lixo_zero\syspzl-api\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D7FB007-C576-4F5F-9E45-B4A4A0125101}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF699227-0EB4-4E61-9881-8308C4C70DC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookPassword="C13C" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-10910" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Auto de Infração" sheetId="1" r:id="rId1"/>
@@ -918,7 +918,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="164">
+  <cellXfs count="167">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1212,50 +1212,162 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="11" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="166" fontId="11" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="166" fontId="11" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="168" fontId="12" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="168" fontId="12" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="168" fontId="12" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="169" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="169" fontId="13" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="169" fontId="13" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="167" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="167" fontId="13" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="167" fontId="13" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="12" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="170" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="170" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="170" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1267,164 +1379,64 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="165" fontId="12" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="170" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="170" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="170" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="11" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="166" fontId="11" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="166" fontId="11" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="168" fontId="12" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="168" fontId="12" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="168" fontId="12" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="169" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="169" fontId="13" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="169" fontId="13" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="167" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="167" fontId="13" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="167" fontId="13" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -2174,7 +2186,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -2226,7 +2238,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -2431,24 +2443,24 @@
   <dimension ref="A1:AT131"/>
   <sheetViews>
     <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" showRuler="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15:AH15"/>
+      <selection activeCell="B3" sqref="B3:D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="2" defaultRowHeight="11.25" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="2" defaultRowHeight="11.25" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="34" width="2" style="19" customWidth="1"/>
-    <col min="35" max="35" width="1.81640625" style="19" customWidth="1"/>
+    <col min="35" max="35" width="1.85546875" style="19" customWidth="1"/>
     <col min="36" max="40" width="2" style="19" customWidth="1"/>
-    <col min="41" max="41" width="2.453125" style="19" customWidth="1"/>
+    <col min="41" max="41" width="2.42578125" style="19" customWidth="1"/>
     <col min="42" max="47" width="2" style="19" customWidth="1"/>
     <col min="48" max="50" width="2" style="19"/>
-    <col min="51" max="51" width="6.54296875" style="19" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="6.5703125" style="19" bestFit="1" customWidth="1"/>
     <col min="52" max="52" width="2" style="19"/>
-    <col min="53" max="53" width="6.54296875" style="19" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="6.5703125" style="19" bestFit="1" customWidth="1"/>
     <col min="54" max="16384" width="2" style="19"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:46" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:46" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
@@ -2498,7 +2510,7 @@
       <c r="AS1" s="18"/>
       <c r="AT1" s="18"/>
     </row>
-    <row r="2" spans="1:46" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:46" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2" s="20" t="s">
         <v>1</v>
       </c>
@@ -2548,17 +2560,17 @@
       <c r="AS2" s="22"/>
       <c r="AT2" s="22"/>
     </row>
-    <row r="3" spans="1:46" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="136"/>
-      <c r="C3" s="137"/>
-      <c r="D3" s="138"/>
+    <row r="3" spans="1:46" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B3" s="139"/>
+      <c r="C3" s="140"/>
+      <c r="D3" s="141"/>
       <c r="E3" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="139"/>
-      <c r="G3" s="140"/>
-      <c r="H3" s="140"/>
-      <c r="I3" s="141"/>
+      <c r="F3" s="142"/>
+      <c r="G3" s="143"/>
+      <c r="H3" s="143"/>
+      <c r="I3" s="144"/>
       <c r="J3" s="21"/>
       <c r="K3" s="21"/>
       <c r="L3" s="21"/>
@@ -2599,7 +2611,7 @@
       <c r="AS3" s="26"/>
       <c r="AT3" s="27"/>
     </row>
-    <row r="4" spans="1:46" ht="2.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:46" ht="2.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="21"/>
       <c r="B4" s="21"/>
       <c r="C4" s="21"/>
@@ -2647,7 +2659,7 @@
       <c r="AS4" s="21"/>
       <c r="AT4" s="21"/>
     </row>
-    <row r="5" spans="1:46" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:46" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="28" t="s">
         <v>4</v>
       </c>
@@ -2699,55 +2711,55 @@
       <c r="AS5" s="30"/>
       <c r="AT5" s="31"/>
     </row>
-    <row r="6" spans="1:46" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:46" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="32"/>
-      <c r="B6" s="121"/>
-      <c r="C6" s="131"/>
-      <c r="D6" s="131"/>
-      <c r="E6" s="131"/>
-      <c r="F6" s="131"/>
-      <c r="G6" s="131"/>
-      <c r="H6" s="131"/>
-      <c r="I6" s="131"/>
-      <c r="J6" s="131"/>
-      <c r="K6" s="131"/>
-      <c r="L6" s="131"/>
-      <c r="M6" s="131"/>
-      <c r="N6" s="131"/>
-      <c r="O6" s="131"/>
-      <c r="P6" s="131"/>
-      <c r="Q6" s="131"/>
-      <c r="R6" s="131"/>
-      <c r="S6" s="131"/>
-      <c r="T6" s="131"/>
-      <c r="U6" s="131"/>
-      <c r="V6" s="131"/>
-      <c r="W6" s="131"/>
-      <c r="X6" s="131"/>
-      <c r="Y6" s="131"/>
-      <c r="Z6" s="131"/>
-      <c r="AA6" s="131"/>
-      <c r="AB6" s="131"/>
-      <c r="AC6" s="131"/>
-      <c r="AD6" s="131"/>
-      <c r="AE6" s="131"/>
-      <c r="AF6" s="131"/>
-      <c r="AG6" s="131"/>
-      <c r="AH6" s="131"/>
-      <c r="AI6" s="131"/>
-      <c r="AJ6" s="131"/>
-      <c r="AK6" s="131"/>
-      <c r="AL6" s="131"/>
-      <c r="AM6" s="131"/>
-      <c r="AN6" s="131"/>
-      <c r="AO6" s="131"/>
-      <c r="AP6" s="131"/>
-      <c r="AQ6" s="131"/>
-      <c r="AR6" s="131"/>
-      <c r="AS6" s="132"/>
+      <c r="B6" s="119"/>
+      <c r="C6" s="122"/>
+      <c r="D6" s="122"/>
+      <c r="E6" s="122"/>
+      <c r="F6" s="122"/>
+      <c r="G6" s="122"/>
+      <c r="H6" s="122"/>
+      <c r="I6" s="122"/>
+      <c r="J6" s="122"/>
+      <c r="K6" s="122"/>
+      <c r="L6" s="122"/>
+      <c r="M6" s="122"/>
+      <c r="N6" s="122"/>
+      <c r="O6" s="122"/>
+      <c r="P6" s="122"/>
+      <c r="Q6" s="122"/>
+      <c r="R6" s="122"/>
+      <c r="S6" s="122"/>
+      <c r="T6" s="122"/>
+      <c r="U6" s="122"/>
+      <c r="V6" s="122"/>
+      <c r="W6" s="122"/>
+      <c r="X6" s="122"/>
+      <c r="Y6" s="122"/>
+      <c r="Z6" s="122"/>
+      <c r="AA6" s="122"/>
+      <c r="AB6" s="122"/>
+      <c r="AC6" s="122"/>
+      <c r="AD6" s="122"/>
+      <c r="AE6" s="122"/>
+      <c r="AF6" s="122"/>
+      <c r="AG6" s="122"/>
+      <c r="AH6" s="122"/>
+      <c r="AI6" s="122"/>
+      <c r="AJ6" s="122"/>
+      <c r="AK6" s="122"/>
+      <c r="AL6" s="122"/>
+      <c r="AM6" s="122"/>
+      <c r="AN6" s="122"/>
+      <c r="AO6" s="122"/>
+      <c r="AP6" s="122"/>
+      <c r="AQ6" s="122"/>
+      <c r="AR6" s="122"/>
+      <c r="AS6" s="123"/>
       <c r="AT6" s="33"/>
     </row>
-    <row r="7" spans="1:46" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:46" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="32"/>
       <c r="B7" s="22" t="s">
         <v>121</v>
@@ -2797,55 +2809,55 @@
       <c r="AS7" s="13"/>
       <c r="AT7" s="33"/>
     </row>
-    <row r="8" spans="1:46" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:46" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="34"/>
-      <c r="B8" s="121"/>
-      <c r="C8" s="131"/>
-      <c r="D8" s="131"/>
-      <c r="E8" s="131"/>
-      <c r="F8" s="131"/>
-      <c r="G8" s="131"/>
-      <c r="H8" s="131"/>
-      <c r="I8" s="131"/>
-      <c r="J8" s="131"/>
-      <c r="K8" s="131"/>
-      <c r="L8" s="131"/>
-      <c r="M8" s="131"/>
-      <c r="N8" s="131"/>
-      <c r="O8" s="131"/>
-      <c r="P8" s="131"/>
-      <c r="Q8" s="131"/>
-      <c r="R8" s="131"/>
-      <c r="S8" s="131"/>
-      <c r="T8" s="131"/>
-      <c r="U8" s="131"/>
-      <c r="V8" s="131"/>
-      <c r="W8" s="131"/>
-      <c r="X8" s="131"/>
-      <c r="Y8" s="131"/>
-      <c r="Z8" s="131"/>
-      <c r="AA8" s="131"/>
-      <c r="AB8" s="131"/>
-      <c r="AC8" s="131"/>
-      <c r="AD8" s="131"/>
-      <c r="AE8" s="131"/>
-      <c r="AF8" s="131"/>
-      <c r="AG8" s="131"/>
-      <c r="AH8" s="131"/>
-      <c r="AI8" s="131"/>
-      <c r="AJ8" s="131"/>
-      <c r="AK8" s="131"/>
-      <c r="AL8" s="131"/>
-      <c r="AM8" s="131"/>
-      <c r="AN8" s="131"/>
-      <c r="AO8" s="131"/>
-      <c r="AP8" s="131"/>
-      <c r="AQ8" s="131"/>
-      <c r="AR8" s="131"/>
-      <c r="AS8" s="132"/>
+      <c r="B8" s="119"/>
+      <c r="C8" s="122"/>
+      <c r="D8" s="122"/>
+      <c r="E8" s="122"/>
+      <c r="F8" s="122"/>
+      <c r="G8" s="122"/>
+      <c r="H8" s="122"/>
+      <c r="I8" s="122"/>
+      <c r="J8" s="122"/>
+      <c r="K8" s="122"/>
+      <c r="L8" s="122"/>
+      <c r="M8" s="122"/>
+      <c r="N8" s="122"/>
+      <c r="O8" s="122"/>
+      <c r="P8" s="122"/>
+      <c r="Q8" s="122"/>
+      <c r="R8" s="122"/>
+      <c r="S8" s="122"/>
+      <c r="T8" s="122"/>
+      <c r="U8" s="122"/>
+      <c r="V8" s="122"/>
+      <c r="W8" s="122"/>
+      <c r="X8" s="122"/>
+      <c r="Y8" s="122"/>
+      <c r="Z8" s="122"/>
+      <c r="AA8" s="122"/>
+      <c r="AB8" s="122"/>
+      <c r="AC8" s="122"/>
+      <c r="AD8" s="122"/>
+      <c r="AE8" s="122"/>
+      <c r="AF8" s="122"/>
+      <c r="AG8" s="122"/>
+      <c r="AH8" s="122"/>
+      <c r="AI8" s="122"/>
+      <c r="AJ8" s="122"/>
+      <c r="AK8" s="122"/>
+      <c r="AL8" s="122"/>
+      <c r="AM8" s="122"/>
+      <c r="AN8" s="122"/>
+      <c r="AO8" s="122"/>
+      <c r="AP8" s="122"/>
+      <c r="AQ8" s="122"/>
+      <c r="AR8" s="122"/>
+      <c r="AS8" s="123"/>
       <c r="AT8" s="33"/>
     </row>
-    <row r="9" spans="1:46" ht="2.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:46" ht="2.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="34"/>
       <c r="B9" s="13"/>
       <c r="C9" s="13"/>
@@ -2893,7 +2905,7 @@
       <c r="AS9" s="13"/>
       <c r="AT9" s="33"/>
     </row>
-    <row r="10" spans="1:46" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:46" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="32" t="s">
         <v>5</v>
       </c>
@@ -2945,20 +2957,20 @@
       <c r="AS10" s="13"/>
       <c r="AT10" s="33"/>
     </row>
-    <row r="11" spans="1:46" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:46" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="34"/>
-      <c r="B11" s="133"/>
-      <c r="C11" s="134"/>
-      <c r="D11" s="134"/>
-      <c r="E11" s="134"/>
-      <c r="F11" s="134"/>
-      <c r="G11" s="134"/>
-      <c r="H11" s="134"/>
-      <c r="I11" s="134"/>
-      <c r="J11" s="134"/>
-      <c r="K11" s="134"/>
-      <c r="L11" s="134"/>
-      <c r="M11" s="135"/>
+      <c r="B11" s="136"/>
+      <c r="C11" s="137"/>
+      <c r="D11" s="137"/>
+      <c r="E11" s="137"/>
+      <c r="F11" s="137"/>
+      <c r="G11" s="137"/>
+      <c r="H11" s="137"/>
+      <c r="I11" s="137"/>
+      <c r="J11" s="137"/>
+      <c r="K11" s="137"/>
+      <c r="L11" s="137"/>
+      <c r="M11" s="138"/>
       <c r="N11" s="13"/>
       <c r="Z11" s="35"/>
       <c r="AA11" s="36"/>
@@ -2968,21 +2980,21 @@
       <c r="AE11" s="36"/>
       <c r="AF11" s="36"/>
       <c r="AG11" s="37"/>
-      <c r="AH11" s="146"/>
-      <c r="AI11" s="147"/>
-      <c r="AJ11" s="147"/>
-      <c r="AK11" s="147"/>
-      <c r="AL11" s="147"/>
-      <c r="AM11" s="147"/>
-      <c r="AN11" s="147"/>
-      <c r="AO11" s="147"/>
-      <c r="AP11" s="147"/>
-      <c r="AQ11" s="147"/>
-      <c r="AR11" s="147"/>
-      <c r="AS11" s="148"/>
+      <c r="AH11" s="104"/>
+      <c r="AI11" s="105"/>
+      <c r="AJ11" s="105"/>
+      <c r="AK11" s="105"/>
+      <c r="AL11" s="105"/>
+      <c r="AM11" s="105"/>
+      <c r="AN11" s="105"/>
+      <c r="AO11" s="105"/>
+      <c r="AP11" s="105"/>
+      <c r="AQ11" s="105"/>
+      <c r="AR11" s="105"/>
+      <c r="AS11" s="106"/>
       <c r="AT11" s="33"/>
     </row>
-    <row r="12" spans="1:46" ht="2.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:46" ht="2.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="34"/>
       <c r="B12" s="13"/>
       <c r="C12" s="13"/>
@@ -3030,7 +3042,7 @@
       <c r="AS12" s="13"/>
       <c r="AT12" s="33"/>
     </row>
-    <row r="13" spans="1:46" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:46" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="32" t="s">
         <v>8</v>
       </c>
@@ -3082,7 +3094,7 @@
       <c r="AS13" s="39"/>
       <c r="AT13" s="33"/>
     </row>
-    <row r="14" spans="1:46" ht="2.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:46" ht="2.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="40"/>
       <c r="B14" s="22"/>
       <c r="C14" s="13"/>
@@ -3130,59 +3142,59 @@
       <c r="AS14" s="13"/>
       <c r="AT14" s="33"/>
     </row>
-    <row r="15" spans="1:46" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:46" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="34"/>
-      <c r="B15" s="114" t="s">
+      <c r="B15" s="116" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="125"/>
-      <c r="D15" s="121"/>
-      <c r="E15" s="122"/>
-      <c r="F15" s="122"/>
-      <c r="G15" s="122"/>
-      <c r="H15" s="122"/>
-      <c r="I15" s="122"/>
-      <c r="J15" s="122"/>
-      <c r="K15" s="122"/>
-      <c r="L15" s="122"/>
-      <c r="M15" s="122"/>
-      <c r="N15" s="122"/>
-      <c r="O15" s="122"/>
-      <c r="P15" s="122"/>
-      <c r="Q15" s="122"/>
-      <c r="R15" s="122"/>
-      <c r="S15" s="122"/>
-      <c r="T15" s="122"/>
-      <c r="U15" s="122"/>
-      <c r="V15" s="122"/>
-      <c r="W15" s="122"/>
-      <c r="X15" s="122"/>
-      <c r="Y15" s="122"/>
-      <c r="Z15" s="122"/>
-      <c r="AA15" s="122"/>
-      <c r="AB15" s="122"/>
-      <c r="AC15" s="122"/>
-      <c r="AD15" s="122"/>
-      <c r="AE15" s="122"/>
-      <c r="AF15" s="122"/>
-      <c r="AG15" s="122"/>
-      <c r="AH15" s="123"/>
+      <c r="C15" s="117"/>
+      <c r="D15" s="119"/>
+      <c r="E15" s="120"/>
+      <c r="F15" s="120"/>
+      <c r="G15" s="120"/>
+      <c r="H15" s="120"/>
+      <c r="I15" s="120"/>
+      <c r="J15" s="120"/>
+      <c r="K15" s="120"/>
+      <c r="L15" s="120"/>
+      <c r="M15" s="120"/>
+      <c r="N15" s="120"/>
+      <c r="O15" s="120"/>
+      <c r="P15" s="120"/>
+      <c r="Q15" s="120"/>
+      <c r="R15" s="120"/>
+      <c r="S15" s="120"/>
+      <c r="T15" s="120"/>
+      <c r="U15" s="120"/>
+      <c r="V15" s="120"/>
+      <c r="W15" s="120"/>
+      <c r="X15" s="120"/>
+      <c r="Y15" s="120"/>
+      <c r="Z15" s="120"/>
+      <c r="AA15" s="120"/>
+      <c r="AB15" s="120"/>
+      <c r="AC15" s="120"/>
+      <c r="AD15" s="120"/>
+      <c r="AE15" s="120"/>
+      <c r="AF15" s="120"/>
+      <c r="AG15" s="120"/>
+      <c r="AH15" s="121"/>
       <c r="AI15" s="39"/>
       <c r="AJ15" s="36" t="s">
         <v>123</v>
       </c>
       <c r="AK15" s="39"/>
-      <c r="AL15" s="161"/>
-      <c r="AM15" s="162"/>
-      <c r="AN15" s="162"/>
-      <c r="AO15" s="162"/>
-      <c r="AP15" s="162"/>
-      <c r="AQ15" s="162"/>
-      <c r="AR15" s="162"/>
-      <c r="AS15" s="163"/>
+      <c r="AL15" s="130"/>
+      <c r="AM15" s="131"/>
+      <c r="AN15" s="131"/>
+      <c r="AO15" s="131"/>
+      <c r="AP15" s="131"/>
+      <c r="AQ15" s="131"/>
+      <c r="AR15" s="131"/>
+      <c r="AS15" s="132"/>
       <c r="AT15" s="33"/>
     </row>
-    <row r="16" spans="1:46" ht="2.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:46" ht="2.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="34"/>
       <c r="B16" s="21"/>
       <c r="C16" s="21"/>
@@ -3230,61 +3242,61 @@
       <c r="AS16" s="21"/>
       <c r="AT16" s="33"/>
     </row>
-    <row r="17" spans="1:46" ht="11.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:46" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="34"/>
-      <c r="B17" s="114" t="s">
+      <c r="B17" s="116" t="s">
         <v>11</v>
       </c>
-      <c r="C17" s="124"/>
-      <c r="D17" s="125"/>
-      <c r="E17" s="121"/>
-      <c r="F17" s="122"/>
-      <c r="G17" s="122"/>
-      <c r="H17" s="122"/>
-      <c r="I17" s="122"/>
-      <c r="J17" s="123"/>
-      <c r="K17" s="114" t="s">
+      <c r="C17" s="118"/>
+      <c r="D17" s="117"/>
+      <c r="E17" s="164"/>
+      <c r="F17" s="165"/>
+      <c r="G17" s="165"/>
+      <c r="H17" s="165"/>
+      <c r="I17" s="165"/>
+      <c r="J17" s="166"/>
+      <c r="K17" s="116" t="s">
         <v>12</v>
       </c>
-      <c r="L17" s="124"/>
-      <c r="M17" s="125"/>
-      <c r="N17" s="121"/>
-      <c r="O17" s="131"/>
-      <c r="P17" s="131"/>
-      <c r="Q17" s="131"/>
-      <c r="R17" s="131"/>
-      <c r="S17" s="131"/>
-      <c r="T17" s="131"/>
-      <c r="U17" s="131"/>
-      <c r="V17" s="131"/>
-      <c r="W17" s="131"/>
-      <c r="X17" s="131"/>
-      <c r="Y17" s="131"/>
-      <c r="Z17" s="131"/>
-      <c r="AA17" s="131"/>
-      <c r="AB17" s="131"/>
-      <c r="AC17" s="131"/>
-      <c r="AD17" s="131"/>
-      <c r="AE17" s="131"/>
-      <c r="AF17" s="131"/>
-      <c r="AG17" s="131"/>
-      <c r="AH17" s="132"/>
+      <c r="L17" s="118"/>
+      <c r="M17" s="117"/>
+      <c r="N17" s="119"/>
+      <c r="O17" s="122"/>
+      <c r="P17" s="122"/>
+      <c r="Q17" s="122"/>
+      <c r="R17" s="122"/>
+      <c r="S17" s="122"/>
+      <c r="T17" s="122"/>
+      <c r="U17" s="122"/>
+      <c r="V17" s="122"/>
+      <c r="W17" s="122"/>
+      <c r="X17" s="122"/>
+      <c r="Y17" s="122"/>
+      <c r="Z17" s="122"/>
+      <c r="AA17" s="122"/>
+      <c r="AB17" s="122"/>
+      <c r="AC17" s="122"/>
+      <c r="AD17" s="122"/>
+      <c r="AE17" s="122"/>
+      <c r="AF17" s="122"/>
+      <c r="AG17" s="122"/>
+      <c r="AH17" s="123"/>
       <c r="AI17" s="13"/>
       <c r="AJ17" s="14" t="s">
         <v>104</v>
       </c>
       <c r="AK17" s="14"/>
-      <c r="AL17" s="126"/>
-      <c r="AM17" s="127"/>
-      <c r="AN17" s="127"/>
-      <c r="AO17" s="127"/>
-      <c r="AP17" s="127"/>
-      <c r="AQ17" s="127"/>
-      <c r="AR17" s="127"/>
-      <c r="AS17" s="128"/>
+      <c r="AL17" s="124"/>
+      <c r="AM17" s="125"/>
+      <c r="AN17" s="125"/>
+      <c r="AO17" s="125"/>
+      <c r="AP17" s="125"/>
+      <c r="AQ17" s="125"/>
+      <c r="AR17" s="125"/>
+      <c r="AS17" s="126"/>
       <c r="AT17" s="33"/>
     </row>
-    <row r="18" spans="1:46" ht="2.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:46" ht="2.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="34"/>
       <c r="B18" s="13"/>
       <c r="C18" s="13"/>
@@ -3332,7 +3344,7 @@
       <c r="AS18" s="13"/>
       <c r="AT18" s="33"/>
     </row>
-    <row r="19" spans="1:46" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:46" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="28" t="s">
         <v>13</v>
       </c>
@@ -3396,7 +3408,7 @@
       <c r="AS19" s="30"/>
       <c r="AT19" s="31"/>
     </row>
-    <row r="20" spans="1:46" ht="2.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:46" ht="2.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="34"/>
       <c r="B20" s="13"/>
       <c r="C20" s="13"/>
@@ -3444,14 +3456,14 @@
       <c r="AS20" s="13"/>
       <c r="AT20" s="33"/>
     </row>
-    <row r="21" spans="1:46" ht="11.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:46" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="44"/>
-      <c r="B21" s="155"/>
-      <c r="C21" s="156"/>
-      <c r="D21" s="156"/>
-      <c r="E21" s="156"/>
-      <c r="F21" s="156"/>
-      <c r="G21" s="157"/>
+      <c r="B21" s="113"/>
+      <c r="C21" s="114"/>
+      <c r="D21" s="114"/>
+      <c r="E21" s="114"/>
+      <c r="F21" s="114"/>
+      <c r="G21" s="115"/>
       <c r="H21" s="13"/>
       <c r="I21" s="13"/>
       <c r="J21" s="13"/>
@@ -3463,10 +3475,10 @@
       <c r="P21" s="21"/>
       <c r="Q21" s="21"/>
       <c r="R21" s="21"/>
-      <c r="S21" s="158"/>
-      <c r="T21" s="159"/>
-      <c r="U21" s="159"/>
-      <c r="V21" s="160"/>
+      <c r="S21" s="127"/>
+      <c r="T21" s="128"/>
+      <c r="U21" s="128"/>
+      <c r="V21" s="129"/>
       <c r="W21" s="13"/>
       <c r="X21" s="13"/>
       <c r="Y21" s="13"/>
@@ -3475,24 +3487,24 @@
       <c r="AB21" s="21"/>
       <c r="AC21" s="21"/>
       <c r="AD21" s="21"/>
-      <c r="AE21" s="149"/>
-      <c r="AF21" s="150"/>
-      <c r="AG21" s="150"/>
-      <c r="AH21" s="150"/>
-      <c r="AI21" s="150"/>
-      <c r="AJ21" s="150"/>
-      <c r="AK21" s="150"/>
-      <c r="AL21" s="150"/>
-      <c r="AM21" s="150"/>
-      <c r="AN21" s="151"/>
+      <c r="AE21" s="107"/>
+      <c r="AF21" s="108"/>
+      <c r="AG21" s="108"/>
+      <c r="AH21" s="108"/>
+      <c r="AI21" s="108"/>
+      <c r="AJ21" s="108"/>
+      <c r="AK21" s="108"/>
+      <c r="AL21" s="108"/>
+      <c r="AM21" s="108"/>
+      <c r="AN21" s="109"/>
       <c r="AO21" s="36"/>
-      <c r="AP21" s="152"/>
-      <c r="AQ21" s="153"/>
-      <c r="AR21" s="153"/>
-      <c r="AS21" s="154"/>
+      <c r="AP21" s="110"/>
+      <c r="AQ21" s="111"/>
+      <c r="AR21" s="111"/>
+      <c r="AS21" s="112"/>
       <c r="AT21" s="33"/>
     </row>
-    <row r="22" spans="1:46" ht="2.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:46" ht="2.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="34"/>
       <c r="B22" s="13"/>
       <c r="C22" s="13"/>
@@ -3540,7 +3552,7 @@
       <c r="AS22" s="13"/>
       <c r="AT22" s="33"/>
     </row>
-    <row r="23" spans="1:46" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:46" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="32" t="s">
         <v>24</v>
       </c>
@@ -3592,57 +3604,57 @@
       <c r="AS23" s="13"/>
       <c r="AT23" s="33"/>
     </row>
-    <row r="24" spans="1:46" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:46" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="34"/>
-      <c r="B24" s="114" t="s">
+      <c r="B24" s="116" t="s">
         <v>10</v>
       </c>
-      <c r="C24" s="125"/>
-      <c r="D24" s="121"/>
-      <c r="E24" s="122"/>
-      <c r="F24" s="122"/>
-      <c r="G24" s="122"/>
-      <c r="H24" s="122"/>
-      <c r="I24" s="122"/>
-      <c r="J24" s="122"/>
-      <c r="K24" s="122"/>
-      <c r="L24" s="122"/>
-      <c r="M24" s="122"/>
-      <c r="N24" s="122"/>
-      <c r="O24" s="122"/>
-      <c r="P24" s="122"/>
-      <c r="Q24" s="122"/>
-      <c r="R24" s="122"/>
-      <c r="S24" s="122"/>
-      <c r="T24" s="122"/>
-      <c r="U24" s="122"/>
-      <c r="V24" s="122"/>
-      <c r="W24" s="122"/>
-      <c r="X24" s="122"/>
-      <c r="Y24" s="122"/>
-      <c r="Z24" s="122"/>
-      <c r="AA24" s="122"/>
-      <c r="AB24" s="122"/>
-      <c r="AC24" s="122"/>
-      <c r="AD24" s="122"/>
-      <c r="AE24" s="122"/>
-      <c r="AF24" s="122"/>
-      <c r="AG24" s="122"/>
-      <c r="AH24" s="122"/>
-      <c r="AI24" s="122"/>
-      <c r="AJ24" s="122"/>
-      <c r="AK24" s="122"/>
-      <c r="AL24" s="122"/>
-      <c r="AM24" s="122"/>
-      <c r="AN24" s="122"/>
-      <c r="AO24" s="122"/>
-      <c r="AP24" s="122"/>
-      <c r="AQ24" s="122"/>
-      <c r="AR24" s="122"/>
-      <c r="AS24" s="123"/>
+      <c r="C24" s="117"/>
+      <c r="D24" s="119"/>
+      <c r="E24" s="120"/>
+      <c r="F24" s="120"/>
+      <c r="G24" s="120"/>
+      <c r="H24" s="120"/>
+      <c r="I24" s="120"/>
+      <c r="J24" s="120"/>
+      <c r="K24" s="120"/>
+      <c r="L24" s="120"/>
+      <c r="M24" s="120"/>
+      <c r="N24" s="120"/>
+      <c r="O24" s="120"/>
+      <c r="P24" s="120"/>
+      <c r="Q24" s="120"/>
+      <c r="R24" s="120"/>
+      <c r="S24" s="120"/>
+      <c r="T24" s="120"/>
+      <c r="U24" s="120"/>
+      <c r="V24" s="120"/>
+      <c r="W24" s="120"/>
+      <c r="X24" s="120"/>
+      <c r="Y24" s="120"/>
+      <c r="Z24" s="120"/>
+      <c r="AA24" s="120"/>
+      <c r="AB24" s="120"/>
+      <c r="AC24" s="120"/>
+      <c r="AD24" s="120"/>
+      <c r="AE24" s="120"/>
+      <c r="AF24" s="120"/>
+      <c r="AG24" s="120"/>
+      <c r="AH24" s="120"/>
+      <c r="AI24" s="120"/>
+      <c r="AJ24" s="120"/>
+      <c r="AK24" s="120"/>
+      <c r="AL24" s="120"/>
+      <c r="AM24" s="120"/>
+      <c r="AN24" s="120"/>
+      <c r="AO24" s="120"/>
+      <c r="AP24" s="120"/>
+      <c r="AQ24" s="120"/>
+      <c r="AR24" s="120"/>
+      <c r="AS24" s="121"/>
       <c r="AT24" s="33"/>
     </row>
-    <row r="25" spans="1:46" ht="2.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:46" ht="2.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="34"/>
       <c r="B25" s="14"/>
       <c r="C25" s="14"/>
@@ -3690,61 +3702,61 @@
       <c r="AS25" s="13"/>
       <c r="AT25" s="33"/>
     </row>
-    <row r="26" spans="1:46" ht="11.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:46" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="34"/>
-      <c r="B26" s="114" t="s">
+      <c r="B26" s="116" t="s">
         <v>11</v>
       </c>
-      <c r="C26" s="124"/>
-      <c r="D26" s="125"/>
-      <c r="E26" s="121"/>
-      <c r="F26" s="122"/>
-      <c r="G26" s="122"/>
-      <c r="H26" s="122"/>
-      <c r="I26" s="122"/>
-      <c r="J26" s="123"/>
-      <c r="K26" s="114" t="s">
+      <c r="C26" s="118"/>
+      <c r="D26" s="117"/>
+      <c r="E26" s="119"/>
+      <c r="F26" s="120"/>
+      <c r="G26" s="120"/>
+      <c r="H26" s="120"/>
+      <c r="I26" s="120"/>
+      <c r="J26" s="121"/>
+      <c r="K26" s="116" t="s">
         <v>12</v>
       </c>
-      <c r="L26" s="124"/>
-      <c r="M26" s="125"/>
-      <c r="N26" s="121"/>
-      <c r="O26" s="122"/>
-      <c r="P26" s="122"/>
-      <c r="Q26" s="122"/>
-      <c r="R26" s="122"/>
-      <c r="S26" s="122"/>
-      <c r="T26" s="122"/>
-      <c r="U26" s="122"/>
-      <c r="V26" s="122"/>
-      <c r="W26" s="122"/>
-      <c r="X26" s="122"/>
-      <c r="Y26" s="122"/>
-      <c r="Z26" s="122"/>
-      <c r="AA26" s="122"/>
-      <c r="AB26" s="122"/>
-      <c r="AC26" s="122"/>
-      <c r="AD26" s="122"/>
-      <c r="AE26" s="122"/>
-      <c r="AF26" s="122"/>
-      <c r="AG26" s="122"/>
-      <c r="AH26" s="123"/>
+      <c r="L26" s="118"/>
+      <c r="M26" s="117"/>
+      <c r="N26" s="119"/>
+      <c r="O26" s="120"/>
+      <c r="P26" s="120"/>
+      <c r="Q26" s="120"/>
+      <c r="R26" s="120"/>
+      <c r="S26" s="120"/>
+      <c r="T26" s="120"/>
+      <c r="U26" s="120"/>
+      <c r="V26" s="120"/>
+      <c r="W26" s="120"/>
+      <c r="X26" s="120"/>
+      <c r="Y26" s="120"/>
+      <c r="Z26" s="120"/>
+      <c r="AA26" s="120"/>
+      <c r="AB26" s="120"/>
+      <c r="AC26" s="120"/>
+      <c r="AD26" s="120"/>
+      <c r="AE26" s="120"/>
+      <c r="AF26" s="120"/>
+      <c r="AG26" s="120"/>
+      <c r="AH26" s="121"/>
       <c r="AI26" s="13"/>
       <c r="AJ26" s="14" t="s">
         <v>104</v>
       </c>
       <c r="AK26" s="14"/>
-      <c r="AL26" s="126"/>
-      <c r="AM26" s="127"/>
-      <c r="AN26" s="127"/>
-      <c r="AO26" s="127"/>
-      <c r="AP26" s="127"/>
-      <c r="AQ26" s="127"/>
-      <c r="AR26" s="127"/>
-      <c r="AS26" s="128"/>
+      <c r="AL26" s="124"/>
+      <c r="AM26" s="125"/>
+      <c r="AN26" s="125"/>
+      <c r="AO26" s="125"/>
+      <c r="AP26" s="125"/>
+      <c r="AQ26" s="125"/>
+      <c r="AR26" s="125"/>
+      <c r="AS26" s="126"/>
       <c r="AT26" s="33"/>
     </row>
-    <row r="27" spans="1:46" ht="2.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:46" ht="2.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="34"/>
       <c r="B27" s="13"/>
       <c r="C27" s="13"/>
@@ -3792,7 +3804,7 @@
       <c r="AS27" s="13"/>
       <c r="AT27" s="33"/>
     </row>
-    <row r="28" spans="1:46" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:46" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="28" t="s">
         <v>26</v>
       </c>
@@ -3844,7 +3856,7 @@
       <c r="AS28" s="30"/>
       <c r="AT28" s="31"/>
     </row>
-    <row r="29" spans="1:46" ht="2.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:46" ht="2.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="40"/>
       <c r="B29" s="22"/>
       <c r="C29" s="13"/>
@@ -3892,7 +3904,7 @@
       <c r="AS29" s="13"/>
       <c r="AT29" s="33"/>
     </row>
-    <row r="30" spans="1:46" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:46" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="34"/>
       <c r="B30" s="1"/>
       <c r="C30" s="13" t="s">
@@ -3942,7 +3954,7 @@
       <c r="AQ30" s="13"/>
       <c r="AT30" s="46"/>
     </row>
-    <row r="31" spans="1:46" ht="2.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:46" ht="2.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="34"/>
       <c r="B31" s="13"/>
       <c r="C31" s="13"/>
@@ -3988,7 +4000,7 @@
       <c r="AQ31" s="13"/>
       <c r="AT31" s="46"/>
     </row>
-    <row r="32" spans="1:46" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:46" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="34"/>
       <c r="B32" s="1"/>
       <c r="C32" s="13" t="s">
@@ -4038,7 +4050,7 @@
       <c r="AQ32" s="13"/>
       <c r="AT32" s="46"/>
     </row>
-    <row r="33" spans="1:46" ht="2.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:46" ht="2.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="34"/>
       <c r="B33" s="13"/>
       <c r="C33" s="13"/>
@@ -4084,7 +4096,7 @@
       <c r="AQ33" s="13"/>
       <c r="AT33" s="46"/>
     </row>
-    <row r="34" spans="1:46" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:46" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="34"/>
       <c r="B34" s="1"/>
       <c r="C34" s="13" t="s">
@@ -4134,7 +4146,7 @@
       <c r="AQ34" s="13"/>
       <c r="AT34" s="46"/>
     </row>
-    <row r="35" spans="1:46" ht="2.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:46" ht="2.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="34"/>
       <c r="B35" s="13"/>
       <c r="C35" s="13"/>
@@ -4180,7 +4192,7 @@
       <c r="AQ35" s="13"/>
       <c r="AT35" s="46"/>
     </row>
-    <row r="36" spans="1:46" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:46" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="34"/>
       <c r="B36" s="1"/>
       <c r="C36" s="13" t="s">
@@ -4230,7 +4242,7 @@
       <c r="AQ36" s="13"/>
       <c r="AT36" s="46"/>
     </row>
-    <row r="37" spans="1:46" ht="2.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:46" ht="2.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="34"/>
       <c r="B37" s="13"/>
       <c r="C37" s="13"/>
@@ -4276,7 +4288,7 @@
       <c r="AQ37" s="13"/>
       <c r="AT37" s="46"/>
     </row>
-    <row r="38" spans="1:46" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:46" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="34"/>
       <c r="B38" s="1"/>
       <c r="C38" s="13" t="s">
@@ -4326,7 +4338,7 @@
       <c r="AQ38" s="13"/>
       <c r="AT38" s="46"/>
     </row>
-    <row r="39" spans="1:46" ht="2.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:46" ht="2.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="34"/>
       <c r="B39" s="13"/>
       <c r="C39" s="13"/>
@@ -4374,7 +4386,7 @@
       <c r="AS39" s="13"/>
       <c r="AT39" s="33"/>
     </row>
-    <row r="40" spans="1:46" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:46" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="34"/>
       <c r="B40" s="1"/>
       <c r="C40" s="13" t="s">
@@ -4382,49 +4394,49 @@
       </c>
       <c r="D40" s="13"/>
       <c r="E40" s="13"/>
-      <c r="F40" s="122"/>
-      <c r="G40" s="122"/>
-      <c r="H40" s="122"/>
-      <c r="I40" s="122"/>
-      <c r="J40" s="122"/>
-      <c r="K40" s="122"/>
-      <c r="L40" s="122"/>
-      <c r="M40" s="122"/>
-      <c r="N40" s="122"/>
-      <c r="O40" s="122"/>
-      <c r="P40" s="122"/>
-      <c r="Q40" s="122"/>
-      <c r="R40" s="122"/>
-      <c r="S40" s="122"/>
-      <c r="T40" s="122"/>
-      <c r="U40" s="122"/>
-      <c r="V40" s="122"/>
-      <c r="W40" s="122"/>
-      <c r="X40" s="122"/>
-      <c r="Y40" s="122"/>
-      <c r="Z40" s="122"/>
-      <c r="AA40" s="122"/>
-      <c r="AB40" s="122"/>
-      <c r="AC40" s="122"/>
-      <c r="AD40" s="122"/>
-      <c r="AE40" s="122"/>
-      <c r="AF40" s="122"/>
-      <c r="AG40" s="122"/>
-      <c r="AH40" s="122"/>
-      <c r="AI40" s="122"/>
-      <c r="AJ40" s="122"/>
-      <c r="AK40" s="122"/>
-      <c r="AL40" s="122"/>
-      <c r="AM40" s="122"/>
-      <c r="AN40" s="122"/>
-      <c r="AO40" s="122"/>
-      <c r="AP40" s="122"/>
-      <c r="AQ40" s="122"/>
-      <c r="AR40" s="122"/>
-      <c r="AS40" s="122"/>
+      <c r="F40" s="120"/>
+      <c r="G40" s="120"/>
+      <c r="H40" s="120"/>
+      <c r="I40" s="120"/>
+      <c r="J40" s="120"/>
+      <c r="K40" s="120"/>
+      <c r="L40" s="120"/>
+      <c r="M40" s="120"/>
+      <c r="N40" s="120"/>
+      <c r="O40" s="120"/>
+      <c r="P40" s="120"/>
+      <c r="Q40" s="120"/>
+      <c r="R40" s="120"/>
+      <c r="S40" s="120"/>
+      <c r="T40" s="120"/>
+      <c r="U40" s="120"/>
+      <c r="V40" s="120"/>
+      <c r="W40" s="120"/>
+      <c r="X40" s="120"/>
+      <c r="Y40" s="120"/>
+      <c r="Z40" s="120"/>
+      <c r="AA40" s="120"/>
+      <c r="AB40" s="120"/>
+      <c r="AC40" s="120"/>
+      <c r="AD40" s="120"/>
+      <c r="AE40" s="120"/>
+      <c r="AF40" s="120"/>
+      <c r="AG40" s="120"/>
+      <c r="AH40" s="120"/>
+      <c r="AI40" s="120"/>
+      <c r="AJ40" s="120"/>
+      <c r="AK40" s="120"/>
+      <c r="AL40" s="120"/>
+      <c r="AM40" s="120"/>
+      <c r="AN40" s="120"/>
+      <c r="AO40" s="120"/>
+      <c r="AP40" s="120"/>
+      <c r="AQ40" s="120"/>
+      <c r="AR40" s="120"/>
+      <c r="AS40" s="120"/>
       <c r="AT40" s="33"/>
     </row>
-    <row r="41" spans="1:46" ht="2.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:46" ht="2.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="34"/>
       <c r="B41" s="13"/>
       <c r="C41" s="13"/>
@@ -4472,57 +4484,57 @@
       <c r="AS41" s="13"/>
       <c r="AT41" s="33"/>
     </row>
-    <row r="42" spans="1:46" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="129" t="s">
+    <row r="42" spans="1:46" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="148" t="s">
         <v>39</v>
       </c>
-      <c r="B42" s="130"/>
-      <c r="C42" s="130"/>
-      <c r="D42" s="130"/>
-      <c r="E42" s="130"/>
-      <c r="F42" s="122"/>
-      <c r="G42" s="122"/>
-      <c r="H42" s="122"/>
-      <c r="I42" s="122"/>
-      <c r="J42" s="122"/>
-      <c r="K42" s="122"/>
-      <c r="L42" s="122"/>
-      <c r="M42" s="122"/>
-      <c r="N42" s="122"/>
-      <c r="O42" s="122"/>
-      <c r="P42" s="122"/>
-      <c r="Q42" s="122"/>
-      <c r="R42" s="122"/>
-      <c r="S42" s="122"/>
-      <c r="T42" s="122"/>
-      <c r="U42" s="122"/>
-      <c r="V42" s="122"/>
-      <c r="W42" s="122"/>
-      <c r="X42" s="122"/>
-      <c r="Y42" s="122"/>
-      <c r="Z42" s="122"/>
-      <c r="AA42" s="122"/>
-      <c r="AB42" s="122"/>
-      <c r="AC42" s="122"/>
-      <c r="AD42" s="122"/>
-      <c r="AE42" s="122"/>
-      <c r="AF42" s="122"/>
-      <c r="AG42" s="122"/>
-      <c r="AH42" s="122"/>
-      <c r="AI42" s="122"/>
-      <c r="AJ42" s="122"/>
-      <c r="AK42" s="122"/>
-      <c r="AL42" s="122"/>
-      <c r="AM42" s="122"/>
-      <c r="AN42" s="122"/>
-      <c r="AO42" s="122"/>
-      <c r="AP42" s="122"/>
-      <c r="AQ42" s="122"/>
-      <c r="AR42" s="122"/>
-      <c r="AS42" s="122"/>
+      <c r="B42" s="149"/>
+      <c r="C42" s="149"/>
+      <c r="D42" s="149"/>
+      <c r="E42" s="149"/>
+      <c r="F42" s="120"/>
+      <c r="G42" s="120"/>
+      <c r="H42" s="120"/>
+      <c r="I42" s="120"/>
+      <c r="J42" s="120"/>
+      <c r="K42" s="120"/>
+      <c r="L42" s="120"/>
+      <c r="M42" s="120"/>
+      <c r="N42" s="120"/>
+      <c r="O42" s="120"/>
+      <c r="P42" s="120"/>
+      <c r="Q42" s="120"/>
+      <c r="R42" s="120"/>
+      <c r="S42" s="120"/>
+      <c r="T42" s="120"/>
+      <c r="U42" s="120"/>
+      <c r="V42" s="120"/>
+      <c r="W42" s="120"/>
+      <c r="X42" s="120"/>
+      <c r="Y42" s="120"/>
+      <c r="Z42" s="120"/>
+      <c r="AA42" s="120"/>
+      <c r="AB42" s="120"/>
+      <c r="AC42" s="120"/>
+      <c r="AD42" s="120"/>
+      <c r="AE42" s="120"/>
+      <c r="AF42" s="120"/>
+      <c r="AG42" s="120"/>
+      <c r="AH42" s="120"/>
+      <c r="AI42" s="120"/>
+      <c r="AJ42" s="120"/>
+      <c r="AK42" s="120"/>
+      <c r="AL42" s="120"/>
+      <c r="AM42" s="120"/>
+      <c r="AN42" s="120"/>
+      <c r="AO42" s="120"/>
+      <c r="AP42" s="120"/>
+      <c r="AQ42" s="120"/>
+      <c r="AR42" s="120"/>
+      <c r="AS42" s="120"/>
       <c r="AT42" s="33"/>
     </row>
-    <row r="43" spans="1:46" ht="2.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:46" ht="2.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="34"/>
       <c r="B43" s="13"/>
       <c r="C43" s="13"/>
@@ -4570,55 +4582,55 @@
       <c r="AS43" s="13"/>
       <c r="AT43" s="33"/>
     </row>
-    <row r="44" spans="1:46" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:46" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="34"/>
-      <c r="B44" s="122"/>
-      <c r="C44" s="122"/>
-      <c r="D44" s="122"/>
-      <c r="E44" s="122"/>
-      <c r="F44" s="122"/>
-      <c r="G44" s="122"/>
-      <c r="H44" s="122"/>
-      <c r="I44" s="122"/>
-      <c r="J44" s="122"/>
-      <c r="K44" s="122"/>
-      <c r="L44" s="122"/>
-      <c r="M44" s="122"/>
-      <c r="N44" s="122"/>
-      <c r="O44" s="122"/>
-      <c r="P44" s="122"/>
-      <c r="Q44" s="122"/>
-      <c r="R44" s="122"/>
-      <c r="S44" s="122"/>
-      <c r="T44" s="122"/>
-      <c r="U44" s="122"/>
-      <c r="V44" s="122"/>
-      <c r="W44" s="122"/>
-      <c r="X44" s="122"/>
-      <c r="Y44" s="122"/>
-      <c r="Z44" s="122"/>
-      <c r="AA44" s="122"/>
-      <c r="AB44" s="122"/>
-      <c r="AC44" s="122"/>
-      <c r="AD44" s="122"/>
-      <c r="AE44" s="122"/>
-      <c r="AF44" s="122"/>
-      <c r="AG44" s="122"/>
-      <c r="AH44" s="122"/>
-      <c r="AI44" s="122"/>
-      <c r="AJ44" s="122"/>
-      <c r="AK44" s="122"/>
-      <c r="AL44" s="122"/>
-      <c r="AM44" s="122"/>
-      <c r="AN44" s="122"/>
-      <c r="AO44" s="122"/>
-      <c r="AP44" s="122"/>
-      <c r="AQ44" s="122"/>
-      <c r="AR44" s="122"/>
-      <c r="AS44" s="122"/>
+      <c r="B44" s="120"/>
+      <c r="C44" s="120"/>
+      <c r="D44" s="120"/>
+      <c r="E44" s="120"/>
+      <c r="F44" s="120"/>
+      <c r="G44" s="120"/>
+      <c r="H44" s="120"/>
+      <c r="I44" s="120"/>
+      <c r="J44" s="120"/>
+      <c r="K44" s="120"/>
+      <c r="L44" s="120"/>
+      <c r="M44" s="120"/>
+      <c r="N44" s="120"/>
+      <c r="O44" s="120"/>
+      <c r="P44" s="120"/>
+      <c r="Q44" s="120"/>
+      <c r="R44" s="120"/>
+      <c r="S44" s="120"/>
+      <c r="T44" s="120"/>
+      <c r="U44" s="120"/>
+      <c r="V44" s="120"/>
+      <c r="W44" s="120"/>
+      <c r="X44" s="120"/>
+      <c r="Y44" s="120"/>
+      <c r="Z44" s="120"/>
+      <c r="AA44" s="120"/>
+      <c r="AB44" s="120"/>
+      <c r="AC44" s="120"/>
+      <c r="AD44" s="120"/>
+      <c r="AE44" s="120"/>
+      <c r="AF44" s="120"/>
+      <c r="AG44" s="120"/>
+      <c r="AH44" s="120"/>
+      <c r="AI44" s="120"/>
+      <c r="AJ44" s="120"/>
+      <c r="AK44" s="120"/>
+      <c r="AL44" s="120"/>
+      <c r="AM44" s="120"/>
+      <c r="AN44" s="120"/>
+      <c r="AO44" s="120"/>
+      <c r="AP44" s="120"/>
+      <c r="AQ44" s="120"/>
+      <c r="AR44" s="120"/>
+      <c r="AS44" s="120"/>
       <c r="AT44" s="33"/>
     </row>
-    <row r="45" spans="1:46" ht="2.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:46" ht="2.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="47"/>
       <c r="B45" s="48"/>
       <c r="C45" s="48"/>
@@ -4666,7 +4678,7 @@
       <c r="AS45" s="48"/>
       <c r="AT45" s="49"/>
     </row>
-    <row r="46" spans="1:46" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:46" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="50" t="s">
         <v>40</v>
       </c>
@@ -4687,41 +4699,41 @@
       <c r="N46" s="53"/>
       <c r="O46" s="52"/>
       <c r="P46" s="52"/>
-      <c r="Q46" s="118" t="str">
+      <c r="Q46" s="145" t="str">
         <f>IFERROR(VLOOKUP(B48,Dados!$A$16:$B$21,2,0),"")</f>
         <v/>
       </c>
-      <c r="R46" s="118"/>
-      <c r="S46" s="118"/>
-      <c r="T46" s="118"/>
-      <c r="U46" s="118"/>
-      <c r="V46" s="118"/>
-      <c r="W46" s="118"/>
-      <c r="X46" s="118"/>
-      <c r="Y46" s="118"/>
-      <c r="Z46" s="118"/>
-      <c r="AA46" s="118"/>
-      <c r="AB46" s="118"/>
-      <c r="AC46" s="118"/>
-      <c r="AD46" s="118"/>
-      <c r="AE46" s="118"/>
-      <c r="AF46" s="118"/>
-      <c r="AG46" s="118"/>
-      <c r="AH46" s="118"/>
-      <c r="AI46" s="118"/>
-      <c r="AJ46" s="118"/>
-      <c r="AK46" s="118"/>
-      <c r="AL46" s="118"/>
-      <c r="AM46" s="118"/>
-      <c r="AN46" s="118"/>
-      <c r="AO46" s="118"/>
-      <c r="AP46" s="118"/>
-      <c r="AQ46" s="118"/>
-      <c r="AR46" s="118"/>
-      <c r="AS46" s="118"/>
+      <c r="R46" s="145"/>
+      <c r="S46" s="145"/>
+      <c r="T46" s="145"/>
+      <c r="U46" s="145"/>
+      <c r="V46" s="145"/>
+      <c r="W46" s="145"/>
+      <c r="X46" s="145"/>
+      <c r="Y46" s="145"/>
+      <c r="Z46" s="145"/>
+      <c r="AA46" s="145"/>
+      <c r="AB46" s="145"/>
+      <c r="AC46" s="145"/>
+      <c r="AD46" s="145"/>
+      <c r="AE46" s="145"/>
+      <c r="AF46" s="145"/>
+      <c r="AG46" s="145"/>
+      <c r="AH46" s="145"/>
+      <c r="AI46" s="145"/>
+      <c r="AJ46" s="145"/>
+      <c r="AK46" s="145"/>
+      <c r="AL46" s="145"/>
+      <c r="AM46" s="145"/>
+      <c r="AN46" s="145"/>
+      <c r="AO46" s="145"/>
+      <c r="AP46" s="145"/>
+      <c r="AQ46" s="145"/>
+      <c r="AR46" s="145"/>
+      <c r="AS46" s="145"/>
       <c r="AT46" s="31"/>
     </row>
-    <row r="47" spans="1:46" ht="2.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:46" ht="2.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="44"/>
       <c r="B47" s="13"/>
       <c r="C47" s="13"/>
@@ -4738,86 +4750,86 @@
       <c r="N47" s="13"/>
       <c r="O47" s="13"/>
       <c r="P47" s="13"/>
-      <c r="Q47" s="119"/>
-      <c r="R47" s="119"/>
-      <c r="S47" s="119"/>
-      <c r="T47" s="119"/>
-      <c r="U47" s="119"/>
-      <c r="V47" s="119"/>
-      <c r="W47" s="119"/>
-      <c r="X47" s="119"/>
-      <c r="Y47" s="119"/>
-      <c r="Z47" s="119"/>
-      <c r="AA47" s="119"/>
-      <c r="AB47" s="119"/>
-      <c r="AC47" s="119"/>
-      <c r="AD47" s="119"/>
-      <c r="AE47" s="119"/>
-      <c r="AF47" s="119"/>
-      <c r="AG47" s="119"/>
-      <c r="AH47" s="119"/>
-      <c r="AI47" s="119"/>
-      <c r="AJ47" s="119"/>
-      <c r="AK47" s="119"/>
-      <c r="AL47" s="119"/>
-      <c r="AM47" s="119"/>
-      <c r="AN47" s="119"/>
-      <c r="AO47" s="119"/>
-      <c r="AP47" s="119"/>
-      <c r="AQ47" s="119"/>
-      <c r="AR47" s="119"/>
-      <c r="AS47" s="119"/>
+      <c r="Q47" s="146"/>
+      <c r="R47" s="146"/>
+      <c r="S47" s="146"/>
+      <c r="T47" s="146"/>
+      <c r="U47" s="146"/>
+      <c r="V47" s="146"/>
+      <c r="W47" s="146"/>
+      <c r="X47" s="146"/>
+      <c r="Y47" s="146"/>
+      <c r="Z47" s="146"/>
+      <c r="AA47" s="146"/>
+      <c r="AB47" s="146"/>
+      <c r="AC47" s="146"/>
+      <c r="AD47" s="146"/>
+      <c r="AE47" s="146"/>
+      <c r="AF47" s="146"/>
+      <c r="AG47" s="146"/>
+      <c r="AH47" s="146"/>
+      <c r="AI47" s="146"/>
+      <c r="AJ47" s="146"/>
+      <c r="AK47" s="146"/>
+      <c r="AL47" s="146"/>
+      <c r="AM47" s="146"/>
+      <c r="AN47" s="146"/>
+      <c r="AO47" s="146"/>
+      <c r="AP47" s="146"/>
+      <c r="AQ47" s="146"/>
+      <c r="AR47" s="146"/>
+      <c r="AS47" s="146"/>
       <c r="AT47" s="33"/>
     </row>
-    <row r="48" spans="1:46" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:46" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="44"/>
-      <c r="B48" s="120"/>
-      <c r="C48" s="120"/>
-      <c r="D48" s="120"/>
-      <c r="E48" s="120"/>
-      <c r="F48" s="120"/>
-      <c r="G48" s="120"/>
-      <c r="H48" s="120"/>
-      <c r="I48" s="120"/>
-      <c r="J48" s="120"/>
-      <c r="K48" s="120"/>
-      <c r="L48" s="120"/>
-      <c r="M48" s="120"/>
-      <c r="N48" s="120"/>
-      <c r="O48" s="120"/>
+      <c r="B48" s="147"/>
+      <c r="C48" s="147"/>
+      <c r="D48" s="147"/>
+      <c r="E48" s="147"/>
+      <c r="F48" s="147"/>
+      <c r="G48" s="147"/>
+      <c r="H48" s="147"/>
+      <c r="I48" s="147"/>
+      <c r="J48" s="147"/>
+      <c r="K48" s="147"/>
+      <c r="L48" s="147"/>
+      <c r="M48" s="147"/>
+      <c r="N48" s="147"/>
+      <c r="O48" s="147"/>
       <c r="P48" s="13"/>
-      <c r="Q48" s="119"/>
-      <c r="R48" s="119"/>
-      <c r="S48" s="119"/>
-      <c r="T48" s="119"/>
-      <c r="U48" s="119"/>
-      <c r="V48" s="119"/>
-      <c r="W48" s="119"/>
-      <c r="X48" s="119"/>
-      <c r="Y48" s="119"/>
-      <c r="Z48" s="119"/>
-      <c r="AA48" s="119"/>
-      <c r="AB48" s="119"/>
-      <c r="AC48" s="119"/>
-      <c r="AD48" s="119"/>
-      <c r="AE48" s="119"/>
-      <c r="AF48" s="119"/>
-      <c r="AG48" s="119"/>
-      <c r="AH48" s="119"/>
-      <c r="AI48" s="119"/>
-      <c r="AJ48" s="119"/>
-      <c r="AK48" s="119"/>
-      <c r="AL48" s="119"/>
-      <c r="AM48" s="119"/>
-      <c r="AN48" s="119"/>
-      <c r="AO48" s="119"/>
-      <c r="AP48" s="119"/>
-      <c r="AQ48" s="119"/>
-      <c r="AR48" s="119"/>
-      <c r="AS48" s="119"/>
+      <c r="Q48" s="146"/>
+      <c r="R48" s="146"/>
+      <c r="S48" s="146"/>
+      <c r="T48" s="146"/>
+      <c r="U48" s="146"/>
+      <c r="V48" s="146"/>
+      <c r="W48" s="146"/>
+      <c r="X48" s="146"/>
+      <c r="Y48" s="146"/>
+      <c r="Z48" s="146"/>
+      <c r="AA48" s="146"/>
+      <c r="AB48" s="146"/>
+      <c r="AC48" s="146"/>
+      <c r="AD48" s="146"/>
+      <c r="AE48" s="146"/>
+      <c r="AF48" s="146"/>
+      <c r="AG48" s="146"/>
+      <c r="AH48" s="146"/>
+      <c r="AI48" s="146"/>
+      <c r="AJ48" s="146"/>
+      <c r="AK48" s="146"/>
+      <c r="AL48" s="146"/>
+      <c r="AM48" s="146"/>
+      <c r="AN48" s="146"/>
+      <c r="AO48" s="146"/>
+      <c r="AP48" s="146"/>
+      <c r="AQ48" s="146"/>
+      <c r="AR48" s="146"/>
+      <c r="AS48" s="146"/>
       <c r="AT48" s="33"/>
     </row>
-    <row r="49" spans="1:46" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:46" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="44"/>
       <c r="B49" s="53"/>
       <c r="C49" s="53"/>
@@ -4834,38 +4846,38 @@
       <c r="N49" s="13"/>
       <c r="O49" s="13"/>
       <c r="P49" s="13"/>
-      <c r="Q49" s="119"/>
-      <c r="R49" s="119"/>
-      <c r="S49" s="119"/>
-      <c r="T49" s="119"/>
-      <c r="U49" s="119"/>
-      <c r="V49" s="119"/>
-      <c r="W49" s="119"/>
-      <c r="X49" s="119"/>
-      <c r="Y49" s="119"/>
-      <c r="Z49" s="119"/>
-      <c r="AA49" s="119"/>
-      <c r="AB49" s="119"/>
-      <c r="AC49" s="119"/>
-      <c r="AD49" s="119"/>
-      <c r="AE49" s="119"/>
-      <c r="AF49" s="119"/>
-      <c r="AG49" s="119"/>
-      <c r="AH49" s="119"/>
-      <c r="AI49" s="119"/>
-      <c r="AJ49" s="119"/>
-      <c r="AK49" s="119"/>
-      <c r="AL49" s="119"/>
-      <c r="AM49" s="119"/>
-      <c r="AN49" s="119"/>
-      <c r="AO49" s="119"/>
-      <c r="AP49" s="119"/>
-      <c r="AQ49" s="119"/>
-      <c r="AR49" s="119"/>
-      <c r="AS49" s="119"/>
+      <c r="Q49" s="146"/>
+      <c r="R49" s="146"/>
+      <c r="S49" s="146"/>
+      <c r="T49" s="146"/>
+      <c r="U49" s="146"/>
+      <c r="V49" s="146"/>
+      <c r="W49" s="146"/>
+      <c r="X49" s="146"/>
+      <c r="Y49" s="146"/>
+      <c r="Z49" s="146"/>
+      <c r="AA49" s="146"/>
+      <c r="AB49" s="146"/>
+      <c r="AC49" s="146"/>
+      <c r="AD49" s="146"/>
+      <c r="AE49" s="146"/>
+      <c r="AF49" s="146"/>
+      <c r="AG49" s="146"/>
+      <c r="AH49" s="146"/>
+      <c r="AI49" s="146"/>
+      <c r="AJ49" s="146"/>
+      <c r="AK49" s="146"/>
+      <c r="AL49" s="146"/>
+      <c r="AM49" s="146"/>
+      <c r="AN49" s="146"/>
+      <c r="AO49" s="146"/>
+      <c r="AP49" s="146"/>
+      <c r="AQ49" s="146"/>
+      <c r="AR49" s="146"/>
+      <c r="AS49" s="146"/>
       <c r="AT49" s="33"/>
     </row>
-    <row r="50" spans="1:46" ht="2.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:46" ht="2.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="47"/>
       <c r="B50" s="48"/>
       <c r="C50" s="48"/>
@@ -4913,7 +4925,7 @@
       <c r="AS50" s="54"/>
       <c r="AT50" s="49"/>
     </row>
-    <row r="51" spans="1:46" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:46" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="28" t="s">
         <v>45</v>
       </c>
@@ -4969,7 +4981,7 @@
       <c r="AS51" s="56"/>
       <c r="AT51" s="57"/>
     </row>
-    <row r="52" spans="1:46" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:46" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="32"/>
       <c r="B52" s="22"/>
       <c r="C52" s="13"/>
@@ -5012,7 +5024,7 @@
       <c r="AQ52" s="13"/>
       <c r="AT52" s="46"/>
     </row>
-    <row r="53" spans="1:46" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:46" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="34"/>
       <c r="B53" s="8"/>
       <c r="C53" s="60" t="s">
@@ -5064,7 +5076,7 @@
       <c r="AS53" s="102"/>
       <c r="AT53" s="46"/>
     </row>
-    <row r="54" spans="1:46" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:46" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="34"/>
       <c r="C54" s="62"/>
       <c r="D54" s="62"/>
@@ -5111,7 +5123,7 @@
       <c r="AS54" s="102"/>
       <c r="AT54" s="46"/>
     </row>
-    <row r="55" spans="1:46" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:46" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="34"/>
       <c r="B55" s="8"/>
       <c r="C55" s="102" t="s">
@@ -5136,7 +5148,7 @@
       <c r="T55" s="102"/>
       <c r="U55" s="102"/>
       <c r="V55" s="102"/>
-      <c r="W55" s="145"/>
+      <c r="W55" s="103"/>
       <c r="X55" s="13"/>
       <c r="Y55" s="1"/>
       <c r="Z55" s="102" t="s">
@@ -5163,7 +5175,7 @@
       <c r="AS55" s="102"/>
       <c r="AT55" s="46"/>
     </row>
-    <row r="56" spans="1:46" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:46" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="34"/>
       <c r="C56" s="102"/>
       <c r="D56" s="102"/>
@@ -5185,7 +5197,7 @@
       <c r="T56" s="102"/>
       <c r="U56" s="102"/>
       <c r="V56" s="102"/>
-      <c r="W56" s="145"/>
+      <c r="W56" s="103"/>
       <c r="X56" s="13"/>
       <c r="Y56" s="13"/>
       <c r="Z56" s="102"/>
@@ -5210,7 +5222,7 @@
       <c r="AS56" s="102"/>
       <c r="AT56" s="46"/>
     </row>
-    <row r="57" spans="1:46" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:46" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="34"/>
       <c r="C57" s="102"/>
       <c r="D57" s="102"/>
@@ -5232,7 +5244,7 @@
       <c r="T57" s="102"/>
       <c r="U57" s="102"/>
       <c r="V57" s="102"/>
-      <c r="W57" s="145"/>
+      <c r="W57" s="103"/>
       <c r="X57" s="14"/>
       <c r="Y57" s="1"/>
       <c r="Z57" s="102" t="s">
@@ -5259,7 +5271,7 @@
       <c r="AS57" s="102"/>
       <c r="AT57" s="46"/>
     </row>
-    <row r="58" spans="1:46" ht="11.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:46" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="34"/>
       <c r="D58"/>
       <c r="E58"/>
@@ -5305,7 +5317,7 @@
       <c r="AS58" s="102"/>
       <c r="AT58" s="46"/>
     </row>
-    <row r="59" spans="1:46" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:46" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="34"/>
       <c r="B59" s="8"/>
       <c r="C59" s="102" t="s">
@@ -5330,7 +5342,7 @@
       <c r="T59" s="102"/>
       <c r="U59" s="102"/>
       <c r="V59" s="102"/>
-      <c r="W59" s="145"/>
+      <c r="W59" s="103"/>
       <c r="X59" s="13"/>
       <c r="Y59" s="1"/>
       <c r="Z59" s="102" t="s">
@@ -5357,7 +5369,7 @@
       <c r="AS59" s="102"/>
       <c r="AT59" s="46"/>
     </row>
-    <row r="60" spans="1:46" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:46" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="34"/>
       <c r="B60" s="13"/>
       <c r="C60" s="102"/>
@@ -5380,7 +5392,7 @@
       <c r="T60" s="102"/>
       <c r="U60" s="102"/>
       <c r="V60" s="102"/>
-      <c r="W60" s="145"/>
+      <c r="W60" s="103"/>
       <c r="X60" s="14"/>
       <c r="Y60" s="13"/>
       <c r="Z60" s="102"/>
@@ -5405,7 +5417,7 @@
       <c r="AS60" s="102"/>
       <c r="AT60" s="46"/>
     </row>
-    <row r="61" spans="1:46" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:46" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="34"/>
       <c r="B61" s="1"/>
       <c r="C61" s="102" t="s">
@@ -5457,7 +5469,7 @@
       <c r="AS61" s="102"/>
       <c r="AT61" s="46"/>
     </row>
-    <row r="62" spans="1:46" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:46" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="34"/>
       <c r="B62" s="14"/>
       <c r="C62" s="102"/>
@@ -5505,7 +5517,7 @@
       <c r="AS62" s="102"/>
       <c r="AT62" s="46"/>
     </row>
-    <row r="63" spans="1:46" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:46" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="34"/>
       <c r="D63" s="13"/>
       <c r="E63" s="13"/>
@@ -5551,7 +5563,7 @@
       <c r="AS63" s="102"/>
       <c r="AT63" s="46"/>
     </row>
-    <row r="64" spans="1:46" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:46" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="34"/>
       <c r="B64" s="1"/>
       <c r="C64" s="21" t="s">
@@ -5601,7 +5613,7 @@
       <c r="AQ64" s="13"/>
       <c r="AT64" s="46"/>
     </row>
-    <row r="65" spans="1:46" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:46" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="34"/>
       <c r="B65" s="13"/>
       <c r="D65" s="13"/>
@@ -5644,7 +5656,7 @@
       <c r="AQ65" s="13"/>
       <c r="AT65" s="46"/>
     </row>
-    <row r="66" spans="1:46" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:46" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="34"/>
       <c r="B66" s="13"/>
       <c r="D66" s="13"/>
@@ -5691,7 +5703,7 @@
       <c r="AQ66" s="13"/>
       <c r="AT66" s="46"/>
     </row>
-    <row r="67" spans="1:46" ht="2.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:46" ht="2.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="47"/>
       <c r="B67" s="48"/>
       <c r="C67" s="25"/>
@@ -5739,7 +5751,7 @@
       <c r="AS67" s="25"/>
       <c r="AT67" s="68"/>
     </row>
-    <row r="68" spans="1:46" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:46" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="28" t="s">
         <v>50</v>
       </c>
@@ -5791,7 +5803,7 @@
       <c r="AS68" s="41"/>
       <c r="AT68" s="31"/>
     </row>
-    <row r="69" spans="1:46" ht="2.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:46" ht="2.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="32"/>
       <c r="B69" s="70"/>
       <c r="C69" s="21"/>
@@ -5839,7 +5851,7 @@
       <c r="AS69" s="21"/>
       <c r="AT69" s="33"/>
     </row>
-    <row r="70" spans="1:46" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:46" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="71" t="s">
         <v>47</v>
       </c>
@@ -5889,7 +5901,7 @@
       <c r="AS70" s="18"/>
       <c r="AT70" s="73"/>
     </row>
-    <row r="71" spans="1:46" ht="2.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:46" ht="2.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="71"/>
       <c r="B71" s="72"/>
       <c r="C71" s="72"/>
@@ -5937,7 +5949,7 @@
       <c r="AS71" s="18"/>
       <c r="AT71" s="73"/>
     </row>
-    <row r="72" spans="1:46" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:46" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="34"/>
       <c r="B72" s="45" t="str">
         <f>IF(AND(Dados!C5=0,Dados!C3&gt;=1),"X","")</f>
@@ -5998,7 +6010,7 @@
       <c r="AS72" s="13"/>
       <c r="AT72" s="33"/>
     </row>
-    <row r="73" spans="1:46" ht="2.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:46" ht="2.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="47"/>
       <c r="B73" s="67"/>
       <c r="C73" s="48"/>
@@ -6046,7 +6058,7 @@
       <c r="AS73" s="48"/>
       <c r="AT73" s="49"/>
     </row>
-    <row r="74" spans="1:46" ht="2.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:46" ht="2.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="13"/>
       <c r="B74" s="13"/>
       <c r="C74" s="13"/>
@@ -6094,7 +6106,7 @@
       <c r="AS74" s="13"/>
       <c r="AT74" s="13"/>
     </row>
-    <row r="75" spans="1:46" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:46" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="28" t="s">
         <v>62</v>
       </c>
@@ -6146,7 +6158,7 @@
       <c r="AS75" s="30"/>
       <c r="AT75" s="31"/>
     </row>
-    <row r="76" spans="1:46" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:46" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="34"/>
       <c r="B76" s="13"/>
       <c r="C76" s="13"/>
@@ -6194,7 +6206,7 @@
       <c r="AS76" s="13"/>
       <c r="AT76" s="33"/>
     </row>
-    <row r="77" spans="1:46" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:46" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="34"/>
       <c r="B77" s="21"/>
       <c r="C77" s="21"/>
@@ -6242,16 +6254,16 @@
       <c r="AS77" s="13"/>
       <c r="AT77" s="33"/>
     </row>
-    <row r="78" spans="1:46" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:46" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="34"/>
-      <c r="B78" s="114" t="str">
+      <c r="B78" s="116" t="str">
         <f>IFERROR(VLOOKUP($B$3,Dados!K1:M9,2,),"")</f>
         <v/>
       </c>
-      <c r="C78" s="110"/>
-      <c r="D78" s="110"/>
-      <c r="E78" s="110"/>
-      <c r="F78" s="115"/>
+      <c r="C78" s="157"/>
+      <c r="D78" s="157"/>
+      <c r="E78" s="157"/>
+      <c r="F78" s="161"/>
       <c r="G78" s="13"/>
       <c r="H78" s="13"/>
       <c r="I78" s="13"/>
@@ -6265,46 +6277,46 @@
       <c r="Q78" s="13"/>
       <c r="R78" s="13"/>
       <c r="S78" s="13"/>
-      <c r="T78" s="116" t="str">
+      <c r="T78" s="162" t="str">
         <f>IFERROR(VLOOKUP($B$3,Dados!K1:M9,3,),"")</f>
         <v/>
       </c>
-      <c r="U78" s="116"/>
-      <c r="V78" s="116"/>
-      <c r="W78" s="116"/>
-      <c r="X78" s="116"/>
-      <c r="Y78" s="116"/>
-      <c r="Z78" s="116"/>
-      <c r="AA78" s="116"/>
-      <c r="AB78" s="116"/>
-      <c r="AC78" s="116"/>
-      <c r="AD78" s="116"/>
-      <c r="AE78" s="116"/>
-      <c r="AF78" s="116"/>
-      <c r="AG78" s="116"/>
-      <c r="AH78" s="116"/>
-      <c r="AI78" s="116"/>
-      <c r="AJ78" s="116"/>
-      <c r="AK78" s="116"/>
-      <c r="AL78" s="116"/>
-      <c r="AM78" s="116"/>
-      <c r="AN78" s="116"/>
-      <c r="AO78" s="116"/>
+      <c r="U78" s="162"/>
+      <c r="V78" s="162"/>
+      <c r="W78" s="162"/>
+      <c r="X78" s="162"/>
+      <c r="Y78" s="162"/>
+      <c r="Z78" s="162"/>
+      <c r="AA78" s="162"/>
+      <c r="AB78" s="162"/>
+      <c r="AC78" s="162"/>
+      <c r="AD78" s="162"/>
+      <c r="AE78" s="162"/>
+      <c r="AF78" s="162"/>
+      <c r="AG78" s="162"/>
+      <c r="AH78" s="162"/>
+      <c r="AI78" s="162"/>
+      <c r="AJ78" s="162"/>
+      <c r="AK78" s="162"/>
+      <c r="AL78" s="162"/>
+      <c r="AM78" s="162"/>
+      <c r="AN78" s="162"/>
+      <c r="AO78" s="162"/>
       <c r="AP78" s="13"/>
       <c r="AQ78" s="13"/>
       <c r="AR78" s="13"/>
       <c r="AS78" s="13"/>
       <c r="AT78" s="33"/>
     </row>
-    <row r="79" spans="1:46" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:46" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="47"/>
-      <c r="B79" s="109" t="s">
+      <c r="B79" s="156" t="s">
         <v>64</v>
       </c>
-      <c r="C79" s="109"/>
-      <c r="D79" s="109"/>
-      <c r="E79" s="109"/>
-      <c r="F79" s="109"/>
+      <c r="C79" s="156"/>
+      <c r="D79" s="156"/>
+      <c r="E79" s="156"/>
+      <c r="F79" s="156"/>
       <c r="G79" s="48"/>
       <c r="H79" s="48"/>
       <c r="I79" s="48"/>
@@ -6318,37 +6330,37 @@
       <c r="Q79" s="48"/>
       <c r="R79" s="48"/>
       <c r="S79" s="48"/>
-      <c r="T79" s="110" t="s">
+      <c r="T79" s="157" t="s">
         <v>65</v>
       </c>
-      <c r="U79" s="110"/>
-      <c r="V79" s="110"/>
-      <c r="W79" s="110"/>
-      <c r="X79" s="110"/>
-      <c r="Y79" s="110"/>
-      <c r="Z79" s="110"/>
-      <c r="AA79" s="110"/>
-      <c r="AB79" s="110"/>
-      <c r="AC79" s="110"/>
-      <c r="AD79" s="110"/>
-      <c r="AE79" s="110"/>
-      <c r="AF79" s="110"/>
-      <c r="AG79" s="110"/>
-      <c r="AH79" s="110"/>
-      <c r="AI79" s="110"/>
-      <c r="AJ79" s="110"/>
-      <c r="AK79" s="110"/>
-      <c r="AL79" s="110"/>
-      <c r="AM79" s="110"/>
-      <c r="AN79" s="110"/>
-      <c r="AO79" s="110"/>
+      <c r="U79" s="157"/>
+      <c r="V79" s="157"/>
+      <c r="W79" s="157"/>
+      <c r="X79" s="157"/>
+      <c r="Y79" s="157"/>
+      <c r="Z79" s="157"/>
+      <c r="AA79" s="157"/>
+      <c r="AB79" s="157"/>
+      <c r="AC79" s="157"/>
+      <c r="AD79" s="157"/>
+      <c r="AE79" s="157"/>
+      <c r="AF79" s="157"/>
+      <c r="AG79" s="157"/>
+      <c r="AH79" s="157"/>
+      <c r="AI79" s="157"/>
+      <c r="AJ79" s="157"/>
+      <c r="AK79" s="157"/>
+      <c r="AL79" s="157"/>
+      <c r="AM79" s="157"/>
+      <c r="AN79" s="157"/>
+      <c r="AO79" s="157"/>
       <c r="AP79" s="48"/>
       <c r="AQ79" s="48"/>
       <c r="AR79" s="48"/>
       <c r="AS79" s="48"/>
       <c r="AT79" s="49"/>
     </row>
-    <row r="80" spans="1:46" ht="2.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:46" ht="2.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="13"/>
       <c r="B80" s="13"/>
       <c r="C80" s="13"/>
@@ -6396,7 +6408,7 @@
       <c r="AS80" s="13"/>
       <c r="AT80" s="13"/>
     </row>
-    <row r="81" spans="1:46" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:46" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="28" t="s">
         <v>66</v>
       </c>
@@ -6448,105 +6460,105 @@
       <c r="AS81" s="30"/>
       <c r="AT81" s="31"/>
     </row>
-    <row r="82" spans="1:46" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="111" t="s">
+    <row r="82" spans="1:46" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A82" s="158" t="s">
         <v>68</v>
       </c>
-      <c r="B82" s="112"/>
-      <c r="C82" s="112"/>
-      <c r="D82" s="112"/>
-      <c r="E82" s="112"/>
-      <c r="F82" s="112"/>
-      <c r="G82" s="112"/>
-      <c r="H82" s="112"/>
-      <c r="I82" s="112"/>
-      <c r="J82" s="112"/>
-      <c r="K82" s="112"/>
-      <c r="L82" s="112"/>
-      <c r="M82" s="112"/>
-      <c r="N82" s="112"/>
-      <c r="O82" s="112"/>
-      <c r="P82" s="112"/>
-      <c r="Q82" s="112"/>
-      <c r="R82" s="112"/>
-      <c r="S82" s="112"/>
-      <c r="T82" s="112"/>
-      <c r="U82" s="112"/>
-      <c r="V82" s="112"/>
-      <c r="W82" s="112"/>
-      <c r="X82" s="112"/>
-      <c r="Y82" s="112"/>
-      <c r="Z82" s="112"/>
-      <c r="AA82" s="112"/>
-      <c r="AB82" s="112"/>
-      <c r="AC82" s="112"/>
-      <c r="AD82" s="112"/>
-      <c r="AE82" s="112"/>
-      <c r="AF82" s="112"/>
-      <c r="AG82" s="112"/>
-      <c r="AH82" s="112"/>
-      <c r="AI82" s="112"/>
-      <c r="AJ82" s="112"/>
-      <c r="AK82" s="112"/>
-      <c r="AL82" s="112"/>
-      <c r="AM82" s="112"/>
-      <c r="AN82" s="112"/>
-      <c r="AO82" s="112"/>
-      <c r="AP82" s="112"/>
-      <c r="AQ82" s="112"/>
-      <c r="AR82" s="112"/>
-      <c r="AS82" s="112"/>
-      <c r="AT82" s="113"/>
-    </row>
-    <row r="83" spans="1:46" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="111"/>
-      <c r="B83" s="112"/>
-      <c r="C83" s="112"/>
-      <c r="D83" s="112"/>
-      <c r="E83" s="112"/>
-      <c r="F83" s="112"/>
-      <c r="G83" s="112"/>
-      <c r="H83" s="112"/>
-      <c r="I83" s="112"/>
-      <c r="J83" s="112"/>
-      <c r="K83" s="112"/>
-      <c r="L83" s="112"/>
-      <c r="M83" s="112"/>
-      <c r="N83" s="112"/>
-      <c r="O83" s="112"/>
-      <c r="P83" s="112"/>
-      <c r="Q83" s="112"/>
-      <c r="R83" s="112"/>
-      <c r="S83" s="112"/>
-      <c r="T83" s="112"/>
-      <c r="U83" s="112"/>
-      <c r="V83" s="112"/>
-      <c r="W83" s="112"/>
-      <c r="X83" s="112"/>
-      <c r="Y83" s="112"/>
-      <c r="Z83" s="112"/>
-      <c r="AA83" s="112"/>
-      <c r="AB83" s="112"/>
-      <c r="AC83" s="112"/>
-      <c r="AD83" s="112"/>
-      <c r="AE83" s="112"/>
-      <c r="AF83" s="112"/>
-      <c r="AG83" s="112"/>
-      <c r="AH83" s="112"/>
-      <c r="AI83" s="112"/>
-      <c r="AJ83" s="112"/>
-      <c r="AK83" s="112"/>
-      <c r="AL83" s="112"/>
-      <c r="AM83" s="112"/>
-      <c r="AN83" s="112"/>
-      <c r="AO83" s="112"/>
-      <c r="AP83" s="112"/>
-      <c r="AQ83" s="112"/>
-      <c r="AR83" s="112"/>
-      <c r="AS83" s="112"/>
-      <c r="AT83" s="113"/>
-    </row>
-    <row r="84" spans="1:46" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B82" s="159"/>
+      <c r="C82" s="159"/>
+      <c r="D82" s="159"/>
+      <c r="E82" s="159"/>
+      <c r="F82" s="159"/>
+      <c r="G82" s="159"/>
+      <c r="H82" s="159"/>
+      <c r="I82" s="159"/>
+      <c r="J82" s="159"/>
+      <c r="K82" s="159"/>
+      <c r="L82" s="159"/>
+      <c r="M82" s="159"/>
+      <c r="N82" s="159"/>
+      <c r="O82" s="159"/>
+      <c r="P82" s="159"/>
+      <c r="Q82" s="159"/>
+      <c r="R82" s="159"/>
+      <c r="S82" s="159"/>
+      <c r="T82" s="159"/>
+      <c r="U82" s="159"/>
+      <c r="V82" s="159"/>
+      <c r="W82" s="159"/>
+      <c r="X82" s="159"/>
+      <c r="Y82" s="159"/>
+      <c r="Z82" s="159"/>
+      <c r="AA82" s="159"/>
+      <c r="AB82" s="159"/>
+      <c r="AC82" s="159"/>
+      <c r="AD82" s="159"/>
+      <c r="AE82" s="159"/>
+      <c r="AF82" s="159"/>
+      <c r="AG82" s="159"/>
+      <c r="AH82" s="159"/>
+      <c r="AI82" s="159"/>
+      <c r="AJ82" s="159"/>
+      <c r="AK82" s="159"/>
+      <c r="AL82" s="159"/>
+      <c r="AM82" s="159"/>
+      <c r="AN82" s="159"/>
+      <c r="AO82" s="159"/>
+      <c r="AP82" s="159"/>
+      <c r="AQ82" s="159"/>
+      <c r="AR82" s="159"/>
+      <c r="AS82" s="159"/>
+      <c r="AT82" s="160"/>
+    </row>
+    <row r="83" spans="1:46" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A83" s="158"/>
+      <c r="B83" s="159"/>
+      <c r="C83" s="159"/>
+      <c r="D83" s="159"/>
+      <c r="E83" s="159"/>
+      <c r="F83" s="159"/>
+      <c r="G83" s="159"/>
+      <c r="H83" s="159"/>
+      <c r="I83" s="159"/>
+      <c r="J83" s="159"/>
+      <c r="K83" s="159"/>
+      <c r="L83" s="159"/>
+      <c r="M83" s="159"/>
+      <c r="N83" s="159"/>
+      <c r="O83" s="159"/>
+      <c r="P83" s="159"/>
+      <c r="Q83" s="159"/>
+      <c r="R83" s="159"/>
+      <c r="S83" s="159"/>
+      <c r="T83" s="159"/>
+      <c r="U83" s="159"/>
+      <c r="V83" s="159"/>
+      <c r="W83" s="159"/>
+      <c r="X83" s="159"/>
+      <c r="Y83" s="159"/>
+      <c r="Z83" s="159"/>
+      <c r="AA83" s="159"/>
+      <c r="AB83" s="159"/>
+      <c r="AC83" s="159"/>
+      <c r="AD83" s="159"/>
+      <c r="AE83" s="159"/>
+      <c r="AF83" s="159"/>
+      <c r="AG83" s="159"/>
+      <c r="AH83" s="159"/>
+      <c r="AI83" s="159"/>
+      <c r="AJ83" s="159"/>
+      <c r="AK83" s="159"/>
+      <c r="AL83" s="159"/>
+      <c r="AM83" s="159"/>
+      <c r="AN83" s="159"/>
+      <c r="AO83" s="159"/>
+      <c r="AP83" s="159"/>
+      <c r="AQ83" s="159"/>
+      <c r="AR83" s="159"/>
+      <c r="AS83" s="159"/>
+      <c r="AT83" s="160"/>
+    </row>
+    <row r="84" spans="1:46" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="74"/>
       <c r="B84" s="21"/>
       <c r="C84" s="21"/>
@@ -6594,7 +6606,7 @@
       <c r="AS84" s="21"/>
       <c r="AT84" s="75"/>
     </row>
-    <row r="85" spans="1:46" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:46" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="74"/>
       <c r="B85" s="13"/>
       <c r="C85" s="21"/>
@@ -6609,10 +6621,10 @@
       <c r="L85" s="21"/>
       <c r="M85" s="21"/>
       <c r="N85" s="21"/>
-      <c r="Q85" s="108" t="s">
+      <c r="Q85" s="155" t="s">
         <v>18</v>
       </c>
-      <c r="R85" s="108"/>
+      <c r="R85" s="155"/>
       <c r="S85" s="76"/>
       <c r="T85" s="76"/>
       <c r="U85" s="77"/>
@@ -6649,7 +6661,7 @@
       <c r="AR85" s="21"/>
       <c r="AT85" s="46"/>
     </row>
-    <row r="86" spans="1:46" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:46" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="74"/>
       <c r="B86" s="13"/>
       <c r="C86" s="13"/>
@@ -6697,7 +6709,7 @@
       <c r="AS86" s="21"/>
       <c r="AT86" s="75"/>
     </row>
-    <row r="87" spans="1:46" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:46" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="74"/>
       <c r="B87" s="13"/>
       <c r="C87" s="36"/>
@@ -6745,7 +6757,7 @@
       <c r="AS87" s="36"/>
       <c r="AT87" s="75"/>
     </row>
-    <row r="88" spans="1:46" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:46" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" s="79" t="s">
         <v>69</v>
       </c>
@@ -6795,7 +6807,7 @@
       <c r="AS88" s="18"/>
       <c r="AT88" s="80"/>
     </row>
-    <row r="89" spans="1:46" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:46" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" s="81"/>
       <c r="B89" s="82"/>
       <c r="C89" s="82"/>
@@ -6843,7 +6855,7 @@
       <c r="AS89" s="82"/>
       <c r="AT89" s="83"/>
     </row>
-    <row r="91" spans="1:46" ht="15.5" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:46" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A91" s="84" t="s">
         <v>72</v>
       </c>
@@ -6893,7 +6905,7 @@
       <c r="AS91" s="86"/>
       <c r="AT91" s="87"/>
     </row>
-    <row r="92" spans="1:46" ht="13" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:46" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A92" s="88"/>
       <c r="B92" s="89"/>
       <c r="C92" s="89"/>
@@ -6940,105 +6952,105 @@
       <c r="AR92" s="89"/>
       <c r="AT92" s="46"/>
     </row>
-    <row r="93" spans="1:46" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:46" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" s="88"/>
       <c r="B93" s="90"/>
-      <c r="C93" s="144" t="s">
+      <c r="C93" s="135" t="s">
         <v>73</v>
       </c>
-      <c r="D93" s="144"/>
-      <c r="E93" s="144"/>
-      <c r="F93" s="144"/>
-      <c r="G93" s="144"/>
-      <c r="H93" s="144"/>
-      <c r="I93" s="144"/>
-      <c r="J93" s="144"/>
-      <c r="K93" s="144"/>
-      <c r="L93" s="144"/>
-      <c r="M93" s="144"/>
-      <c r="N93" s="144"/>
-      <c r="O93" s="144"/>
-      <c r="P93" s="144"/>
-      <c r="Q93" s="144"/>
-      <c r="R93" s="144"/>
-      <c r="S93" s="144"/>
-      <c r="T93" s="144"/>
-      <c r="U93" s="144"/>
-      <c r="V93" s="144"/>
-      <c r="W93" s="144"/>
-      <c r="X93" s="144"/>
-      <c r="Y93" s="144"/>
-      <c r="Z93" s="144"/>
-      <c r="AA93" s="144"/>
-      <c r="AB93" s="144"/>
-      <c r="AC93" s="144"/>
-      <c r="AD93" s="144"/>
-      <c r="AE93" s="144"/>
-      <c r="AF93" s="144"/>
-      <c r="AG93" s="144"/>
-      <c r="AH93" s="144"/>
-      <c r="AI93" s="144"/>
-      <c r="AJ93" s="144"/>
-      <c r="AK93" s="144"/>
-      <c r="AL93" s="144"/>
-      <c r="AM93" s="144"/>
-      <c r="AN93" s="144"/>
-      <c r="AO93" s="144"/>
-      <c r="AP93" s="144"/>
-      <c r="AQ93" s="144"/>
-      <c r="AR93" s="144"/>
-      <c r="AS93" s="144"/>
+      <c r="D93" s="135"/>
+      <c r="E93" s="135"/>
+      <c r="F93" s="135"/>
+      <c r="G93" s="135"/>
+      <c r="H93" s="135"/>
+      <c r="I93" s="135"/>
+      <c r="J93" s="135"/>
+      <c r="K93" s="135"/>
+      <c r="L93" s="135"/>
+      <c r="M93" s="135"/>
+      <c r="N93" s="135"/>
+      <c r="O93" s="135"/>
+      <c r="P93" s="135"/>
+      <c r="Q93" s="135"/>
+      <c r="R93" s="135"/>
+      <c r="S93" s="135"/>
+      <c r="T93" s="135"/>
+      <c r="U93" s="135"/>
+      <c r="V93" s="135"/>
+      <c r="W93" s="135"/>
+      <c r="X93" s="135"/>
+      <c r="Y93" s="135"/>
+      <c r="Z93" s="135"/>
+      <c r="AA93" s="135"/>
+      <c r="AB93" s="135"/>
+      <c r="AC93" s="135"/>
+      <c r="AD93" s="135"/>
+      <c r="AE93" s="135"/>
+      <c r="AF93" s="135"/>
+      <c r="AG93" s="135"/>
+      <c r="AH93" s="135"/>
+      <c r="AI93" s="135"/>
+      <c r="AJ93" s="135"/>
+      <c r="AK93" s="135"/>
+      <c r="AL93" s="135"/>
+      <c r="AM93" s="135"/>
+      <c r="AN93" s="135"/>
+      <c r="AO93" s="135"/>
+      <c r="AP93" s="135"/>
+      <c r="AQ93" s="135"/>
+      <c r="AR93" s="135"/>
+      <c r="AS93" s="135"/>
       <c r="AT93" s="46"/>
     </row>
-    <row r="94" spans="1:46" ht="13" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:46" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A94" s="88"/>
       <c r="B94" s="89"/>
-      <c r="C94" s="144"/>
-      <c r="D94" s="144"/>
-      <c r="E94" s="144"/>
-      <c r="F94" s="144"/>
-      <c r="G94" s="144"/>
-      <c r="H94" s="144"/>
-      <c r="I94" s="144"/>
-      <c r="J94" s="144"/>
-      <c r="K94" s="144"/>
-      <c r="L94" s="144"/>
-      <c r="M94" s="144"/>
-      <c r="N94" s="144"/>
-      <c r="O94" s="144"/>
-      <c r="P94" s="144"/>
-      <c r="Q94" s="144"/>
-      <c r="R94" s="144"/>
-      <c r="S94" s="144"/>
-      <c r="T94" s="144"/>
-      <c r="U94" s="144"/>
-      <c r="V94" s="144"/>
-      <c r="W94" s="144"/>
-      <c r="X94" s="144"/>
-      <c r="Y94" s="144"/>
-      <c r="Z94" s="144"/>
-      <c r="AA94" s="144"/>
-      <c r="AB94" s="144"/>
-      <c r="AC94" s="144"/>
-      <c r="AD94" s="144"/>
-      <c r="AE94" s="144"/>
-      <c r="AF94" s="144"/>
-      <c r="AG94" s="144"/>
-      <c r="AH94" s="144"/>
-      <c r="AI94" s="144"/>
-      <c r="AJ94" s="144"/>
-      <c r="AK94" s="144"/>
-      <c r="AL94" s="144"/>
-      <c r="AM94" s="144"/>
-      <c r="AN94" s="144"/>
-      <c r="AO94" s="144"/>
-      <c r="AP94" s="144"/>
-      <c r="AQ94" s="144"/>
-      <c r="AR94" s="144"/>
-      <c r="AS94" s="144"/>
+      <c r="C94" s="135"/>
+      <c r="D94" s="135"/>
+      <c r="E94" s="135"/>
+      <c r="F94" s="135"/>
+      <c r="G94" s="135"/>
+      <c r="H94" s="135"/>
+      <c r="I94" s="135"/>
+      <c r="J94" s="135"/>
+      <c r="K94" s="135"/>
+      <c r="L94" s="135"/>
+      <c r="M94" s="135"/>
+      <c r="N94" s="135"/>
+      <c r="O94" s="135"/>
+      <c r="P94" s="135"/>
+      <c r="Q94" s="135"/>
+      <c r="R94" s="135"/>
+      <c r="S94" s="135"/>
+      <c r="T94" s="135"/>
+      <c r="U94" s="135"/>
+      <c r="V94" s="135"/>
+      <c r="W94" s="135"/>
+      <c r="X94" s="135"/>
+      <c r="Y94" s="135"/>
+      <c r="Z94" s="135"/>
+      <c r="AA94" s="135"/>
+      <c r="AB94" s="135"/>
+      <c r="AC94" s="135"/>
+      <c r="AD94" s="135"/>
+      <c r="AE94" s="135"/>
+      <c r="AF94" s="135"/>
+      <c r="AG94" s="135"/>
+      <c r="AH94" s="135"/>
+      <c r="AI94" s="135"/>
+      <c r="AJ94" s="135"/>
+      <c r="AK94" s="135"/>
+      <c r="AL94" s="135"/>
+      <c r="AM94" s="135"/>
+      <c r="AN94" s="135"/>
+      <c r="AO94" s="135"/>
+      <c r="AP94" s="135"/>
+      <c r="AQ94" s="135"/>
+      <c r="AR94" s="135"/>
+      <c r="AS94" s="135"/>
       <c r="AT94" s="46"/>
     </row>
-    <row r="95" spans="1:46" ht="13" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:46" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A95" s="88"/>
       <c r="B95" s="89"/>
       <c r="C95" s="91"/>
@@ -7085,105 +7097,105 @@
       <c r="AR95" s="89"/>
       <c r="AT95" s="46"/>
     </row>
-    <row r="96" spans="1:46" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:46" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" s="88"/>
       <c r="B96" s="89"/>
-      <c r="C96" s="143" t="s">
+      <c r="C96" s="134" t="s">
         <v>74</v>
       </c>
-      <c r="D96" s="143"/>
-      <c r="E96" s="143"/>
-      <c r="F96" s="143"/>
-      <c r="G96" s="143"/>
-      <c r="H96" s="143"/>
-      <c r="I96" s="143"/>
-      <c r="J96" s="143"/>
-      <c r="K96" s="143"/>
-      <c r="L96" s="143"/>
-      <c r="M96" s="143"/>
-      <c r="N96" s="143"/>
-      <c r="O96" s="143"/>
-      <c r="P96" s="143"/>
-      <c r="Q96" s="143"/>
-      <c r="R96" s="143"/>
-      <c r="S96" s="143"/>
-      <c r="T96" s="143"/>
-      <c r="U96" s="143"/>
-      <c r="V96" s="143"/>
-      <c r="W96" s="143"/>
-      <c r="X96" s="143"/>
-      <c r="Y96" s="143"/>
-      <c r="Z96" s="143"/>
-      <c r="AA96" s="143"/>
-      <c r="AB96" s="143"/>
-      <c r="AC96" s="143"/>
-      <c r="AD96" s="143"/>
-      <c r="AE96" s="143"/>
-      <c r="AF96" s="143"/>
-      <c r="AG96" s="143"/>
-      <c r="AH96" s="143"/>
-      <c r="AI96" s="143"/>
-      <c r="AJ96" s="143"/>
-      <c r="AK96" s="143"/>
-      <c r="AL96" s="143"/>
-      <c r="AM96" s="143"/>
-      <c r="AN96" s="143"/>
-      <c r="AO96" s="143"/>
-      <c r="AP96" s="143"/>
-      <c r="AQ96" s="143"/>
-      <c r="AR96" s="143"/>
-      <c r="AS96" s="143"/>
+      <c r="D96" s="134"/>
+      <c r="E96" s="134"/>
+      <c r="F96" s="134"/>
+      <c r="G96" s="134"/>
+      <c r="H96" s="134"/>
+      <c r="I96" s="134"/>
+      <c r="J96" s="134"/>
+      <c r="K96" s="134"/>
+      <c r="L96" s="134"/>
+      <c r="M96" s="134"/>
+      <c r="N96" s="134"/>
+      <c r="O96" s="134"/>
+      <c r="P96" s="134"/>
+      <c r="Q96" s="134"/>
+      <c r="R96" s="134"/>
+      <c r="S96" s="134"/>
+      <c r="T96" s="134"/>
+      <c r="U96" s="134"/>
+      <c r="V96" s="134"/>
+      <c r="W96" s="134"/>
+      <c r="X96" s="134"/>
+      <c r="Y96" s="134"/>
+      <c r="Z96" s="134"/>
+      <c r="AA96" s="134"/>
+      <c r="AB96" s="134"/>
+      <c r="AC96" s="134"/>
+      <c r="AD96" s="134"/>
+      <c r="AE96" s="134"/>
+      <c r="AF96" s="134"/>
+      <c r="AG96" s="134"/>
+      <c r="AH96" s="134"/>
+      <c r="AI96" s="134"/>
+      <c r="AJ96" s="134"/>
+      <c r="AK96" s="134"/>
+      <c r="AL96" s="134"/>
+      <c r="AM96" s="134"/>
+      <c r="AN96" s="134"/>
+      <c r="AO96" s="134"/>
+      <c r="AP96" s="134"/>
+      <c r="AQ96" s="134"/>
+      <c r="AR96" s="134"/>
+      <c r="AS96" s="134"/>
       <c r="AT96" s="46"/>
     </row>
-    <row r="97" spans="1:46" ht="13" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:46" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A97" s="88"/>
       <c r="B97" s="89"/>
-      <c r="C97" s="143"/>
-      <c r="D97" s="143"/>
-      <c r="E97" s="143"/>
-      <c r="F97" s="143"/>
-      <c r="G97" s="143"/>
-      <c r="H97" s="143"/>
-      <c r="I97" s="143"/>
-      <c r="J97" s="143"/>
-      <c r="K97" s="143"/>
-      <c r="L97" s="143"/>
-      <c r="M97" s="143"/>
-      <c r="N97" s="143"/>
-      <c r="O97" s="143"/>
-      <c r="P97" s="143"/>
-      <c r="Q97" s="143"/>
-      <c r="R97" s="143"/>
-      <c r="S97" s="143"/>
-      <c r="T97" s="143"/>
-      <c r="U97" s="143"/>
-      <c r="V97" s="143"/>
-      <c r="W97" s="143"/>
-      <c r="X97" s="143"/>
-      <c r="Y97" s="143"/>
-      <c r="Z97" s="143"/>
-      <c r="AA97" s="143"/>
-      <c r="AB97" s="143"/>
-      <c r="AC97" s="143"/>
-      <c r="AD97" s="143"/>
-      <c r="AE97" s="143"/>
-      <c r="AF97" s="143"/>
-      <c r="AG97" s="143"/>
-      <c r="AH97" s="143"/>
-      <c r="AI97" s="143"/>
-      <c r="AJ97" s="143"/>
-      <c r="AK97" s="143"/>
-      <c r="AL97" s="143"/>
-      <c r="AM97" s="143"/>
-      <c r="AN97" s="143"/>
-      <c r="AO97" s="143"/>
-      <c r="AP97" s="143"/>
-      <c r="AQ97" s="143"/>
-      <c r="AR97" s="143"/>
-      <c r="AS97" s="143"/>
+      <c r="C97" s="134"/>
+      <c r="D97" s="134"/>
+      <c r="E97" s="134"/>
+      <c r="F97" s="134"/>
+      <c r="G97" s="134"/>
+      <c r="H97" s="134"/>
+      <c r="I97" s="134"/>
+      <c r="J97" s="134"/>
+      <c r="K97" s="134"/>
+      <c r="L97" s="134"/>
+      <c r="M97" s="134"/>
+      <c r="N97" s="134"/>
+      <c r="O97" s="134"/>
+      <c r="P97" s="134"/>
+      <c r="Q97" s="134"/>
+      <c r="R97" s="134"/>
+      <c r="S97" s="134"/>
+      <c r="T97" s="134"/>
+      <c r="U97" s="134"/>
+      <c r="V97" s="134"/>
+      <c r="W97" s="134"/>
+      <c r="X97" s="134"/>
+      <c r="Y97" s="134"/>
+      <c r="Z97" s="134"/>
+      <c r="AA97" s="134"/>
+      <c r="AB97" s="134"/>
+      <c r="AC97" s="134"/>
+      <c r="AD97" s="134"/>
+      <c r="AE97" s="134"/>
+      <c r="AF97" s="134"/>
+      <c r="AG97" s="134"/>
+      <c r="AH97" s="134"/>
+      <c r="AI97" s="134"/>
+      <c r="AJ97" s="134"/>
+      <c r="AK97" s="134"/>
+      <c r="AL97" s="134"/>
+      <c r="AM97" s="134"/>
+      <c r="AN97" s="134"/>
+      <c r="AO97" s="134"/>
+      <c r="AP97" s="134"/>
+      <c r="AQ97" s="134"/>
+      <c r="AR97" s="134"/>
+      <c r="AS97" s="134"/>
       <c r="AT97" s="46"/>
     </row>
-    <row r="98" spans="1:46" ht="13" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:46" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A98" s="88"/>
       <c r="B98" s="89"/>
       <c r="C98" s="89"/>
@@ -7230,105 +7242,105 @@
       <c r="AR98" s="89"/>
       <c r="AT98" s="46"/>
     </row>
-    <row r="99" spans="1:46" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:46" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" s="88"/>
       <c r="B99" s="90"/>
-      <c r="C99" s="143" t="s">
+      <c r="C99" s="134" t="s">
         <v>87</v>
       </c>
-      <c r="D99" s="143"/>
-      <c r="E99" s="143"/>
-      <c r="F99" s="143"/>
-      <c r="G99" s="143"/>
-      <c r="H99" s="143"/>
-      <c r="I99" s="143"/>
-      <c r="J99" s="143"/>
-      <c r="K99" s="143"/>
-      <c r="L99" s="143"/>
-      <c r="M99" s="143"/>
-      <c r="N99" s="143"/>
-      <c r="O99" s="143"/>
-      <c r="P99" s="143"/>
-      <c r="Q99" s="143"/>
-      <c r="R99" s="143"/>
-      <c r="S99" s="143"/>
-      <c r="T99" s="143"/>
-      <c r="U99" s="143"/>
-      <c r="V99" s="143"/>
-      <c r="W99" s="143"/>
-      <c r="X99" s="143"/>
-      <c r="Y99" s="143"/>
-      <c r="Z99" s="143"/>
-      <c r="AA99" s="143"/>
-      <c r="AB99" s="143"/>
-      <c r="AC99" s="143"/>
-      <c r="AD99" s="143"/>
-      <c r="AE99" s="143"/>
-      <c r="AF99" s="143"/>
-      <c r="AG99" s="143"/>
-      <c r="AH99" s="143"/>
-      <c r="AI99" s="143"/>
-      <c r="AJ99" s="143"/>
-      <c r="AK99" s="143"/>
-      <c r="AL99" s="143"/>
-      <c r="AM99" s="143"/>
-      <c r="AN99" s="143"/>
-      <c r="AO99" s="143"/>
-      <c r="AP99" s="143"/>
-      <c r="AQ99" s="143"/>
-      <c r="AR99" s="143"/>
-      <c r="AS99" s="143"/>
+      <c r="D99" s="134"/>
+      <c r="E99" s="134"/>
+      <c r="F99" s="134"/>
+      <c r="G99" s="134"/>
+      <c r="H99" s="134"/>
+      <c r="I99" s="134"/>
+      <c r="J99" s="134"/>
+      <c r="K99" s="134"/>
+      <c r="L99" s="134"/>
+      <c r="M99" s="134"/>
+      <c r="N99" s="134"/>
+      <c r="O99" s="134"/>
+      <c r="P99" s="134"/>
+      <c r="Q99" s="134"/>
+      <c r="R99" s="134"/>
+      <c r="S99" s="134"/>
+      <c r="T99" s="134"/>
+      <c r="U99" s="134"/>
+      <c r="V99" s="134"/>
+      <c r="W99" s="134"/>
+      <c r="X99" s="134"/>
+      <c r="Y99" s="134"/>
+      <c r="Z99" s="134"/>
+      <c r="AA99" s="134"/>
+      <c r="AB99" s="134"/>
+      <c r="AC99" s="134"/>
+      <c r="AD99" s="134"/>
+      <c r="AE99" s="134"/>
+      <c r="AF99" s="134"/>
+      <c r="AG99" s="134"/>
+      <c r="AH99" s="134"/>
+      <c r="AI99" s="134"/>
+      <c r="AJ99" s="134"/>
+      <c r="AK99" s="134"/>
+      <c r="AL99" s="134"/>
+      <c r="AM99" s="134"/>
+      <c r="AN99" s="134"/>
+      <c r="AO99" s="134"/>
+      <c r="AP99" s="134"/>
+      <c r="AQ99" s="134"/>
+      <c r="AR99" s="134"/>
+      <c r="AS99" s="134"/>
       <c r="AT99" s="46"/>
     </row>
-    <row r="100" spans="1:46" ht="13" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:46" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A100" s="88"/>
       <c r="B100" s="89"/>
-      <c r="C100" s="143"/>
-      <c r="D100" s="143"/>
-      <c r="E100" s="143"/>
-      <c r="F100" s="143"/>
-      <c r="G100" s="143"/>
-      <c r="H100" s="143"/>
-      <c r="I100" s="143"/>
-      <c r="J100" s="143"/>
-      <c r="K100" s="143"/>
-      <c r="L100" s="143"/>
-      <c r="M100" s="143"/>
-      <c r="N100" s="143"/>
-      <c r="O100" s="143"/>
-      <c r="P100" s="143"/>
-      <c r="Q100" s="143"/>
-      <c r="R100" s="143"/>
-      <c r="S100" s="143"/>
-      <c r="T100" s="143"/>
-      <c r="U100" s="143"/>
-      <c r="V100" s="143"/>
-      <c r="W100" s="143"/>
-      <c r="X100" s="143"/>
-      <c r="Y100" s="143"/>
-      <c r="Z100" s="143"/>
-      <c r="AA100" s="143"/>
-      <c r="AB100" s="143"/>
-      <c r="AC100" s="143"/>
-      <c r="AD100" s="143"/>
-      <c r="AE100" s="143"/>
-      <c r="AF100" s="143"/>
-      <c r="AG100" s="143"/>
-      <c r="AH100" s="143"/>
-      <c r="AI100" s="143"/>
-      <c r="AJ100" s="143"/>
-      <c r="AK100" s="143"/>
-      <c r="AL100" s="143"/>
-      <c r="AM100" s="143"/>
-      <c r="AN100" s="143"/>
-      <c r="AO100" s="143"/>
-      <c r="AP100" s="143"/>
-      <c r="AQ100" s="143"/>
-      <c r="AR100" s="143"/>
-      <c r="AS100" s="143"/>
+      <c r="C100" s="134"/>
+      <c r="D100" s="134"/>
+      <c r="E100" s="134"/>
+      <c r="F100" s="134"/>
+      <c r="G100" s="134"/>
+      <c r="H100" s="134"/>
+      <c r="I100" s="134"/>
+      <c r="J100" s="134"/>
+      <c r="K100" s="134"/>
+      <c r="L100" s="134"/>
+      <c r="M100" s="134"/>
+      <c r="N100" s="134"/>
+      <c r="O100" s="134"/>
+      <c r="P100" s="134"/>
+      <c r="Q100" s="134"/>
+      <c r="R100" s="134"/>
+      <c r="S100" s="134"/>
+      <c r="T100" s="134"/>
+      <c r="U100" s="134"/>
+      <c r="V100" s="134"/>
+      <c r="W100" s="134"/>
+      <c r="X100" s="134"/>
+      <c r="Y100" s="134"/>
+      <c r="Z100" s="134"/>
+      <c r="AA100" s="134"/>
+      <c r="AB100" s="134"/>
+      <c r="AC100" s="134"/>
+      <c r="AD100" s="134"/>
+      <c r="AE100" s="134"/>
+      <c r="AF100" s="134"/>
+      <c r="AG100" s="134"/>
+      <c r="AH100" s="134"/>
+      <c r="AI100" s="134"/>
+      <c r="AJ100" s="134"/>
+      <c r="AK100" s="134"/>
+      <c r="AL100" s="134"/>
+      <c r="AM100" s="134"/>
+      <c r="AN100" s="134"/>
+      <c r="AO100" s="134"/>
+      <c r="AP100" s="134"/>
+      <c r="AQ100" s="134"/>
+      <c r="AR100" s="134"/>
+      <c r="AS100" s="134"/>
       <c r="AT100" s="46"/>
     </row>
-    <row r="101" spans="1:46" ht="5.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:46" ht="5.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A101" s="88"/>
       <c r="B101" s="89"/>
       <c r="C101" s="92"/>
@@ -7375,7 +7387,7 @@
       <c r="AR101" s="89"/>
       <c r="AT101" s="46"/>
     </row>
-    <row r="102" spans="1:46" ht="13" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:46" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A102" s="88"/>
       <c r="B102" s="90"/>
       <c r="C102" s="89" t="s">
@@ -7424,7 +7436,7 @@
       <c r="AR102" s="89"/>
       <c r="AT102" s="46"/>
     </row>
-    <row r="103" spans="1:46" ht="5.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:46" ht="5.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A103" s="88"/>
       <c r="B103" s="89"/>
       <c r="C103" s="89"/>
@@ -7471,7 +7483,7 @@
       <c r="AR103" s="89"/>
       <c r="AT103" s="46"/>
     </row>
-    <row r="104" spans="1:46" ht="13" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:46" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A104" s="88"/>
       <c r="B104" s="90"/>
       <c r="C104" s="89" t="s">
@@ -7520,7 +7532,7 @@
       <c r="AR104" s="89"/>
       <c r="AT104" s="46"/>
     </row>
-    <row r="105" spans="1:46" ht="5.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:46" ht="5.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A105" s="88"/>
       <c r="B105" s="89"/>
       <c r="C105" s="89"/>
@@ -7567,7 +7579,7 @@
       <c r="AR105" s="89"/>
       <c r="AT105" s="46"/>
     </row>
-    <row r="106" spans="1:46" ht="13" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:46" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A106" s="88"/>
       <c r="B106" s="90"/>
       <c r="C106" s="89" t="s">
@@ -7616,7 +7628,7 @@
       <c r="AR106" s="89"/>
       <c r="AT106" s="46"/>
     </row>
-    <row r="107" spans="1:46" ht="5.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:46" ht="5.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A107" s="88"/>
       <c r="B107" s="89"/>
       <c r="C107" s="89"/>
@@ -7663,7 +7675,7 @@
       <c r="AR107" s="89"/>
       <c r="AT107" s="46"/>
     </row>
-    <row r="108" spans="1:46" ht="13" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:46" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A108" s="88"/>
       <c r="B108" s="90"/>
       <c r="C108" s="89" t="s">
@@ -7712,7 +7724,7 @@
       <c r="AR108" s="89"/>
       <c r="AT108" s="46"/>
     </row>
-    <row r="109" spans="1:46" ht="5.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:46" ht="5.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A109" s="88"/>
       <c r="B109" s="89"/>
       <c r="C109" s="89"/>
@@ -7759,103 +7771,103 @@
       <c r="AR109" s="89"/>
       <c r="AT109" s="46"/>
     </row>
-    <row r="110" spans="1:46" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:46" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A110" s="88"/>
       <c r="B110" s="90"/>
-      <c r="C110" s="143" t="s">
+      <c r="C110" s="134" t="s">
         <v>79</v>
       </c>
-      <c r="D110" s="143"/>
-      <c r="E110" s="143"/>
-      <c r="F110" s="143"/>
-      <c r="G110" s="143"/>
-      <c r="H110" s="143"/>
-      <c r="I110" s="143"/>
-      <c r="J110" s="143"/>
-      <c r="K110" s="143"/>
-      <c r="L110" s="143"/>
-      <c r="M110" s="143"/>
-      <c r="N110" s="143"/>
-      <c r="O110" s="143"/>
-      <c r="P110" s="143"/>
-      <c r="Q110" s="143"/>
-      <c r="R110" s="143"/>
-      <c r="S110" s="143"/>
-      <c r="T110" s="143"/>
-      <c r="U110" s="143"/>
-      <c r="V110" s="143"/>
-      <c r="W110" s="143"/>
-      <c r="X110" s="143"/>
-      <c r="Y110" s="143"/>
-      <c r="Z110" s="143"/>
-      <c r="AA110" s="143"/>
-      <c r="AB110" s="143"/>
-      <c r="AC110" s="143"/>
-      <c r="AD110" s="143"/>
-      <c r="AE110" s="143"/>
-      <c r="AF110" s="143"/>
-      <c r="AG110" s="143"/>
-      <c r="AH110" s="143"/>
-      <c r="AI110" s="143"/>
-      <c r="AJ110" s="143"/>
-      <c r="AK110" s="143"/>
-      <c r="AL110" s="143"/>
-      <c r="AM110" s="143"/>
-      <c r="AN110" s="143"/>
-      <c r="AO110" s="143"/>
-      <c r="AP110" s="143"/>
-      <c r="AQ110" s="143"/>
+      <c r="D110" s="134"/>
+      <c r="E110" s="134"/>
+      <c r="F110" s="134"/>
+      <c r="G110" s="134"/>
+      <c r="H110" s="134"/>
+      <c r="I110" s="134"/>
+      <c r="J110" s="134"/>
+      <c r="K110" s="134"/>
+      <c r="L110" s="134"/>
+      <c r="M110" s="134"/>
+      <c r="N110" s="134"/>
+      <c r="O110" s="134"/>
+      <c r="P110" s="134"/>
+      <c r="Q110" s="134"/>
+      <c r="R110" s="134"/>
+      <c r="S110" s="134"/>
+      <c r="T110" s="134"/>
+      <c r="U110" s="134"/>
+      <c r="V110" s="134"/>
+      <c r="W110" s="134"/>
+      <c r="X110" s="134"/>
+      <c r="Y110" s="134"/>
+      <c r="Z110" s="134"/>
+      <c r="AA110" s="134"/>
+      <c r="AB110" s="134"/>
+      <c r="AC110" s="134"/>
+      <c r="AD110" s="134"/>
+      <c r="AE110" s="134"/>
+      <c r="AF110" s="134"/>
+      <c r="AG110" s="134"/>
+      <c r="AH110" s="134"/>
+      <c r="AI110" s="134"/>
+      <c r="AJ110" s="134"/>
+      <c r="AK110" s="134"/>
+      <c r="AL110" s="134"/>
+      <c r="AM110" s="134"/>
+      <c r="AN110" s="134"/>
+      <c r="AO110" s="134"/>
+      <c r="AP110" s="134"/>
+      <c r="AQ110" s="134"/>
       <c r="AR110" s="89"/>
       <c r="AT110" s="46"/>
     </row>
-    <row r="111" spans="1:46" ht="13" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:46" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A111" s="88"/>
       <c r="B111" s="93"/>
-      <c r="C111" s="143"/>
-      <c r="D111" s="143"/>
-      <c r="E111" s="143"/>
-      <c r="F111" s="143"/>
-      <c r="G111" s="143"/>
-      <c r="H111" s="143"/>
-      <c r="I111" s="143"/>
-      <c r="J111" s="143"/>
-      <c r="K111" s="143"/>
-      <c r="L111" s="143"/>
-      <c r="M111" s="143"/>
-      <c r="N111" s="143"/>
-      <c r="O111" s="143"/>
-      <c r="P111" s="143"/>
-      <c r="Q111" s="143"/>
-      <c r="R111" s="143"/>
-      <c r="S111" s="143"/>
-      <c r="T111" s="143"/>
-      <c r="U111" s="143"/>
-      <c r="V111" s="143"/>
-      <c r="W111" s="143"/>
-      <c r="X111" s="143"/>
-      <c r="Y111" s="143"/>
-      <c r="Z111" s="143"/>
-      <c r="AA111" s="143"/>
-      <c r="AB111" s="143"/>
-      <c r="AC111" s="143"/>
-      <c r="AD111" s="143"/>
-      <c r="AE111" s="143"/>
-      <c r="AF111" s="143"/>
-      <c r="AG111" s="143"/>
-      <c r="AH111" s="143"/>
-      <c r="AI111" s="143"/>
-      <c r="AJ111" s="143"/>
-      <c r="AK111" s="143"/>
-      <c r="AL111" s="143"/>
-      <c r="AM111" s="143"/>
-      <c r="AN111" s="143"/>
-      <c r="AO111" s="143"/>
-      <c r="AP111" s="143"/>
-      <c r="AQ111" s="143"/>
+      <c r="C111" s="134"/>
+      <c r="D111" s="134"/>
+      <c r="E111" s="134"/>
+      <c r="F111" s="134"/>
+      <c r="G111" s="134"/>
+      <c r="H111" s="134"/>
+      <c r="I111" s="134"/>
+      <c r="J111" s="134"/>
+      <c r="K111" s="134"/>
+      <c r="L111" s="134"/>
+      <c r="M111" s="134"/>
+      <c r="N111" s="134"/>
+      <c r="O111" s="134"/>
+      <c r="P111" s="134"/>
+      <c r="Q111" s="134"/>
+      <c r="R111" s="134"/>
+      <c r="S111" s="134"/>
+      <c r="T111" s="134"/>
+      <c r="U111" s="134"/>
+      <c r="V111" s="134"/>
+      <c r="W111" s="134"/>
+      <c r="X111" s="134"/>
+      <c r="Y111" s="134"/>
+      <c r="Z111" s="134"/>
+      <c r="AA111" s="134"/>
+      <c r="AB111" s="134"/>
+      <c r="AC111" s="134"/>
+      <c r="AD111" s="134"/>
+      <c r="AE111" s="134"/>
+      <c r="AF111" s="134"/>
+      <c r="AG111" s="134"/>
+      <c r="AH111" s="134"/>
+      <c r="AI111" s="134"/>
+      <c r="AJ111" s="134"/>
+      <c r="AK111" s="134"/>
+      <c r="AL111" s="134"/>
+      <c r="AM111" s="134"/>
+      <c r="AN111" s="134"/>
+      <c r="AO111" s="134"/>
+      <c r="AP111" s="134"/>
+      <c r="AQ111" s="134"/>
       <c r="AR111" s="89"/>
       <c r="AT111" s="46"/>
     </row>
-    <row r="112" spans="1:46" ht="5.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:46" ht="5.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A112" s="88"/>
       <c r="B112" s="89"/>
       <c r="C112" s="89"/>
@@ -7902,150 +7914,150 @@
       <c r="AR112" s="89"/>
       <c r="AT112" s="46"/>
     </row>
-    <row r="113" spans="1:46" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:46" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A113" s="88"/>
       <c r="B113" s="90"/>
-      <c r="C113" s="142" t="s">
+      <c r="C113" s="133" t="s">
         <v>80</v>
       </c>
-      <c r="D113" s="142"/>
-      <c r="E113" s="142"/>
-      <c r="F113" s="142"/>
-      <c r="G113" s="142"/>
-      <c r="H113" s="142"/>
-      <c r="I113" s="142"/>
-      <c r="J113" s="142"/>
-      <c r="K113" s="142"/>
-      <c r="L113" s="142"/>
-      <c r="M113" s="142"/>
-      <c r="N113" s="142"/>
-      <c r="O113" s="142"/>
-      <c r="P113" s="142"/>
-      <c r="Q113" s="142"/>
-      <c r="R113" s="142"/>
-      <c r="S113" s="142"/>
-      <c r="T113" s="142"/>
-      <c r="U113" s="142"/>
-      <c r="V113" s="142"/>
-      <c r="W113" s="142"/>
-      <c r="X113" s="142"/>
-      <c r="Y113" s="142"/>
-      <c r="Z113" s="142"/>
-      <c r="AA113" s="142"/>
-      <c r="AB113" s="142"/>
-      <c r="AC113" s="142"/>
-      <c r="AD113" s="142"/>
-      <c r="AE113" s="142"/>
-      <c r="AF113" s="142"/>
-      <c r="AG113" s="142"/>
-      <c r="AH113" s="142"/>
-      <c r="AI113" s="142"/>
-      <c r="AJ113" s="142"/>
-      <c r="AK113" s="142"/>
-      <c r="AL113" s="142"/>
-      <c r="AM113" s="142"/>
-      <c r="AN113" s="142"/>
-      <c r="AO113" s="142"/>
-      <c r="AP113" s="142"/>
-      <c r="AQ113" s="142"/>
-      <c r="AR113" s="142"/>
+      <c r="D113" s="133"/>
+      <c r="E113" s="133"/>
+      <c r="F113" s="133"/>
+      <c r="G113" s="133"/>
+      <c r="H113" s="133"/>
+      <c r="I113" s="133"/>
+      <c r="J113" s="133"/>
+      <c r="K113" s="133"/>
+      <c r="L113" s="133"/>
+      <c r="M113" s="133"/>
+      <c r="N113" s="133"/>
+      <c r="O113" s="133"/>
+      <c r="P113" s="133"/>
+      <c r="Q113" s="133"/>
+      <c r="R113" s="133"/>
+      <c r="S113" s="133"/>
+      <c r="T113" s="133"/>
+      <c r="U113" s="133"/>
+      <c r="V113" s="133"/>
+      <c r="W113" s="133"/>
+      <c r="X113" s="133"/>
+      <c r="Y113" s="133"/>
+      <c r="Z113" s="133"/>
+      <c r="AA113" s="133"/>
+      <c r="AB113" s="133"/>
+      <c r="AC113" s="133"/>
+      <c r="AD113" s="133"/>
+      <c r="AE113" s="133"/>
+      <c r="AF113" s="133"/>
+      <c r="AG113" s="133"/>
+      <c r="AH113" s="133"/>
+      <c r="AI113" s="133"/>
+      <c r="AJ113" s="133"/>
+      <c r="AK113" s="133"/>
+      <c r="AL113" s="133"/>
+      <c r="AM113" s="133"/>
+      <c r="AN113" s="133"/>
+      <c r="AO113" s="133"/>
+      <c r="AP113" s="133"/>
+      <c r="AQ113" s="133"/>
+      <c r="AR113" s="133"/>
       <c r="AT113" s="46"/>
     </row>
-    <row r="114" spans="1:46" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:46" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A114" s="88"/>
       <c r="B114" s="93"/>
-      <c r="C114" s="142"/>
-      <c r="D114" s="142"/>
-      <c r="E114" s="142"/>
-      <c r="F114" s="142"/>
-      <c r="G114" s="142"/>
-      <c r="H114" s="142"/>
-      <c r="I114" s="142"/>
-      <c r="J114" s="142"/>
-      <c r="K114" s="142"/>
-      <c r="L114" s="142"/>
-      <c r="M114" s="142"/>
-      <c r="N114" s="142"/>
-      <c r="O114" s="142"/>
-      <c r="P114" s="142"/>
-      <c r="Q114" s="142"/>
-      <c r="R114" s="142"/>
-      <c r="S114" s="142"/>
-      <c r="T114" s="142"/>
-      <c r="U114" s="142"/>
-      <c r="V114" s="142"/>
-      <c r="W114" s="142"/>
-      <c r="X114" s="142"/>
-      <c r="Y114" s="142"/>
-      <c r="Z114" s="142"/>
-      <c r="AA114" s="142"/>
-      <c r="AB114" s="142"/>
-      <c r="AC114" s="142"/>
-      <c r="AD114" s="142"/>
-      <c r="AE114" s="142"/>
-      <c r="AF114" s="142"/>
-      <c r="AG114" s="142"/>
-      <c r="AH114" s="142"/>
-      <c r="AI114" s="142"/>
-      <c r="AJ114" s="142"/>
-      <c r="AK114" s="142"/>
-      <c r="AL114" s="142"/>
-      <c r="AM114" s="142"/>
-      <c r="AN114" s="142"/>
-      <c r="AO114" s="142"/>
-      <c r="AP114" s="142"/>
-      <c r="AQ114" s="142"/>
-      <c r="AR114" s="142"/>
+      <c r="C114" s="133"/>
+      <c r="D114" s="133"/>
+      <c r="E114" s="133"/>
+      <c r="F114" s="133"/>
+      <c r="G114" s="133"/>
+      <c r="H114" s="133"/>
+      <c r="I114" s="133"/>
+      <c r="J114" s="133"/>
+      <c r="K114" s="133"/>
+      <c r="L114" s="133"/>
+      <c r="M114" s="133"/>
+      <c r="N114" s="133"/>
+      <c r="O114" s="133"/>
+      <c r="P114" s="133"/>
+      <c r="Q114" s="133"/>
+      <c r="R114" s="133"/>
+      <c r="S114" s="133"/>
+      <c r="T114" s="133"/>
+      <c r="U114" s="133"/>
+      <c r="V114" s="133"/>
+      <c r="W114" s="133"/>
+      <c r="X114" s="133"/>
+      <c r="Y114" s="133"/>
+      <c r="Z114" s="133"/>
+      <c r="AA114" s="133"/>
+      <c r="AB114" s="133"/>
+      <c r="AC114" s="133"/>
+      <c r="AD114" s="133"/>
+      <c r="AE114" s="133"/>
+      <c r="AF114" s="133"/>
+      <c r="AG114" s="133"/>
+      <c r="AH114" s="133"/>
+      <c r="AI114" s="133"/>
+      <c r="AJ114" s="133"/>
+      <c r="AK114" s="133"/>
+      <c r="AL114" s="133"/>
+      <c r="AM114" s="133"/>
+      <c r="AN114" s="133"/>
+      <c r="AO114" s="133"/>
+      <c r="AP114" s="133"/>
+      <c r="AQ114" s="133"/>
+      <c r="AR114" s="133"/>
       <c r="AT114" s="46"/>
     </row>
-    <row r="115" spans="1:46" ht="13" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:46" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A115" s="88"/>
       <c r="B115" s="93"/>
-      <c r="C115" s="142"/>
-      <c r="D115" s="142"/>
-      <c r="E115" s="142"/>
-      <c r="F115" s="142"/>
-      <c r="G115" s="142"/>
-      <c r="H115" s="142"/>
-      <c r="I115" s="142"/>
-      <c r="J115" s="142"/>
-      <c r="K115" s="142"/>
-      <c r="L115" s="142"/>
-      <c r="M115" s="142"/>
-      <c r="N115" s="142"/>
-      <c r="O115" s="142"/>
-      <c r="P115" s="142"/>
-      <c r="Q115" s="142"/>
-      <c r="R115" s="142"/>
-      <c r="S115" s="142"/>
-      <c r="T115" s="142"/>
-      <c r="U115" s="142"/>
-      <c r="V115" s="142"/>
-      <c r="W115" s="142"/>
-      <c r="X115" s="142"/>
-      <c r="Y115" s="142"/>
-      <c r="Z115" s="142"/>
-      <c r="AA115" s="142"/>
-      <c r="AB115" s="142"/>
-      <c r="AC115" s="142"/>
-      <c r="AD115" s="142"/>
-      <c r="AE115" s="142"/>
-      <c r="AF115" s="142"/>
-      <c r="AG115" s="142"/>
-      <c r="AH115" s="142"/>
-      <c r="AI115" s="142"/>
-      <c r="AJ115" s="142"/>
-      <c r="AK115" s="142"/>
-      <c r="AL115" s="142"/>
-      <c r="AM115" s="142"/>
-      <c r="AN115" s="142"/>
-      <c r="AO115" s="142"/>
-      <c r="AP115" s="142"/>
-      <c r="AQ115" s="142"/>
-      <c r="AR115" s="142"/>
+      <c r="C115" s="133"/>
+      <c r="D115" s="133"/>
+      <c r="E115" s="133"/>
+      <c r="F115" s="133"/>
+      <c r="G115" s="133"/>
+      <c r="H115" s="133"/>
+      <c r="I115" s="133"/>
+      <c r="J115" s="133"/>
+      <c r="K115" s="133"/>
+      <c r="L115" s="133"/>
+      <c r="M115" s="133"/>
+      <c r="N115" s="133"/>
+      <c r="O115" s="133"/>
+      <c r="P115" s="133"/>
+      <c r="Q115" s="133"/>
+      <c r="R115" s="133"/>
+      <c r="S115" s="133"/>
+      <c r="T115" s="133"/>
+      <c r="U115" s="133"/>
+      <c r="V115" s="133"/>
+      <c r="W115" s="133"/>
+      <c r="X115" s="133"/>
+      <c r="Y115" s="133"/>
+      <c r="Z115" s="133"/>
+      <c r="AA115" s="133"/>
+      <c r="AB115" s="133"/>
+      <c r="AC115" s="133"/>
+      <c r="AD115" s="133"/>
+      <c r="AE115" s="133"/>
+      <c r="AF115" s="133"/>
+      <c r="AG115" s="133"/>
+      <c r="AH115" s="133"/>
+      <c r="AI115" s="133"/>
+      <c r="AJ115" s="133"/>
+      <c r="AK115" s="133"/>
+      <c r="AL115" s="133"/>
+      <c r="AM115" s="133"/>
+      <c r="AN115" s="133"/>
+      <c r="AO115" s="133"/>
+      <c r="AP115" s="133"/>
+      <c r="AQ115" s="133"/>
+      <c r="AR115" s="133"/>
       <c r="AT115" s="46"/>
     </row>
-    <row r="116" spans="1:46" ht="5.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:46" ht="5.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A116" s="88"/>
       <c r="B116" s="89"/>
       <c r="C116" s="89"/>
@@ -8092,7 +8104,7 @@
       <c r="AR116" s="89"/>
       <c r="AT116" s="46"/>
     </row>
-    <row r="117" spans="1:46" ht="13" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:46" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A117" s="88"/>
       <c r="B117" s="90"/>
       <c r="C117" s="89" t="s">
@@ -8141,7 +8153,7 @@
       <c r="AR117" s="89"/>
       <c r="AT117" s="46"/>
     </row>
-    <row r="118" spans="1:46" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:46" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A118" s="88"/>
       <c r="B118" s="93"/>
       <c r="C118" s="89"/>
@@ -8189,7 +8201,7 @@
       <c r="AS118" s="56"/>
       <c r="AT118" s="46"/>
     </row>
-    <row r="119" spans="1:46" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:46" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A119" s="88"/>
       <c r="B119" s="89"/>
       <c r="C119" s="89"/>
@@ -8237,7 +8249,7 @@
       <c r="AS119" s="25"/>
       <c r="AT119" s="46"/>
     </row>
-    <row r="120" spans="1:46" ht="13" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:46" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A120" s="88"/>
       <c r="B120" s="89"/>
       <c r="C120" s="89"/>
@@ -8284,105 +8296,105 @@
       <c r="AR120" s="89"/>
       <c r="AT120" s="46"/>
     </row>
-    <row r="121" spans="1:46" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:46" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A121" s="88"/>
       <c r="B121" s="89"/>
-      <c r="C121" s="117" t="s">
+      <c r="C121" s="163" t="s">
         <v>82</v>
       </c>
-      <c r="D121" s="117"/>
-      <c r="E121" s="117"/>
-      <c r="F121" s="117"/>
-      <c r="G121" s="117"/>
-      <c r="H121" s="117"/>
-      <c r="I121" s="117"/>
-      <c r="J121" s="117"/>
-      <c r="K121" s="117"/>
-      <c r="L121" s="117"/>
-      <c r="M121" s="117"/>
-      <c r="N121" s="117"/>
-      <c r="O121" s="117"/>
-      <c r="P121" s="117"/>
-      <c r="Q121" s="117"/>
-      <c r="R121" s="117"/>
-      <c r="S121" s="117"/>
-      <c r="T121" s="117"/>
-      <c r="U121" s="117"/>
-      <c r="V121" s="117"/>
-      <c r="W121" s="117"/>
-      <c r="X121" s="117"/>
-      <c r="Y121" s="117"/>
-      <c r="Z121" s="117"/>
-      <c r="AA121" s="117"/>
-      <c r="AB121" s="117"/>
-      <c r="AC121" s="117"/>
-      <c r="AD121" s="117"/>
-      <c r="AE121" s="117"/>
-      <c r="AF121" s="117"/>
-      <c r="AG121" s="117"/>
-      <c r="AH121" s="117"/>
-      <c r="AI121" s="117"/>
-      <c r="AJ121" s="117"/>
-      <c r="AK121" s="117"/>
-      <c r="AL121" s="117"/>
-      <c r="AM121" s="117"/>
-      <c r="AN121" s="117"/>
-      <c r="AO121" s="117"/>
-      <c r="AP121" s="117"/>
-      <c r="AQ121" s="117"/>
-      <c r="AR121" s="117"/>
-      <c r="AS121" s="117"/>
+      <c r="D121" s="163"/>
+      <c r="E121" s="163"/>
+      <c r="F121" s="163"/>
+      <c r="G121" s="163"/>
+      <c r="H121" s="163"/>
+      <c r="I121" s="163"/>
+      <c r="J121" s="163"/>
+      <c r="K121" s="163"/>
+      <c r="L121" s="163"/>
+      <c r="M121" s="163"/>
+      <c r="N121" s="163"/>
+      <c r="O121" s="163"/>
+      <c r="P121" s="163"/>
+      <c r="Q121" s="163"/>
+      <c r="R121" s="163"/>
+      <c r="S121" s="163"/>
+      <c r="T121" s="163"/>
+      <c r="U121" s="163"/>
+      <c r="V121" s="163"/>
+      <c r="W121" s="163"/>
+      <c r="X121" s="163"/>
+      <c r="Y121" s="163"/>
+      <c r="Z121" s="163"/>
+      <c r="AA121" s="163"/>
+      <c r="AB121" s="163"/>
+      <c r="AC121" s="163"/>
+      <c r="AD121" s="163"/>
+      <c r="AE121" s="163"/>
+      <c r="AF121" s="163"/>
+      <c r="AG121" s="163"/>
+      <c r="AH121" s="163"/>
+      <c r="AI121" s="163"/>
+      <c r="AJ121" s="163"/>
+      <c r="AK121" s="163"/>
+      <c r="AL121" s="163"/>
+      <c r="AM121" s="163"/>
+      <c r="AN121" s="163"/>
+      <c r="AO121" s="163"/>
+      <c r="AP121" s="163"/>
+      <c r="AQ121" s="163"/>
+      <c r="AR121" s="163"/>
+      <c r="AS121" s="163"/>
       <c r="AT121" s="46"/>
     </row>
-    <row r="122" spans="1:46" ht="13" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:46" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A122" s="88"/>
       <c r="B122" s="89"/>
-      <c r="C122" s="117"/>
-      <c r="D122" s="117"/>
-      <c r="E122" s="117"/>
-      <c r="F122" s="117"/>
-      <c r="G122" s="117"/>
-      <c r="H122" s="117"/>
-      <c r="I122" s="117"/>
-      <c r="J122" s="117"/>
-      <c r="K122" s="117"/>
-      <c r="L122" s="117"/>
-      <c r="M122" s="117"/>
-      <c r="N122" s="117"/>
-      <c r="O122" s="117"/>
-      <c r="P122" s="117"/>
-      <c r="Q122" s="117"/>
-      <c r="R122" s="117"/>
-      <c r="S122" s="117"/>
-      <c r="T122" s="117"/>
-      <c r="U122" s="117"/>
-      <c r="V122" s="117"/>
-      <c r="W122" s="117"/>
-      <c r="X122" s="117"/>
-      <c r="Y122" s="117"/>
-      <c r="Z122" s="117"/>
-      <c r="AA122" s="117"/>
-      <c r="AB122" s="117"/>
-      <c r="AC122" s="117"/>
-      <c r="AD122" s="117"/>
-      <c r="AE122" s="117"/>
-      <c r="AF122" s="117"/>
-      <c r="AG122" s="117"/>
-      <c r="AH122" s="117"/>
-      <c r="AI122" s="117"/>
-      <c r="AJ122" s="117"/>
-      <c r="AK122" s="117"/>
-      <c r="AL122" s="117"/>
-      <c r="AM122" s="117"/>
-      <c r="AN122" s="117"/>
-      <c r="AO122" s="117"/>
-      <c r="AP122" s="117"/>
-      <c r="AQ122" s="117"/>
-      <c r="AR122" s="117"/>
-      <c r="AS122" s="117"/>
+      <c r="C122" s="163"/>
+      <c r="D122" s="163"/>
+      <c r="E122" s="163"/>
+      <c r="F122" s="163"/>
+      <c r="G122" s="163"/>
+      <c r="H122" s="163"/>
+      <c r="I122" s="163"/>
+      <c r="J122" s="163"/>
+      <c r="K122" s="163"/>
+      <c r="L122" s="163"/>
+      <c r="M122" s="163"/>
+      <c r="N122" s="163"/>
+      <c r="O122" s="163"/>
+      <c r="P122" s="163"/>
+      <c r="Q122" s="163"/>
+      <c r="R122" s="163"/>
+      <c r="S122" s="163"/>
+      <c r="T122" s="163"/>
+      <c r="U122" s="163"/>
+      <c r="V122" s="163"/>
+      <c r="W122" s="163"/>
+      <c r="X122" s="163"/>
+      <c r="Y122" s="163"/>
+      <c r="Z122" s="163"/>
+      <c r="AA122" s="163"/>
+      <c r="AB122" s="163"/>
+      <c r="AC122" s="163"/>
+      <c r="AD122" s="163"/>
+      <c r="AE122" s="163"/>
+      <c r="AF122" s="163"/>
+      <c r="AG122" s="163"/>
+      <c r="AH122" s="163"/>
+      <c r="AI122" s="163"/>
+      <c r="AJ122" s="163"/>
+      <c r="AK122" s="163"/>
+      <c r="AL122" s="163"/>
+      <c r="AM122" s="163"/>
+      <c r="AN122" s="163"/>
+      <c r="AO122" s="163"/>
+      <c r="AP122" s="163"/>
+      <c r="AQ122" s="163"/>
+      <c r="AR122" s="163"/>
+      <c r="AS122" s="163"/>
       <c r="AT122" s="46"/>
     </row>
-    <row r="123" spans="1:46" ht="13" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:46" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A123" s="88"/>
       <c r="B123" s="89"/>
       <c r="C123" s="89"/>
@@ -8429,7 +8441,7 @@
       <c r="AR123" s="89"/>
       <c r="AT123" s="46"/>
     </row>
-    <row r="124" spans="1:46" ht="13" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:46" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A124" s="96" t="s">
         <v>83</v>
       </c>
@@ -8479,7 +8491,7 @@
       <c r="AS124" s="98"/>
       <c r="AT124" s="99"/>
     </row>
-    <row r="125" spans="1:46" ht="13" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:46" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A125" s="88"/>
       <c r="B125" s="89"/>
       <c r="C125" s="89"/>
@@ -8526,7 +8538,7 @@
       <c r="AR125" s="89"/>
       <c r="AT125" s="46"/>
     </row>
-    <row r="126" spans="1:46" ht="13" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:46" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A126" s="88"/>
       <c r="B126" s="89"/>
       <c r="C126" s="89"/>
@@ -8573,7 +8585,7 @@
       <c r="AR126" s="89"/>
       <c r="AT126" s="46"/>
     </row>
-    <row r="127" spans="1:46" ht="13" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:46" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A127" s="88"/>
       <c r="B127" s="89"/>
       <c r="C127" s="89"/>
@@ -8620,71 +8632,71 @@
       <c r="AR127" s="89"/>
       <c r="AT127" s="46"/>
     </row>
-    <row r="128" spans="1:46" ht="13" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:46" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A128" s="88"/>
-      <c r="B128" s="104" t="s">
+      <c r="B128" s="151" t="s">
         <v>84</v>
       </c>
-      <c r="C128" s="104"/>
-      <c r="D128" s="104"/>
-      <c r="E128" s="104"/>
-      <c r="F128" s="104"/>
-      <c r="G128" s="104"/>
-      <c r="H128" s="104"/>
-      <c r="I128" s="104"/>
-      <c r="J128" s="104"/>
-      <c r="K128" s="104"/>
-      <c r="L128" s="104"/>
-      <c r="M128" s="104"/>
+      <c r="C128" s="151"/>
+      <c r="D128" s="151"/>
+      <c r="E128" s="151"/>
+      <c r="F128" s="151"/>
+      <c r="G128" s="151"/>
+      <c r="H128" s="151"/>
+      <c r="I128" s="151"/>
+      <c r="J128" s="151"/>
+      <c r="K128" s="151"/>
+      <c r="L128" s="151"/>
+      <c r="M128" s="151"/>
       <c r="N128" s="89"/>
       <c r="O128" s="89"/>
-      <c r="Q128" s="104" t="s">
+      <c r="Q128" s="151" t="s">
         <v>85</v>
       </c>
-      <c r="R128" s="104"/>
-      <c r="S128" s="104"/>
-      <c r="T128" s="104"/>
-      <c r="U128" s="104"/>
-      <c r="V128" s="104"/>
-      <c r="W128" s="104"/>
-      <c r="X128" s="104"/>
-      <c r="Y128" s="104"/>
-      <c r="Z128" s="104"/>
-      <c r="AA128" s="104"/>
-      <c r="AB128" s="104"/>
-      <c r="AC128" s="104"/>
-      <c r="AD128" s="104"/>
+      <c r="R128" s="151"/>
+      <c r="S128" s="151"/>
+      <c r="T128" s="151"/>
+      <c r="U128" s="151"/>
+      <c r="V128" s="151"/>
+      <c r="W128" s="151"/>
+      <c r="X128" s="151"/>
+      <c r="Y128" s="151"/>
+      <c r="Z128" s="151"/>
+      <c r="AA128" s="151"/>
+      <c r="AB128" s="151"/>
+      <c r="AC128" s="151"/>
+      <c r="AD128" s="151"/>
       <c r="AE128" s="89"/>
-      <c r="AH128" s="104" t="s">
+      <c r="AH128" s="151" t="s">
         <v>85</v>
       </c>
-      <c r="AI128" s="104"/>
-      <c r="AJ128" s="104"/>
-      <c r="AK128" s="104"/>
-      <c r="AL128" s="104"/>
-      <c r="AM128" s="104"/>
-      <c r="AN128" s="104"/>
-      <c r="AO128" s="104"/>
-      <c r="AP128" s="104"/>
-      <c r="AQ128" s="104"/>
-      <c r="AR128" s="104"/>
-      <c r="AS128" s="104"/>
+      <c r="AI128" s="151"/>
+      <c r="AJ128" s="151"/>
+      <c r="AK128" s="151"/>
+      <c r="AL128" s="151"/>
+      <c r="AM128" s="151"/>
+      <c r="AN128" s="151"/>
+      <c r="AO128" s="151"/>
+      <c r="AP128" s="151"/>
+      <c r="AQ128" s="151"/>
+      <c r="AR128" s="151"/>
+      <c r="AS128" s="151"/>
       <c r="AT128" s="46"/>
     </row>
-    <row r="129" spans="1:46" ht="13" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:46" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A129" s="88"/>
       <c r="B129" s="100"/>
       <c r="C129" s="100"/>
       <c r="D129" s="100"/>
-      <c r="E129" s="105" t="str">
+      <c r="E129" s="152" t="str">
         <f>IFERROR(VLOOKUP($B$3,Dados!K1:M9,2,),"")</f>
         <v/>
       </c>
-      <c r="F129" s="106"/>
-      <c r="G129" s="106"/>
-      <c r="H129" s="106"/>
-      <c r="I129" s="106"/>
-      <c r="J129" s="107"/>
+      <c r="F129" s="153"/>
+      <c r="G129" s="153"/>
+      <c r="H129" s="153"/>
+      <c r="I129" s="153"/>
+      <c r="J129" s="154"/>
       <c r="K129" s="89"/>
       <c r="L129" s="89"/>
       <c r="M129" s="89"/>
@@ -8719,19 +8731,19 @@
       <c r="AS129" s="89"/>
       <c r="AT129" s="46"/>
     </row>
-    <row r="130" spans="1:46" ht="13" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:46" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A130" s="88"/>
       <c r="B130" s="100"/>
       <c r="C130" s="100"/>
       <c r="D130" s="100"/>
-      <c r="E130" s="103" t="s">
+      <c r="E130" s="150" t="s">
         <v>64</v>
       </c>
-      <c r="F130" s="103"/>
-      <c r="G130" s="103"/>
-      <c r="H130" s="103"/>
-      <c r="I130" s="103"/>
-      <c r="J130" s="103"/>
+      <c r="F130" s="150"/>
+      <c r="G130" s="150"/>
+      <c r="H130" s="150"/>
+      <c r="I130" s="150"/>
+      <c r="J130" s="150"/>
       <c r="K130" s="89"/>
       <c r="L130" s="89"/>
       <c r="M130" s="89"/>
@@ -8770,7 +8782,7 @@
       <c r="AS130" s="94"/>
       <c r="AT130" s="46"/>
     </row>
-    <row r="131" spans="1:46" ht="13" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:46" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A131" s="101"/>
       <c r="B131" s="95"/>
       <c r="C131" s="95"/>
@@ -8819,8 +8831,48 @@
       <c r="AT131" s="68"/>
     </row>
   </sheetData>
-  <sheetProtection password="C13C" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection selectLockedCells="1"/>
   <mergeCells count="56">
+    <mergeCell ref="Z55:AS56"/>
+    <mergeCell ref="Z57:AS58"/>
+    <mergeCell ref="Z59:AS60"/>
+    <mergeCell ref="Z61:AS63"/>
+    <mergeCell ref="E130:J130"/>
+    <mergeCell ref="Q128:AD128"/>
+    <mergeCell ref="AH128:AS128"/>
+    <mergeCell ref="B128:M128"/>
+    <mergeCell ref="E129:J129"/>
+    <mergeCell ref="Q85:R85"/>
+    <mergeCell ref="B79:F79"/>
+    <mergeCell ref="T79:AO79"/>
+    <mergeCell ref="A82:AT83"/>
+    <mergeCell ref="B78:F78"/>
+    <mergeCell ref="T78:AO78"/>
+    <mergeCell ref="C121:AS122"/>
+    <mergeCell ref="Z53:AS54"/>
+    <mergeCell ref="Q46:AS49"/>
+    <mergeCell ref="B48:O48"/>
+    <mergeCell ref="D24:AS24"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="E26:J26"/>
+    <mergeCell ref="K26:M26"/>
+    <mergeCell ref="N26:AH26"/>
+    <mergeCell ref="AL26:AS26"/>
+    <mergeCell ref="F40:AS40"/>
+    <mergeCell ref="F42:AS42"/>
+    <mergeCell ref="B44:AS44"/>
+    <mergeCell ref="A42:E42"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B6:AS6"/>
+    <mergeCell ref="B11:M11"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="F3:I3"/>
+    <mergeCell ref="B8:AS8"/>
+    <mergeCell ref="C113:AR115"/>
+    <mergeCell ref="C110:AQ111"/>
+    <mergeCell ref="C99:AS100"/>
+    <mergeCell ref="C96:AS97"/>
+    <mergeCell ref="C93:AS94"/>
     <mergeCell ref="C61:V62"/>
     <mergeCell ref="C59:W60"/>
     <mergeCell ref="C55:W57"/>
@@ -8837,46 +8889,6 @@
     <mergeCell ref="D15:AH15"/>
     <mergeCell ref="S21:V21"/>
     <mergeCell ref="AL15:AS15"/>
-    <mergeCell ref="C113:AR115"/>
-    <mergeCell ref="C110:AQ111"/>
-    <mergeCell ref="C99:AS100"/>
-    <mergeCell ref="C96:AS97"/>
-    <mergeCell ref="C93:AS94"/>
-    <mergeCell ref="B6:AS6"/>
-    <mergeCell ref="B11:M11"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="F3:I3"/>
-    <mergeCell ref="B8:AS8"/>
-    <mergeCell ref="Z53:AS54"/>
-    <mergeCell ref="Q46:AS49"/>
-    <mergeCell ref="B48:O48"/>
-    <mergeCell ref="D24:AS24"/>
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="E26:J26"/>
-    <mergeCell ref="K26:M26"/>
-    <mergeCell ref="N26:AH26"/>
-    <mergeCell ref="AL26:AS26"/>
-    <mergeCell ref="F40:AS40"/>
-    <mergeCell ref="F42:AS42"/>
-    <mergeCell ref="B44:AS44"/>
-    <mergeCell ref="A42:E42"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="Z55:AS56"/>
-    <mergeCell ref="Z57:AS58"/>
-    <mergeCell ref="Z59:AS60"/>
-    <mergeCell ref="Z61:AS63"/>
-    <mergeCell ref="E130:J130"/>
-    <mergeCell ref="Q128:AD128"/>
-    <mergeCell ref="AH128:AS128"/>
-    <mergeCell ref="B128:M128"/>
-    <mergeCell ref="E129:J129"/>
-    <mergeCell ref="Q85:R85"/>
-    <mergeCell ref="B79:F79"/>
-    <mergeCell ref="T79:AO79"/>
-    <mergeCell ref="A82:AT83"/>
-    <mergeCell ref="B78:F78"/>
-    <mergeCell ref="T78:AO78"/>
-    <mergeCell ref="C121:AS122"/>
   </mergeCells>
   <conditionalFormatting sqref="A51:AT73">
     <cfRule type="expression" dxfId="5" priority="4">
@@ -8908,7 +8920,7 @@
       <formula>LEN(TRIM(B8))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations disablePrompts="1" count="9">
+  <dataValidations count="9">
     <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Opa!!" error="Digíte somente números!!" sqref="F3" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>1</formula1>
     </dataValidation>
@@ -8916,18 +8928,14 @@
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="III - Muito Graves, aquelas em que forem verificadas duas circunstâncias agravantes;" sqref="X72" xr:uid="{00000000-0002-0000-0000-000002000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="II - Graves, aquelas em que for verificada uma circunstância agravante;" sqref="L72" xr:uid="{00000000-0002-0000-0000-000003000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="I - Leves, aquelas em que o infrator seja beneficiado por circunstâncias atenuantes;" sqref="B72" xr:uid="{00000000-0002-0000-0000-000004000000}"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3:D3" xr:uid="{00000000-0002-0000-0000-000005000000}">
-      <formula1>"AIAN,AIMC,AITS,AIWL"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="E17:J17 E26:J26" xr:uid="{00000000-0002-0000-0000-000006000000}">
-      <formula1>"S/N"</formula1>
-    </dataValidation>
+    <dataValidation allowBlank="1" showInputMessage="1" sqref="E26:J26" xr:uid="{00000000-0002-0000-0000-000006000000}"/>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S21:V21" xr:uid="{00000000-0002-0000-0000-000007000000}">
       <formula1>"SIM,NÃO"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="B8:AS8" xr:uid="{00000000-0002-0000-0000-000008000000}">
       <formula1>"N/A"</formula1>
     </dataValidation>
+    <dataValidation allowBlank="1" showInputMessage="1" sqref="E17:J17" xr:uid="{68F80EDD-65B4-466D-A5BE-1AB772BE3762}"/>
   </dataValidations>
   <pageMargins left="0.51181102362204722" right="0.51181102362204722" top="0.78740157480314965" bottom="0.78740157480314965" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="93" fitToHeight="0" orientation="portrait" r:id="rId1"/>
@@ -8944,7 +8952,7 @@
   <legacyDrawingHF r:id="rId3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="7">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="7">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000009000000}">
           <x14:formula1>
             <xm:f>Dados!$C$8:$C$14</xm:f>
@@ -9001,15 +9009,15 @@
       <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.81640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="12" width="9.1796875" style="2"/>
-    <col min="13" max="13" width="37.54296875" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="9.1796875" style="2"/>
+    <col min="1" max="1" width="33.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="12" width="9.140625" style="2"/>
+    <col min="13" max="13" width="37.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="K1" s="5" t="s">
         <v>88</v>
       </c>
@@ -9020,7 +9028,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C2" s="6" t="s">
         <v>91</v>
       </c>
@@ -9039,7 +9047,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C3" s="7">
         <f>COUNTIF('Auto de Infração'!B53:B64,"X")</f>
         <v>0</v>
@@ -9060,7 +9068,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C4" s="6" t="s">
         <v>92</v>
       </c>
@@ -9080,7 +9088,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C5" s="7">
         <f>COUNTIF('Auto de Infração'!Y53:Y66,"X")</f>
         <v>0</v>
@@ -9100,12 +9108,12 @@
         <v>147</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="K6" s="9"/>
       <c r="L6" s="9"/>
       <c r="M6" s="9"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C7" s="11" t="s">
         <v>103</v>
       </c>
@@ -9117,7 +9125,7 @@
       <c r="L7" s="9"/>
       <c r="M7" s="9"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C8" s="10" t="s">
         <v>96</v>
       </c>
@@ -9131,7 +9139,7 @@
       <c r="L8" s="9"/>
       <c r="M8" s="9"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C9" s="10" t="s">
         <v>97</v>
       </c>
@@ -9145,32 +9153,32 @@
       <c r="L9" s="9"/>
       <c r="M9" s="9"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C10" s="10" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C11" s="10" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C12" s="10" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C13" s="10" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C14" s="10" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="10" t="s">
         <v>42</v>
       </c>
@@ -9178,7 +9186,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="10" t="s">
         <v>43</v>
       </c>
@@ -9186,7 +9194,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="10" t="s">
         <v>44</v>
       </c>
@@ -9194,7 +9202,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="10" t="s">
         <v>109</v>
       </c>
@@ -9202,7 +9210,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="10" t="s">
         <v>110</v>
       </c>
@@ -9210,7 +9218,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="10" t="s">
         <v>111</v>
       </c>
@@ -9218,7 +9226,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B23" s="15" t="s">
         <v>126</v>
       </c>
@@ -9232,7 +9240,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B24" s="16">
         <v>1</v>
       </c>
@@ -9246,7 +9254,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B25" s="16">
         <v>2</v>
       </c>
@@ -9260,7 +9268,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B26" s="16">
         <v>3</v>
       </c>
@@ -9274,7 +9282,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B27" s="16">
         <v>4</v>
       </c>
@@ -9288,7 +9296,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B28" s="16">
         <v>5</v>
       </c>
@@ -9302,7 +9310,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B29" s="16">
         <v>6</v>
       </c>
@@ -9316,7 +9324,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B30" s="16">
         <v>7</v>
       </c>
@@ -9330,7 +9338,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B31" s="16">
         <v>8</v>
       </c>

</xml_diff>

<commit_message>
back ajustando api para inserir numero do autuado na planilha
</commit_message>
<xml_diff>
--- a/syspzl-api/templates/modelo-auto-de-infracao.xlsx
+++ b/syspzl-api/templates/modelo-auto-de-infracao.xlsx
@@ -8,10 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\sistema_lixo_zero\syspzl-api\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF699227-0EB4-4E61-9881-8308C4C70DC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCC4E6EA-1608-4565-A471-469C227CFBCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookPassword="C13C" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-10910" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Auto de Infração" sheetId="1" r:id="rId1"/>
@@ -1212,6 +1212,148 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="165" fontId="12" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="170" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="170" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="170" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1261,45 +1403,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
@@ -1323,109 +1426,6 @@
     <xf numFmtId="167" fontId="13" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="12" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="170" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="170" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="170" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
@@ -2442,8 +2442,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AT131"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" showRuler="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:D3"/>
+    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" showRuler="0" topLeftCell="A3" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26:J26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2" defaultRowHeight="11.25" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2561,16 +2561,16 @@
       <c r="AT2" s="22"/>
     </row>
     <row r="3" spans="1:46" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="139"/>
-      <c r="C3" s="140"/>
-      <c r="D3" s="141"/>
+      <c r="B3" s="136"/>
+      <c r="C3" s="137"/>
+      <c r="D3" s="138"/>
       <c r="E3" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="142"/>
-      <c r="G3" s="143"/>
-      <c r="H3" s="143"/>
-      <c r="I3" s="144"/>
+      <c r="F3" s="139"/>
+      <c r="G3" s="140"/>
+      <c r="H3" s="140"/>
+      <c r="I3" s="141"/>
       <c r="J3" s="21"/>
       <c r="K3" s="21"/>
       <c r="L3" s="21"/>
@@ -2713,50 +2713,50 @@
     </row>
     <row r="6" spans="1:46" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="32"/>
-      <c r="B6" s="119"/>
-      <c r="C6" s="122"/>
-      <c r="D6" s="122"/>
-      <c r="E6" s="122"/>
-      <c r="F6" s="122"/>
-      <c r="G6" s="122"/>
-      <c r="H6" s="122"/>
-      <c r="I6" s="122"/>
-      <c r="J6" s="122"/>
-      <c r="K6" s="122"/>
-      <c r="L6" s="122"/>
-      <c r="M6" s="122"/>
-      <c r="N6" s="122"/>
-      <c r="O6" s="122"/>
-      <c r="P6" s="122"/>
-      <c r="Q6" s="122"/>
-      <c r="R6" s="122"/>
-      <c r="S6" s="122"/>
-      <c r="T6" s="122"/>
-      <c r="U6" s="122"/>
-      <c r="V6" s="122"/>
-      <c r="W6" s="122"/>
-      <c r="X6" s="122"/>
-      <c r="Y6" s="122"/>
-      <c r="Z6" s="122"/>
-      <c r="AA6" s="122"/>
-      <c r="AB6" s="122"/>
-      <c r="AC6" s="122"/>
-      <c r="AD6" s="122"/>
-      <c r="AE6" s="122"/>
-      <c r="AF6" s="122"/>
-      <c r="AG6" s="122"/>
-      <c r="AH6" s="122"/>
-      <c r="AI6" s="122"/>
-      <c r="AJ6" s="122"/>
-      <c r="AK6" s="122"/>
-      <c r="AL6" s="122"/>
-      <c r="AM6" s="122"/>
-      <c r="AN6" s="122"/>
-      <c r="AO6" s="122"/>
-      <c r="AP6" s="122"/>
-      <c r="AQ6" s="122"/>
-      <c r="AR6" s="122"/>
-      <c r="AS6" s="123"/>
+      <c r="B6" s="121"/>
+      <c r="C6" s="131"/>
+      <c r="D6" s="131"/>
+      <c r="E6" s="131"/>
+      <c r="F6" s="131"/>
+      <c r="G6" s="131"/>
+      <c r="H6" s="131"/>
+      <c r="I6" s="131"/>
+      <c r="J6" s="131"/>
+      <c r="K6" s="131"/>
+      <c r="L6" s="131"/>
+      <c r="M6" s="131"/>
+      <c r="N6" s="131"/>
+      <c r="O6" s="131"/>
+      <c r="P6" s="131"/>
+      <c r="Q6" s="131"/>
+      <c r="R6" s="131"/>
+      <c r="S6" s="131"/>
+      <c r="T6" s="131"/>
+      <c r="U6" s="131"/>
+      <c r="V6" s="131"/>
+      <c r="W6" s="131"/>
+      <c r="X6" s="131"/>
+      <c r="Y6" s="131"/>
+      <c r="Z6" s="131"/>
+      <c r="AA6" s="131"/>
+      <c r="AB6" s="131"/>
+      <c r="AC6" s="131"/>
+      <c r="AD6" s="131"/>
+      <c r="AE6" s="131"/>
+      <c r="AF6" s="131"/>
+      <c r="AG6" s="131"/>
+      <c r="AH6" s="131"/>
+      <c r="AI6" s="131"/>
+      <c r="AJ6" s="131"/>
+      <c r="AK6" s="131"/>
+      <c r="AL6" s="131"/>
+      <c r="AM6" s="131"/>
+      <c r="AN6" s="131"/>
+      <c r="AO6" s="131"/>
+      <c r="AP6" s="131"/>
+      <c r="AQ6" s="131"/>
+      <c r="AR6" s="131"/>
+      <c r="AS6" s="132"/>
       <c r="AT6" s="33"/>
     </row>
     <row r="7" spans="1:46" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -2811,50 +2811,50 @@
     </row>
     <row r="8" spans="1:46" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="34"/>
-      <c r="B8" s="119"/>
-      <c r="C8" s="122"/>
-      <c r="D8" s="122"/>
-      <c r="E8" s="122"/>
-      <c r="F8" s="122"/>
-      <c r="G8" s="122"/>
-      <c r="H8" s="122"/>
-      <c r="I8" s="122"/>
-      <c r="J8" s="122"/>
-      <c r="K8" s="122"/>
-      <c r="L8" s="122"/>
-      <c r="M8" s="122"/>
-      <c r="N8" s="122"/>
-      <c r="O8" s="122"/>
-      <c r="P8" s="122"/>
-      <c r="Q8" s="122"/>
-      <c r="R8" s="122"/>
-      <c r="S8" s="122"/>
-      <c r="T8" s="122"/>
-      <c r="U8" s="122"/>
-      <c r="V8" s="122"/>
-      <c r="W8" s="122"/>
-      <c r="X8" s="122"/>
-      <c r="Y8" s="122"/>
-      <c r="Z8" s="122"/>
-      <c r="AA8" s="122"/>
-      <c r="AB8" s="122"/>
-      <c r="AC8" s="122"/>
-      <c r="AD8" s="122"/>
-      <c r="AE8" s="122"/>
-      <c r="AF8" s="122"/>
-      <c r="AG8" s="122"/>
-      <c r="AH8" s="122"/>
-      <c r="AI8" s="122"/>
-      <c r="AJ8" s="122"/>
-      <c r="AK8" s="122"/>
-      <c r="AL8" s="122"/>
-      <c r="AM8" s="122"/>
-      <c r="AN8" s="122"/>
-      <c r="AO8" s="122"/>
-      <c r="AP8" s="122"/>
-      <c r="AQ8" s="122"/>
-      <c r="AR8" s="122"/>
-      <c r="AS8" s="123"/>
+      <c r="B8" s="121"/>
+      <c r="C8" s="131"/>
+      <c r="D8" s="131"/>
+      <c r="E8" s="131"/>
+      <c r="F8" s="131"/>
+      <c r="G8" s="131"/>
+      <c r="H8" s="131"/>
+      <c r="I8" s="131"/>
+      <c r="J8" s="131"/>
+      <c r="K8" s="131"/>
+      <c r="L8" s="131"/>
+      <c r="M8" s="131"/>
+      <c r="N8" s="131"/>
+      <c r="O8" s="131"/>
+      <c r="P8" s="131"/>
+      <c r="Q8" s="131"/>
+      <c r="R8" s="131"/>
+      <c r="S8" s="131"/>
+      <c r="T8" s="131"/>
+      <c r="U8" s="131"/>
+      <c r="V8" s="131"/>
+      <c r="W8" s="131"/>
+      <c r="X8" s="131"/>
+      <c r="Y8" s="131"/>
+      <c r="Z8" s="131"/>
+      <c r="AA8" s="131"/>
+      <c r="AB8" s="131"/>
+      <c r="AC8" s="131"/>
+      <c r="AD8" s="131"/>
+      <c r="AE8" s="131"/>
+      <c r="AF8" s="131"/>
+      <c r="AG8" s="131"/>
+      <c r="AH8" s="131"/>
+      <c r="AI8" s="131"/>
+      <c r="AJ8" s="131"/>
+      <c r="AK8" s="131"/>
+      <c r="AL8" s="131"/>
+      <c r="AM8" s="131"/>
+      <c r="AN8" s="131"/>
+      <c r="AO8" s="131"/>
+      <c r="AP8" s="131"/>
+      <c r="AQ8" s="131"/>
+      <c r="AR8" s="131"/>
+      <c r="AS8" s="132"/>
       <c r="AT8" s="33"/>
     </row>
     <row r="9" spans="1:46" ht="2.85" customHeight="1" x14ac:dyDescent="0.2">
@@ -2959,18 +2959,18 @@
     </row>
     <row r="11" spans="1:46" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="34"/>
-      <c r="B11" s="136"/>
-      <c r="C11" s="137"/>
-      <c r="D11" s="137"/>
-      <c r="E11" s="137"/>
-      <c r="F11" s="137"/>
-      <c r="G11" s="137"/>
-      <c r="H11" s="137"/>
-      <c r="I11" s="137"/>
-      <c r="J11" s="137"/>
-      <c r="K11" s="137"/>
-      <c r="L11" s="137"/>
-      <c r="M11" s="138"/>
+      <c r="B11" s="133"/>
+      <c r="C11" s="134"/>
+      <c r="D11" s="134"/>
+      <c r="E11" s="134"/>
+      <c r="F11" s="134"/>
+      <c r="G11" s="134"/>
+      <c r="H11" s="134"/>
+      <c r="I11" s="134"/>
+      <c r="J11" s="134"/>
+      <c r="K11" s="134"/>
+      <c r="L11" s="134"/>
+      <c r="M11" s="135"/>
       <c r="N11" s="13"/>
       <c r="Z11" s="35"/>
       <c r="AA11" s="36"/>
@@ -2980,18 +2980,18 @@
       <c r="AE11" s="36"/>
       <c r="AF11" s="36"/>
       <c r="AG11" s="37"/>
-      <c r="AH11" s="104"/>
-      <c r="AI11" s="105"/>
-      <c r="AJ11" s="105"/>
-      <c r="AK11" s="105"/>
-      <c r="AL11" s="105"/>
-      <c r="AM11" s="105"/>
-      <c r="AN11" s="105"/>
-      <c r="AO11" s="105"/>
-      <c r="AP11" s="105"/>
-      <c r="AQ11" s="105"/>
-      <c r="AR11" s="105"/>
-      <c r="AS11" s="106"/>
+      <c r="AH11" s="146"/>
+      <c r="AI11" s="147"/>
+      <c r="AJ11" s="147"/>
+      <c r="AK11" s="147"/>
+      <c r="AL11" s="147"/>
+      <c r="AM11" s="147"/>
+      <c r="AN11" s="147"/>
+      <c r="AO11" s="147"/>
+      <c r="AP11" s="147"/>
+      <c r="AQ11" s="147"/>
+      <c r="AR11" s="147"/>
+      <c r="AS11" s="148"/>
       <c r="AT11" s="33"/>
     </row>
     <row r="12" spans="1:46" ht="2.85" customHeight="1" x14ac:dyDescent="0.2">
@@ -3144,54 +3144,54 @@
     </row>
     <row r="15" spans="1:46" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="34"/>
-      <c r="B15" s="116" t="s">
+      <c r="B15" s="114" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="117"/>
-      <c r="D15" s="119"/>
-      <c r="E15" s="120"/>
-      <c r="F15" s="120"/>
-      <c r="G15" s="120"/>
-      <c r="H15" s="120"/>
-      <c r="I15" s="120"/>
-      <c r="J15" s="120"/>
-      <c r="K15" s="120"/>
-      <c r="L15" s="120"/>
-      <c r="M15" s="120"/>
-      <c r="N15" s="120"/>
-      <c r="O15" s="120"/>
-      <c r="P15" s="120"/>
-      <c r="Q15" s="120"/>
-      <c r="R15" s="120"/>
-      <c r="S15" s="120"/>
-      <c r="T15" s="120"/>
-      <c r="U15" s="120"/>
-      <c r="V15" s="120"/>
-      <c r="W15" s="120"/>
-      <c r="X15" s="120"/>
-      <c r="Y15" s="120"/>
-      <c r="Z15" s="120"/>
-      <c r="AA15" s="120"/>
-      <c r="AB15" s="120"/>
-      <c r="AC15" s="120"/>
-      <c r="AD15" s="120"/>
-      <c r="AE15" s="120"/>
-      <c r="AF15" s="120"/>
-      <c r="AG15" s="120"/>
-      <c r="AH15" s="121"/>
+      <c r="C15" s="125"/>
+      <c r="D15" s="121"/>
+      <c r="E15" s="122"/>
+      <c r="F15" s="122"/>
+      <c r="G15" s="122"/>
+      <c r="H15" s="122"/>
+      <c r="I15" s="122"/>
+      <c r="J15" s="122"/>
+      <c r="K15" s="122"/>
+      <c r="L15" s="122"/>
+      <c r="M15" s="122"/>
+      <c r="N15" s="122"/>
+      <c r="O15" s="122"/>
+      <c r="P15" s="122"/>
+      <c r="Q15" s="122"/>
+      <c r="R15" s="122"/>
+      <c r="S15" s="122"/>
+      <c r="T15" s="122"/>
+      <c r="U15" s="122"/>
+      <c r="V15" s="122"/>
+      <c r="W15" s="122"/>
+      <c r="X15" s="122"/>
+      <c r="Y15" s="122"/>
+      <c r="Z15" s="122"/>
+      <c r="AA15" s="122"/>
+      <c r="AB15" s="122"/>
+      <c r="AC15" s="122"/>
+      <c r="AD15" s="122"/>
+      <c r="AE15" s="122"/>
+      <c r="AF15" s="122"/>
+      <c r="AG15" s="122"/>
+      <c r="AH15" s="123"/>
       <c r="AI15" s="39"/>
       <c r="AJ15" s="36" t="s">
         <v>123</v>
       </c>
       <c r="AK15" s="39"/>
-      <c r="AL15" s="130"/>
-      <c r="AM15" s="131"/>
-      <c r="AN15" s="131"/>
-      <c r="AO15" s="131"/>
-      <c r="AP15" s="131"/>
-      <c r="AQ15" s="131"/>
-      <c r="AR15" s="131"/>
-      <c r="AS15" s="132"/>
+      <c r="AL15" s="161"/>
+      <c r="AM15" s="162"/>
+      <c r="AN15" s="162"/>
+      <c r="AO15" s="162"/>
+      <c r="AP15" s="162"/>
+      <c r="AQ15" s="162"/>
+      <c r="AR15" s="162"/>
+      <c r="AS15" s="163"/>
       <c r="AT15" s="33"/>
     </row>
     <row r="16" spans="1:46" ht="2.85" customHeight="1" x14ac:dyDescent="0.2">
@@ -3244,56 +3244,56 @@
     </row>
     <row r="17" spans="1:46" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="34"/>
-      <c r="B17" s="116" t="s">
+      <c r="B17" s="114" t="s">
         <v>11</v>
       </c>
-      <c r="C17" s="118"/>
-      <c r="D17" s="117"/>
+      <c r="C17" s="124"/>
+      <c r="D17" s="125"/>
       <c r="E17" s="164"/>
       <c r="F17" s="165"/>
       <c r="G17" s="165"/>
       <c r="H17" s="165"/>
       <c r="I17" s="165"/>
       <c r="J17" s="166"/>
-      <c r="K17" s="116" t="s">
+      <c r="K17" s="114" t="s">
         <v>12</v>
       </c>
-      <c r="L17" s="118"/>
-      <c r="M17" s="117"/>
-      <c r="N17" s="119"/>
-      <c r="O17" s="122"/>
-      <c r="P17" s="122"/>
-      <c r="Q17" s="122"/>
-      <c r="R17" s="122"/>
-      <c r="S17" s="122"/>
-      <c r="T17" s="122"/>
-      <c r="U17" s="122"/>
-      <c r="V17" s="122"/>
-      <c r="W17" s="122"/>
-      <c r="X17" s="122"/>
-      <c r="Y17" s="122"/>
-      <c r="Z17" s="122"/>
-      <c r="AA17" s="122"/>
-      <c r="AB17" s="122"/>
-      <c r="AC17" s="122"/>
-      <c r="AD17" s="122"/>
-      <c r="AE17" s="122"/>
-      <c r="AF17" s="122"/>
-      <c r="AG17" s="122"/>
-      <c r="AH17" s="123"/>
+      <c r="L17" s="124"/>
+      <c r="M17" s="125"/>
+      <c r="N17" s="121"/>
+      <c r="O17" s="131"/>
+      <c r="P17" s="131"/>
+      <c r="Q17" s="131"/>
+      <c r="R17" s="131"/>
+      <c r="S17" s="131"/>
+      <c r="T17" s="131"/>
+      <c r="U17" s="131"/>
+      <c r="V17" s="131"/>
+      <c r="W17" s="131"/>
+      <c r="X17" s="131"/>
+      <c r="Y17" s="131"/>
+      <c r="Z17" s="131"/>
+      <c r="AA17" s="131"/>
+      <c r="AB17" s="131"/>
+      <c r="AC17" s="131"/>
+      <c r="AD17" s="131"/>
+      <c r="AE17" s="131"/>
+      <c r="AF17" s="131"/>
+      <c r="AG17" s="131"/>
+      <c r="AH17" s="132"/>
       <c r="AI17" s="13"/>
       <c r="AJ17" s="14" t="s">
         <v>104</v>
       </c>
       <c r="AK17" s="14"/>
-      <c r="AL17" s="124"/>
-      <c r="AM17" s="125"/>
-      <c r="AN17" s="125"/>
-      <c r="AO17" s="125"/>
-      <c r="AP17" s="125"/>
-      <c r="AQ17" s="125"/>
-      <c r="AR17" s="125"/>
-      <c r="AS17" s="126"/>
+      <c r="AL17" s="126"/>
+      <c r="AM17" s="127"/>
+      <c r="AN17" s="127"/>
+      <c r="AO17" s="127"/>
+      <c r="AP17" s="127"/>
+      <c r="AQ17" s="127"/>
+      <c r="AR17" s="127"/>
+      <c r="AS17" s="128"/>
       <c r="AT17" s="33"/>
     </row>
     <row r="18" spans="1:46" ht="2.85" customHeight="1" x14ac:dyDescent="0.2">
@@ -3458,12 +3458,12 @@
     </row>
     <row r="21" spans="1:46" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="44"/>
-      <c r="B21" s="113"/>
-      <c r="C21" s="114"/>
-      <c r="D21" s="114"/>
-      <c r="E21" s="114"/>
-      <c r="F21" s="114"/>
-      <c r="G21" s="115"/>
+      <c r="B21" s="155"/>
+      <c r="C21" s="156"/>
+      <c r="D21" s="156"/>
+      <c r="E21" s="156"/>
+      <c r="F21" s="156"/>
+      <c r="G21" s="157"/>
       <c r="H21" s="13"/>
       <c r="I21" s="13"/>
       <c r="J21" s="13"/>
@@ -3475,10 +3475,10 @@
       <c r="P21" s="21"/>
       <c r="Q21" s="21"/>
       <c r="R21" s="21"/>
-      <c r="S21" s="127"/>
-      <c r="T21" s="128"/>
-      <c r="U21" s="128"/>
-      <c r="V21" s="129"/>
+      <c r="S21" s="158"/>
+      <c r="T21" s="159"/>
+      <c r="U21" s="159"/>
+      <c r="V21" s="160"/>
       <c r="W21" s="13"/>
       <c r="X21" s="13"/>
       <c r="Y21" s="13"/>
@@ -3487,21 +3487,21 @@
       <c r="AB21" s="21"/>
       <c r="AC21" s="21"/>
       <c r="AD21" s="21"/>
-      <c r="AE21" s="107"/>
-      <c r="AF21" s="108"/>
-      <c r="AG21" s="108"/>
-      <c r="AH21" s="108"/>
-      <c r="AI21" s="108"/>
-      <c r="AJ21" s="108"/>
-      <c r="AK21" s="108"/>
-      <c r="AL21" s="108"/>
-      <c r="AM21" s="108"/>
-      <c r="AN21" s="109"/>
+      <c r="AE21" s="149"/>
+      <c r="AF21" s="150"/>
+      <c r="AG21" s="150"/>
+      <c r="AH21" s="150"/>
+      <c r="AI21" s="150"/>
+      <c r="AJ21" s="150"/>
+      <c r="AK21" s="150"/>
+      <c r="AL21" s="150"/>
+      <c r="AM21" s="150"/>
+      <c r="AN21" s="151"/>
       <c r="AO21" s="36"/>
-      <c r="AP21" s="110"/>
-      <c r="AQ21" s="111"/>
-      <c r="AR21" s="111"/>
-      <c r="AS21" s="112"/>
+      <c r="AP21" s="152"/>
+      <c r="AQ21" s="153"/>
+      <c r="AR21" s="153"/>
+      <c r="AS21" s="154"/>
       <c r="AT21" s="33"/>
     </row>
     <row r="22" spans="1:46" ht="2.85" customHeight="1" x14ac:dyDescent="0.2">
@@ -3606,52 +3606,52 @@
     </row>
     <row r="24" spans="1:46" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="34"/>
-      <c r="B24" s="116" t="s">
+      <c r="B24" s="114" t="s">
         <v>10</v>
       </c>
-      <c r="C24" s="117"/>
-      <c r="D24" s="119"/>
-      <c r="E24" s="120"/>
-      <c r="F24" s="120"/>
-      <c r="G24" s="120"/>
-      <c r="H24" s="120"/>
-      <c r="I24" s="120"/>
-      <c r="J24" s="120"/>
-      <c r="K24" s="120"/>
-      <c r="L24" s="120"/>
-      <c r="M24" s="120"/>
-      <c r="N24" s="120"/>
-      <c r="O24" s="120"/>
-      <c r="P24" s="120"/>
-      <c r="Q24" s="120"/>
-      <c r="R24" s="120"/>
-      <c r="S24" s="120"/>
-      <c r="T24" s="120"/>
-      <c r="U24" s="120"/>
-      <c r="V24" s="120"/>
-      <c r="W24" s="120"/>
-      <c r="X24" s="120"/>
-      <c r="Y24" s="120"/>
-      <c r="Z24" s="120"/>
-      <c r="AA24" s="120"/>
-      <c r="AB24" s="120"/>
-      <c r="AC24" s="120"/>
-      <c r="AD24" s="120"/>
-      <c r="AE24" s="120"/>
-      <c r="AF24" s="120"/>
-      <c r="AG24" s="120"/>
-      <c r="AH24" s="120"/>
-      <c r="AI24" s="120"/>
-      <c r="AJ24" s="120"/>
-      <c r="AK24" s="120"/>
-      <c r="AL24" s="120"/>
-      <c r="AM24" s="120"/>
-      <c r="AN24" s="120"/>
-      <c r="AO24" s="120"/>
-      <c r="AP24" s="120"/>
-      <c r="AQ24" s="120"/>
-      <c r="AR24" s="120"/>
-      <c r="AS24" s="121"/>
+      <c r="C24" s="125"/>
+      <c r="D24" s="121"/>
+      <c r="E24" s="122"/>
+      <c r="F24" s="122"/>
+      <c r="G24" s="122"/>
+      <c r="H24" s="122"/>
+      <c r="I24" s="122"/>
+      <c r="J24" s="122"/>
+      <c r="K24" s="122"/>
+      <c r="L24" s="122"/>
+      <c r="M24" s="122"/>
+      <c r="N24" s="122"/>
+      <c r="O24" s="122"/>
+      <c r="P24" s="122"/>
+      <c r="Q24" s="122"/>
+      <c r="R24" s="122"/>
+      <c r="S24" s="122"/>
+      <c r="T24" s="122"/>
+      <c r="U24" s="122"/>
+      <c r="V24" s="122"/>
+      <c r="W24" s="122"/>
+      <c r="X24" s="122"/>
+      <c r="Y24" s="122"/>
+      <c r="Z24" s="122"/>
+      <c r="AA24" s="122"/>
+      <c r="AB24" s="122"/>
+      <c r="AC24" s="122"/>
+      <c r="AD24" s="122"/>
+      <c r="AE24" s="122"/>
+      <c r="AF24" s="122"/>
+      <c r="AG24" s="122"/>
+      <c r="AH24" s="122"/>
+      <c r="AI24" s="122"/>
+      <c r="AJ24" s="122"/>
+      <c r="AK24" s="122"/>
+      <c r="AL24" s="122"/>
+      <c r="AM24" s="122"/>
+      <c r="AN24" s="122"/>
+      <c r="AO24" s="122"/>
+      <c r="AP24" s="122"/>
+      <c r="AQ24" s="122"/>
+      <c r="AR24" s="122"/>
+      <c r="AS24" s="123"/>
       <c r="AT24" s="33"/>
     </row>
     <row r="25" spans="1:46" ht="2.85" customHeight="1" x14ac:dyDescent="0.2">
@@ -3704,56 +3704,56 @@
     </row>
     <row r="26" spans="1:46" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="34"/>
-      <c r="B26" s="116" t="s">
+      <c r="B26" s="114" t="s">
         <v>11</v>
       </c>
-      <c r="C26" s="118"/>
-      <c r="D26" s="117"/>
-      <c r="E26" s="119"/>
-      <c r="F26" s="120"/>
-      <c r="G26" s="120"/>
-      <c r="H26" s="120"/>
-      <c r="I26" s="120"/>
-      <c r="J26" s="121"/>
-      <c r="K26" s="116" t="s">
+      <c r="C26" s="124"/>
+      <c r="D26" s="125"/>
+      <c r="E26" s="164"/>
+      <c r="F26" s="165"/>
+      <c r="G26" s="165"/>
+      <c r="H26" s="165"/>
+      <c r="I26" s="165"/>
+      <c r="J26" s="166"/>
+      <c r="K26" s="114" t="s">
         <v>12</v>
       </c>
-      <c r="L26" s="118"/>
-      <c r="M26" s="117"/>
-      <c r="N26" s="119"/>
-      <c r="O26" s="120"/>
-      <c r="P26" s="120"/>
-      <c r="Q26" s="120"/>
-      <c r="R26" s="120"/>
-      <c r="S26" s="120"/>
-      <c r="T26" s="120"/>
-      <c r="U26" s="120"/>
-      <c r="V26" s="120"/>
-      <c r="W26" s="120"/>
-      <c r="X26" s="120"/>
-      <c r="Y26" s="120"/>
-      <c r="Z26" s="120"/>
-      <c r="AA26" s="120"/>
-      <c r="AB26" s="120"/>
-      <c r="AC26" s="120"/>
-      <c r="AD26" s="120"/>
-      <c r="AE26" s="120"/>
-      <c r="AF26" s="120"/>
-      <c r="AG26" s="120"/>
-      <c r="AH26" s="121"/>
+      <c r="L26" s="124"/>
+      <c r="M26" s="125"/>
+      <c r="N26" s="121"/>
+      <c r="O26" s="122"/>
+      <c r="P26" s="122"/>
+      <c r="Q26" s="122"/>
+      <c r="R26" s="122"/>
+      <c r="S26" s="122"/>
+      <c r="T26" s="122"/>
+      <c r="U26" s="122"/>
+      <c r="V26" s="122"/>
+      <c r="W26" s="122"/>
+      <c r="X26" s="122"/>
+      <c r="Y26" s="122"/>
+      <c r="Z26" s="122"/>
+      <c r="AA26" s="122"/>
+      <c r="AB26" s="122"/>
+      <c r="AC26" s="122"/>
+      <c r="AD26" s="122"/>
+      <c r="AE26" s="122"/>
+      <c r="AF26" s="122"/>
+      <c r="AG26" s="122"/>
+      <c r="AH26" s="123"/>
       <c r="AI26" s="13"/>
       <c r="AJ26" s="14" t="s">
         <v>104</v>
       </c>
       <c r="AK26" s="14"/>
-      <c r="AL26" s="124"/>
-      <c r="AM26" s="125"/>
-      <c r="AN26" s="125"/>
-      <c r="AO26" s="125"/>
-      <c r="AP26" s="125"/>
-      <c r="AQ26" s="125"/>
-      <c r="AR26" s="125"/>
-      <c r="AS26" s="126"/>
+      <c r="AL26" s="126"/>
+      <c r="AM26" s="127"/>
+      <c r="AN26" s="127"/>
+      <c r="AO26" s="127"/>
+      <c r="AP26" s="127"/>
+      <c r="AQ26" s="127"/>
+      <c r="AR26" s="127"/>
+      <c r="AS26" s="128"/>
       <c r="AT26" s="33"/>
     </row>
     <row r="27" spans="1:46" ht="2.85" customHeight="1" x14ac:dyDescent="0.2">
@@ -4394,46 +4394,46 @@
       </c>
       <c r="D40" s="13"/>
       <c r="E40" s="13"/>
-      <c r="F40" s="120"/>
-      <c r="G40" s="120"/>
-      <c r="H40" s="120"/>
-      <c r="I40" s="120"/>
-      <c r="J40" s="120"/>
-      <c r="K40" s="120"/>
-      <c r="L40" s="120"/>
-      <c r="M40" s="120"/>
-      <c r="N40" s="120"/>
-      <c r="O40" s="120"/>
-      <c r="P40" s="120"/>
-      <c r="Q40" s="120"/>
-      <c r="R40" s="120"/>
-      <c r="S40" s="120"/>
-      <c r="T40" s="120"/>
-      <c r="U40" s="120"/>
-      <c r="V40" s="120"/>
-      <c r="W40" s="120"/>
-      <c r="X40" s="120"/>
-      <c r="Y40" s="120"/>
-      <c r="Z40" s="120"/>
-      <c r="AA40" s="120"/>
-      <c r="AB40" s="120"/>
-      <c r="AC40" s="120"/>
-      <c r="AD40" s="120"/>
-      <c r="AE40" s="120"/>
-      <c r="AF40" s="120"/>
-      <c r="AG40" s="120"/>
-      <c r="AH40" s="120"/>
-      <c r="AI40" s="120"/>
-      <c r="AJ40" s="120"/>
-      <c r="AK40" s="120"/>
-      <c r="AL40" s="120"/>
-      <c r="AM40" s="120"/>
-      <c r="AN40" s="120"/>
-      <c r="AO40" s="120"/>
-      <c r="AP40" s="120"/>
-      <c r="AQ40" s="120"/>
-      <c r="AR40" s="120"/>
-      <c r="AS40" s="120"/>
+      <c r="F40" s="122"/>
+      <c r="G40" s="122"/>
+      <c r="H40" s="122"/>
+      <c r="I40" s="122"/>
+      <c r="J40" s="122"/>
+      <c r="K40" s="122"/>
+      <c r="L40" s="122"/>
+      <c r="M40" s="122"/>
+      <c r="N40" s="122"/>
+      <c r="O40" s="122"/>
+      <c r="P40" s="122"/>
+      <c r="Q40" s="122"/>
+      <c r="R40" s="122"/>
+      <c r="S40" s="122"/>
+      <c r="T40" s="122"/>
+      <c r="U40" s="122"/>
+      <c r="V40" s="122"/>
+      <c r="W40" s="122"/>
+      <c r="X40" s="122"/>
+      <c r="Y40" s="122"/>
+      <c r="Z40" s="122"/>
+      <c r="AA40" s="122"/>
+      <c r="AB40" s="122"/>
+      <c r="AC40" s="122"/>
+      <c r="AD40" s="122"/>
+      <c r="AE40" s="122"/>
+      <c r="AF40" s="122"/>
+      <c r="AG40" s="122"/>
+      <c r="AH40" s="122"/>
+      <c r="AI40" s="122"/>
+      <c r="AJ40" s="122"/>
+      <c r="AK40" s="122"/>
+      <c r="AL40" s="122"/>
+      <c r="AM40" s="122"/>
+      <c r="AN40" s="122"/>
+      <c r="AO40" s="122"/>
+      <c r="AP40" s="122"/>
+      <c r="AQ40" s="122"/>
+      <c r="AR40" s="122"/>
+      <c r="AS40" s="122"/>
       <c r="AT40" s="33"/>
     </row>
     <row r="41" spans="1:46" ht="2.85" customHeight="1" x14ac:dyDescent="0.2">
@@ -4485,53 +4485,53 @@
       <c r="AT41" s="33"/>
     </row>
     <row r="42" spans="1:46" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="148" t="s">
+      <c r="A42" s="129" t="s">
         <v>39</v>
       </c>
-      <c r="B42" s="149"/>
-      <c r="C42" s="149"/>
-      <c r="D42" s="149"/>
-      <c r="E42" s="149"/>
-      <c r="F42" s="120"/>
-      <c r="G42" s="120"/>
-      <c r="H42" s="120"/>
-      <c r="I42" s="120"/>
-      <c r="J42" s="120"/>
-      <c r="K42" s="120"/>
-      <c r="L42" s="120"/>
-      <c r="M42" s="120"/>
-      <c r="N42" s="120"/>
-      <c r="O42" s="120"/>
-      <c r="P42" s="120"/>
-      <c r="Q42" s="120"/>
-      <c r="R42" s="120"/>
-      <c r="S42" s="120"/>
-      <c r="T42" s="120"/>
-      <c r="U42" s="120"/>
-      <c r="V42" s="120"/>
-      <c r="W42" s="120"/>
-      <c r="X42" s="120"/>
-      <c r="Y42" s="120"/>
-      <c r="Z42" s="120"/>
-      <c r="AA42" s="120"/>
-      <c r="AB42" s="120"/>
-      <c r="AC42" s="120"/>
-      <c r="AD42" s="120"/>
-      <c r="AE42" s="120"/>
-      <c r="AF42" s="120"/>
-      <c r="AG42" s="120"/>
-      <c r="AH42" s="120"/>
-      <c r="AI42" s="120"/>
-      <c r="AJ42" s="120"/>
-      <c r="AK42" s="120"/>
-      <c r="AL42" s="120"/>
-      <c r="AM42" s="120"/>
-      <c r="AN42" s="120"/>
-      <c r="AO42" s="120"/>
-      <c r="AP42" s="120"/>
-      <c r="AQ42" s="120"/>
-      <c r="AR42" s="120"/>
-      <c r="AS42" s="120"/>
+      <c r="B42" s="130"/>
+      <c r="C42" s="130"/>
+      <c r="D42" s="130"/>
+      <c r="E42" s="130"/>
+      <c r="F42" s="122"/>
+      <c r="G42" s="122"/>
+      <c r="H42" s="122"/>
+      <c r="I42" s="122"/>
+      <c r="J42" s="122"/>
+      <c r="K42" s="122"/>
+      <c r="L42" s="122"/>
+      <c r="M42" s="122"/>
+      <c r="N42" s="122"/>
+      <c r="O42" s="122"/>
+      <c r="P42" s="122"/>
+      <c r="Q42" s="122"/>
+      <c r="R42" s="122"/>
+      <c r="S42" s="122"/>
+      <c r="T42" s="122"/>
+      <c r="U42" s="122"/>
+      <c r="V42" s="122"/>
+      <c r="W42" s="122"/>
+      <c r="X42" s="122"/>
+      <c r="Y42" s="122"/>
+      <c r="Z42" s="122"/>
+      <c r="AA42" s="122"/>
+      <c r="AB42" s="122"/>
+      <c r="AC42" s="122"/>
+      <c r="AD42" s="122"/>
+      <c r="AE42" s="122"/>
+      <c r="AF42" s="122"/>
+      <c r="AG42" s="122"/>
+      <c r="AH42" s="122"/>
+      <c r="AI42" s="122"/>
+      <c r="AJ42" s="122"/>
+      <c r="AK42" s="122"/>
+      <c r="AL42" s="122"/>
+      <c r="AM42" s="122"/>
+      <c r="AN42" s="122"/>
+      <c r="AO42" s="122"/>
+      <c r="AP42" s="122"/>
+      <c r="AQ42" s="122"/>
+      <c r="AR42" s="122"/>
+      <c r="AS42" s="122"/>
       <c r="AT42" s="33"/>
     </row>
     <row r="43" spans="1:46" ht="2.85" customHeight="1" x14ac:dyDescent="0.2">
@@ -4584,50 +4584,50 @@
     </row>
     <row r="44" spans="1:46" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="34"/>
-      <c r="B44" s="120"/>
-      <c r="C44" s="120"/>
-      <c r="D44" s="120"/>
-      <c r="E44" s="120"/>
-      <c r="F44" s="120"/>
-      <c r="G44" s="120"/>
-      <c r="H44" s="120"/>
-      <c r="I44" s="120"/>
-      <c r="J44" s="120"/>
-      <c r="K44" s="120"/>
-      <c r="L44" s="120"/>
-      <c r="M44" s="120"/>
-      <c r="N44" s="120"/>
-      <c r="O44" s="120"/>
-      <c r="P44" s="120"/>
-      <c r="Q44" s="120"/>
-      <c r="R44" s="120"/>
-      <c r="S44" s="120"/>
-      <c r="T44" s="120"/>
-      <c r="U44" s="120"/>
-      <c r="V44" s="120"/>
-      <c r="W44" s="120"/>
-      <c r="X44" s="120"/>
-      <c r="Y44" s="120"/>
-      <c r="Z44" s="120"/>
-      <c r="AA44" s="120"/>
-      <c r="AB44" s="120"/>
-      <c r="AC44" s="120"/>
-      <c r="AD44" s="120"/>
-      <c r="AE44" s="120"/>
-      <c r="AF44" s="120"/>
-      <c r="AG44" s="120"/>
-      <c r="AH44" s="120"/>
-      <c r="AI44" s="120"/>
-      <c r="AJ44" s="120"/>
-      <c r="AK44" s="120"/>
-      <c r="AL44" s="120"/>
-      <c r="AM44" s="120"/>
-      <c r="AN44" s="120"/>
-      <c r="AO44" s="120"/>
-      <c r="AP44" s="120"/>
-      <c r="AQ44" s="120"/>
-      <c r="AR44" s="120"/>
-      <c r="AS44" s="120"/>
+      <c r="B44" s="122"/>
+      <c r="C44" s="122"/>
+      <c r="D44" s="122"/>
+      <c r="E44" s="122"/>
+      <c r="F44" s="122"/>
+      <c r="G44" s="122"/>
+      <c r="H44" s="122"/>
+      <c r="I44" s="122"/>
+      <c r="J44" s="122"/>
+      <c r="K44" s="122"/>
+      <c r="L44" s="122"/>
+      <c r="M44" s="122"/>
+      <c r="N44" s="122"/>
+      <c r="O44" s="122"/>
+      <c r="P44" s="122"/>
+      <c r="Q44" s="122"/>
+      <c r="R44" s="122"/>
+      <c r="S44" s="122"/>
+      <c r="T44" s="122"/>
+      <c r="U44" s="122"/>
+      <c r="V44" s="122"/>
+      <c r="W44" s="122"/>
+      <c r="X44" s="122"/>
+      <c r="Y44" s="122"/>
+      <c r="Z44" s="122"/>
+      <c r="AA44" s="122"/>
+      <c r="AB44" s="122"/>
+      <c r="AC44" s="122"/>
+      <c r="AD44" s="122"/>
+      <c r="AE44" s="122"/>
+      <c r="AF44" s="122"/>
+      <c r="AG44" s="122"/>
+      <c r="AH44" s="122"/>
+      <c r="AI44" s="122"/>
+      <c r="AJ44" s="122"/>
+      <c r="AK44" s="122"/>
+      <c r="AL44" s="122"/>
+      <c r="AM44" s="122"/>
+      <c r="AN44" s="122"/>
+      <c r="AO44" s="122"/>
+      <c r="AP44" s="122"/>
+      <c r="AQ44" s="122"/>
+      <c r="AR44" s="122"/>
+      <c r="AS44" s="122"/>
       <c r="AT44" s="33"/>
     </row>
     <row r="45" spans="1:46" ht="2.85" customHeight="1" x14ac:dyDescent="0.2">
@@ -4699,38 +4699,38 @@
       <c r="N46" s="53"/>
       <c r="O46" s="52"/>
       <c r="P46" s="52"/>
-      <c r="Q46" s="145" t="str">
+      <c r="Q46" s="118" t="str">
         <f>IFERROR(VLOOKUP(B48,Dados!$A$16:$B$21,2,0),"")</f>
         <v/>
       </c>
-      <c r="R46" s="145"/>
-      <c r="S46" s="145"/>
-      <c r="T46" s="145"/>
-      <c r="U46" s="145"/>
-      <c r="V46" s="145"/>
-      <c r="W46" s="145"/>
-      <c r="X46" s="145"/>
-      <c r="Y46" s="145"/>
-      <c r="Z46" s="145"/>
-      <c r="AA46" s="145"/>
-      <c r="AB46" s="145"/>
-      <c r="AC46" s="145"/>
-      <c r="AD46" s="145"/>
-      <c r="AE46" s="145"/>
-      <c r="AF46" s="145"/>
-      <c r="AG46" s="145"/>
-      <c r="AH46" s="145"/>
-      <c r="AI46" s="145"/>
-      <c r="AJ46" s="145"/>
-      <c r="AK46" s="145"/>
-      <c r="AL46" s="145"/>
-      <c r="AM46" s="145"/>
-      <c r="AN46" s="145"/>
-      <c r="AO46" s="145"/>
-      <c r="AP46" s="145"/>
-      <c r="AQ46" s="145"/>
-      <c r="AR46" s="145"/>
-      <c r="AS46" s="145"/>
+      <c r="R46" s="118"/>
+      <c r="S46" s="118"/>
+      <c r="T46" s="118"/>
+      <c r="U46" s="118"/>
+      <c r="V46" s="118"/>
+      <c r="W46" s="118"/>
+      <c r="X46" s="118"/>
+      <c r="Y46" s="118"/>
+      <c r="Z46" s="118"/>
+      <c r="AA46" s="118"/>
+      <c r="AB46" s="118"/>
+      <c r="AC46" s="118"/>
+      <c r="AD46" s="118"/>
+      <c r="AE46" s="118"/>
+      <c r="AF46" s="118"/>
+      <c r="AG46" s="118"/>
+      <c r="AH46" s="118"/>
+      <c r="AI46" s="118"/>
+      <c r="AJ46" s="118"/>
+      <c r="AK46" s="118"/>
+      <c r="AL46" s="118"/>
+      <c r="AM46" s="118"/>
+      <c r="AN46" s="118"/>
+      <c r="AO46" s="118"/>
+      <c r="AP46" s="118"/>
+      <c r="AQ46" s="118"/>
+      <c r="AR46" s="118"/>
+      <c r="AS46" s="118"/>
       <c r="AT46" s="31"/>
     </row>
     <row r="47" spans="1:46" ht="2.85" customHeight="1" x14ac:dyDescent="0.2">
@@ -4750,83 +4750,83 @@
       <c r="N47" s="13"/>
       <c r="O47" s="13"/>
       <c r="P47" s="13"/>
-      <c r="Q47" s="146"/>
-      <c r="R47" s="146"/>
-      <c r="S47" s="146"/>
-      <c r="T47" s="146"/>
-      <c r="U47" s="146"/>
-      <c r="V47" s="146"/>
-      <c r="W47" s="146"/>
-      <c r="X47" s="146"/>
-      <c r="Y47" s="146"/>
-      <c r="Z47" s="146"/>
-      <c r="AA47" s="146"/>
-      <c r="AB47" s="146"/>
-      <c r="AC47" s="146"/>
-      <c r="AD47" s="146"/>
-      <c r="AE47" s="146"/>
-      <c r="AF47" s="146"/>
-      <c r="AG47" s="146"/>
-      <c r="AH47" s="146"/>
-      <c r="AI47" s="146"/>
-      <c r="AJ47" s="146"/>
-      <c r="AK47" s="146"/>
-      <c r="AL47" s="146"/>
-      <c r="AM47" s="146"/>
-      <c r="AN47" s="146"/>
-      <c r="AO47" s="146"/>
-      <c r="AP47" s="146"/>
-      <c r="AQ47" s="146"/>
-      <c r="AR47" s="146"/>
-      <c r="AS47" s="146"/>
+      <c r="Q47" s="119"/>
+      <c r="R47" s="119"/>
+      <c r="S47" s="119"/>
+      <c r="T47" s="119"/>
+      <c r="U47" s="119"/>
+      <c r="V47" s="119"/>
+      <c r="W47" s="119"/>
+      <c r="X47" s="119"/>
+      <c r="Y47" s="119"/>
+      <c r="Z47" s="119"/>
+      <c r="AA47" s="119"/>
+      <c r="AB47" s="119"/>
+      <c r="AC47" s="119"/>
+      <c r="AD47" s="119"/>
+      <c r="AE47" s="119"/>
+      <c r="AF47" s="119"/>
+      <c r="AG47" s="119"/>
+      <c r="AH47" s="119"/>
+      <c r="AI47" s="119"/>
+      <c r="AJ47" s="119"/>
+      <c r="AK47" s="119"/>
+      <c r="AL47" s="119"/>
+      <c r="AM47" s="119"/>
+      <c r="AN47" s="119"/>
+      <c r="AO47" s="119"/>
+      <c r="AP47" s="119"/>
+      <c r="AQ47" s="119"/>
+      <c r="AR47" s="119"/>
+      <c r="AS47" s="119"/>
       <c r="AT47" s="33"/>
     </row>
     <row r="48" spans="1:46" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="44"/>
-      <c r="B48" s="147"/>
-      <c r="C48" s="147"/>
-      <c r="D48" s="147"/>
-      <c r="E48" s="147"/>
-      <c r="F48" s="147"/>
-      <c r="G48" s="147"/>
-      <c r="H48" s="147"/>
-      <c r="I48" s="147"/>
-      <c r="J48" s="147"/>
-      <c r="K48" s="147"/>
-      <c r="L48" s="147"/>
-      <c r="M48" s="147"/>
-      <c r="N48" s="147"/>
-      <c r="O48" s="147"/>
+      <c r="B48" s="120"/>
+      <c r="C48" s="120"/>
+      <c r="D48" s="120"/>
+      <c r="E48" s="120"/>
+      <c r="F48" s="120"/>
+      <c r="G48" s="120"/>
+      <c r="H48" s="120"/>
+      <c r="I48" s="120"/>
+      <c r="J48" s="120"/>
+      <c r="K48" s="120"/>
+      <c r="L48" s="120"/>
+      <c r="M48" s="120"/>
+      <c r="N48" s="120"/>
+      <c r="O48" s="120"/>
       <c r="P48" s="13"/>
-      <c r="Q48" s="146"/>
-      <c r="R48" s="146"/>
-      <c r="S48" s="146"/>
-      <c r="T48" s="146"/>
-      <c r="U48" s="146"/>
-      <c r="V48" s="146"/>
-      <c r="W48" s="146"/>
-      <c r="X48" s="146"/>
-      <c r="Y48" s="146"/>
-      <c r="Z48" s="146"/>
-      <c r="AA48" s="146"/>
-      <c r="AB48" s="146"/>
-      <c r="AC48" s="146"/>
-      <c r="AD48" s="146"/>
-      <c r="AE48" s="146"/>
-      <c r="AF48" s="146"/>
-      <c r="AG48" s="146"/>
-      <c r="AH48" s="146"/>
-      <c r="AI48" s="146"/>
-      <c r="AJ48" s="146"/>
-      <c r="AK48" s="146"/>
-      <c r="AL48" s="146"/>
-      <c r="AM48" s="146"/>
-      <c r="AN48" s="146"/>
-      <c r="AO48" s="146"/>
-      <c r="AP48" s="146"/>
-      <c r="AQ48" s="146"/>
-      <c r="AR48" s="146"/>
-      <c r="AS48" s="146"/>
+      <c r="Q48" s="119"/>
+      <c r="R48" s="119"/>
+      <c r="S48" s="119"/>
+      <c r="T48" s="119"/>
+      <c r="U48" s="119"/>
+      <c r="V48" s="119"/>
+      <c r="W48" s="119"/>
+      <c r="X48" s="119"/>
+      <c r="Y48" s="119"/>
+      <c r="Z48" s="119"/>
+      <c r="AA48" s="119"/>
+      <c r="AB48" s="119"/>
+      <c r="AC48" s="119"/>
+      <c r="AD48" s="119"/>
+      <c r="AE48" s="119"/>
+      <c r="AF48" s="119"/>
+      <c r="AG48" s="119"/>
+      <c r="AH48" s="119"/>
+      <c r="AI48" s="119"/>
+      <c r="AJ48" s="119"/>
+      <c r="AK48" s="119"/>
+      <c r="AL48" s="119"/>
+      <c r="AM48" s="119"/>
+      <c r="AN48" s="119"/>
+      <c r="AO48" s="119"/>
+      <c r="AP48" s="119"/>
+      <c r="AQ48" s="119"/>
+      <c r="AR48" s="119"/>
+      <c r="AS48" s="119"/>
       <c r="AT48" s="33"/>
     </row>
     <row r="49" spans="1:46" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -4846,35 +4846,35 @@
       <c r="N49" s="13"/>
       <c r="O49" s="13"/>
       <c r="P49" s="13"/>
-      <c r="Q49" s="146"/>
-      <c r="R49" s="146"/>
-      <c r="S49" s="146"/>
-      <c r="T49" s="146"/>
-      <c r="U49" s="146"/>
-      <c r="V49" s="146"/>
-      <c r="W49" s="146"/>
-      <c r="X49" s="146"/>
-      <c r="Y49" s="146"/>
-      <c r="Z49" s="146"/>
-      <c r="AA49" s="146"/>
-      <c r="AB49" s="146"/>
-      <c r="AC49" s="146"/>
-      <c r="AD49" s="146"/>
-      <c r="AE49" s="146"/>
-      <c r="AF49" s="146"/>
-      <c r="AG49" s="146"/>
-      <c r="AH49" s="146"/>
-      <c r="AI49" s="146"/>
-      <c r="AJ49" s="146"/>
-      <c r="AK49" s="146"/>
-      <c r="AL49" s="146"/>
-      <c r="AM49" s="146"/>
-      <c r="AN49" s="146"/>
-      <c r="AO49" s="146"/>
-      <c r="AP49" s="146"/>
-      <c r="AQ49" s="146"/>
-      <c r="AR49" s="146"/>
-      <c r="AS49" s="146"/>
+      <c r="Q49" s="119"/>
+      <c r="R49" s="119"/>
+      <c r="S49" s="119"/>
+      <c r="T49" s="119"/>
+      <c r="U49" s="119"/>
+      <c r="V49" s="119"/>
+      <c r="W49" s="119"/>
+      <c r="X49" s="119"/>
+      <c r="Y49" s="119"/>
+      <c r="Z49" s="119"/>
+      <c r="AA49" s="119"/>
+      <c r="AB49" s="119"/>
+      <c r="AC49" s="119"/>
+      <c r="AD49" s="119"/>
+      <c r="AE49" s="119"/>
+      <c r="AF49" s="119"/>
+      <c r="AG49" s="119"/>
+      <c r="AH49" s="119"/>
+      <c r="AI49" s="119"/>
+      <c r="AJ49" s="119"/>
+      <c r="AK49" s="119"/>
+      <c r="AL49" s="119"/>
+      <c r="AM49" s="119"/>
+      <c r="AN49" s="119"/>
+      <c r="AO49" s="119"/>
+      <c r="AP49" s="119"/>
+      <c r="AQ49" s="119"/>
+      <c r="AR49" s="119"/>
+      <c r="AS49" s="119"/>
       <c r="AT49" s="33"/>
     </row>
     <row r="50" spans="1:46" ht="2.85" customHeight="1" x14ac:dyDescent="0.2">
@@ -5148,7 +5148,7 @@
       <c r="T55" s="102"/>
       <c r="U55" s="102"/>
       <c r="V55" s="102"/>
-      <c r="W55" s="103"/>
+      <c r="W55" s="145"/>
       <c r="X55" s="13"/>
       <c r="Y55" s="1"/>
       <c r="Z55" s="102" t="s">
@@ -5197,7 +5197,7 @@
       <c r="T56" s="102"/>
       <c r="U56" s="102"/>
       <c r="V56" s="102"/>
-      <c r="W56" s="103"/>
+      <c r="W56" s="145"/>
       <c r="X56" s="13"/>
       <c r="Y56" s="13"/>
       <c r="Z56" s="102"/>
@@ -5244,7 +5244,7 @@
       <c r="T57" s="102"/>
       <c r="U57" s="102"/>
       <c r="V57" s="102"/>
-      <c r="W57" s="103"/>
+      <c r="W57" s="145"/>
       <c r="X57" s="14"/>
       <c r="Y57" s="1"/>
       <c r="Z57" s="102" t="s">
@@ -5342,7 +5342,7 @@
       <c r="T59" s="102"/>
       <c r="U59" s="102"/>
       <c r="V59" s="102"/>
-      <c r="W59" s="103"/>
+      <c r="W59" s="145"/>
       <c r="X59" s="13"/>
       <c r="Y59" s="1"/>
       <c r="Z59" s="102" t="s">
@@ -5392,7 +5392,7 @@
       <c r="T60" s="102"/>
       <c r="U60" s="102"/>
       <c r="V60" s="102"/>
-      <c r="W60" s="103"/>
+      <c r="W60" s="145"/>
       <c r="X60" s="14"/>
       <c r="Y60" s="13"/>
       <c r="Z60" s="102"/>
@@ -6256,14 +6256,14 @@
     </row>
     <row r="78" spans="1:46" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="34"/>
-      <c r="B78" s="116" t="str">
+      <c r="B78" s="114" t="str">
         <f>IFERROR(VLOOKUP($B$3,Dados!K1:M9,2,),"")</f>
         <v/>
       </c>
-      <c r="C78" s="157"/>
-      <c r="D78" s="157"/>
-      <c r="E78" s="157"/>
-      <c r="F78" s="161"/>
+      <c r="C78" s="110"/>
+      <c r="D78" s="110"/>
+      <c r="E78" s="110"/>
+      <c r="F78" s="115"/>
       <c r="G78" s="13"/>
       <c r="H78" s="13"/>
       <c r="I78" s="13"/>
@@ -6277,31 +6277,31 @@
       <c r="Q78" s="13"/>
       <c r="R78" s="13"/>
       <c r="S78" s="13"/>
-      <c r="T78" s="162" t="str">
+      <c r="T78" s="116" t="str">
         <f>IFERROR(VLOOKUP($B$3,Dados!K1:M9,3,),"")</f>
         <v/>
       </c>
-      <c r="U78" s="162"/>
-      <c r="V78" s="162"/>
-      <c r="W78" s="162"/>
-      <c r="X78" s="162"/>
-      <c r="Y78" s="162"/>
-      <c r="Z78" s="162"/>
-      <c r="AA78" s="162"/>
-      <c r="AB78" s="162"/>
-      <c r="AC78" s="162"/>
-      <c r="AD78" s="162"/>
-      <c r="AE78" s="162"/>
-      <c r="AF78" s="162"/>
-      <c r="AG78" s="162"/>
-      <c r="AH78" s="162"/>
-      <c r="AI78" s="162"/>
-      <c r="AJ78" s="162"/>
-      <c r="AK78" s="162"/>
-      <c r="AL78" s="162"/>
-      <c r="AM78" s="162"/>
-      <c r="AN78" s="162"/>
-      <c r="AO78" s="162"/>
+      <c r="U78" s="116"/>
+      <c r="V78" s="116"/>
+      <c r="W78" s="116"/>
+      <c r="X78" s="116"/>
+      <c r="Y78" s="116"/>
+      <c r="Z78" s="116"/>
+      <c r="AA78" s="116"/>
+      <c r="AB78" s="116"/>
+      <c r="AC78" s="116"/>
+      <c r="AD78" s="116"/>
+      <c r="AE78" s="116"/>
+      <c r="AF78" s="116"/>
+      <c r="AG78" s="116"/>
+      <c r="AH78" s="116"/>
+      <c r="AI78" s="116"/>
+      <c r="AJ78" s="116"/>
+      <c r="AK78" s="116"/>
+      <c r="AL78" s="116"/>
+      <c r="AM78" s="116"/>
+      <c r="AN78" s="116"/>
+      <c r="AO78" s="116"/>
       <c r="AP78" s="13"/>
       <c r="AQ78" s="13"/>
       <c r="AR78" s="13"/>
@@ -6310,13 +6310,13 @@
     </row>
     <row r="79" spans="1:46" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="47"/>
-      <c r="B79" s="156" t="s">
+      <c r="B79" s="109" t="s">
         <v>64</v>
       </c>
-      <c r="C79" s="156"/>
-      <c r="D79" s="156"/>
-      <c r="E79" s="156"/>
-      <c r="F79" s="156"/>
+      <c r="C79" s="109"/>
+      <c r="D79" s="109"/>
+      <c r="E79" s="109"/>
+      <c r="F79" s="109"/>
       <c r="G79" s="48"/>
       <c r="H79" s="48"/>
       <c r="I79" s="48"/>
@@ -6330,30 +6330,30 @@
       <c r="Q79" s="48"/>
       <c r="R79" s="48"/>
       <c r="S79" s="48"/>
-      <c r="T79" s="157" t="s">
+      <c r="T79" s="110" t="s">
         <v>65</v>
       </c>
-      <c r="U79" s="157"/>
-      <c r="V79" s="157"/>
-      <c r="W79" s="157"/>
-      <c r="X79" s="157"/>
-      <c r="Y79" s="157"/>
-      <c r="Z79" s="157"/>
-      <c r="AA79" s="157"/>
-      <c r="AB79" s="157"/>
-      <c r="AC79" s="157"/>
-      <c r="AD79" s="157"/>
-      <c r="AE79" s="157"/>
-      <c r="AF79" s="157"/>
-      <c r="AG79" s="157"/>
-      <c r="AH79" s="157"/>
-      <c r="AI79" s="157"/>
-      <c r="AJ79" s="157"/>
-      <c r="AK79" s="157"/>
-      <c r="AL79" s="157"/>
-      <c r="AM79" s="157"/>
-      <c r="AN79" s="157"/>
-      <c r="AO79" s="157"/>
+      <c r="U79" s="110"/>
+      <c r="V79" s="110"/>
+      <c r="W79" s="110"/>
+      <c r="X79" s="110"/>
+      <c r="Y79" s="110"/>
+      <c r="Z79" s="110"/>
+      <c r="AA79" s="110"/>
+      <c r="AB79" s="110"/>
+      <c r="AC79" s="110"/>
+      <c r="AD79" s="110"/>
+      <c r="AE79" s="110"/>
+      <c r="AF79" s="110"/>
+      <c r="AG79" s="110"/>
+      <c r="AH79" s="110"/>
+      <c r="AI79" s="110"/>
+      <c r="AJ79" s="110"/>
+      <c r="AK79" s="110"/>
+      <c r="AL79" s="110"/>
+      <c r="AM79" s="110"/>
+      <c r="AN79" s="110"/>
+      <c r="AO79" s="110"/>
       <c r="AP79" s="48"/>
       <c r="AQ79" s="48"/>
       <c r="AR79" s="48"/>
@@ -6461,102 +6461,102 @@
       <c r="AT81" s="31"/>
     </row>
     <row r="82" spans="1:46" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A82" s="158" t="s">
+      <c r="A82" s="111" t="s">
         <v>68</v>
       </c>
-      <c r="B82" s="159"/>
-      <c r="C82" s="159"/>
-      <c r="D82" s="159"/>
-      <c r="E82" s="159"/>
-      <c r="F82" s="159"/>
-      <c r="G82" s="159"/>
-      <c r="H82" s="159"/>
-      <c r="I82" s="159"/>
-      <c r="J82" s="159"/>
-      <c r="K82" s="159"/>
-      <c r="L82" s="159"/>
-      <c r="M82" s="159"/>
-      <c r="N82" s="159"/>
-      <c r="O82" s="159"/>
-      <c r="P82" s="159"/>
-      <c r="Q82" s="159"/>
-      <c r="R82" s="159"/>
-      <c r="S82" s="159"/>
-      <c r="T82" s="159"/>
-      <c r="U82" s="159"/>
-      <c r="V82" s="159"/>
-      <c r="W82" s="159"/>
-      <c r="X82" s="159"/>
-      <c r="Y82" s="159"/>
-      <c r="Z82" s="159"/>
-      <c r="AA82" s="159"/>
-      <c r="AB82" s="159"/>
-      <c r="AC82" s="159"/>
-      <c r="AD82" s="159"/>
-      <c r="AE82" s="159"/>
-      <c r="AF82" s="159"/>
-      <c r="AG82" s="159"/>
-      <c r="AH82" s="159"/>
-      <c r="AI82" s="159"/>
-      <c r="AJ82" s="159"/>
-      <c r="AK82" s="159"/>
-      <c r="AL82" s="159"/>
-      <c r="AM82" s="159"/>
-      <c r="AN82" s="159"/>
-      <c r="AO82" s="159"/>
-      <c r="AP82" s="159"/>
-      <c r="AQ82" s="159"/>
-      <c r="AR82" s="159"/>
-      <c r="AS82" s="159"/>
-      <c r="AT82" s="160"/>
+      <c r="B82" s="112"/>
+      <c r="C82" s="112"/>
+      <c r="D82" s="112"/>
+      <c r="E82" s="112"/>
+      <c r="F82" s="112"/>
+      <c r="G82" s="112"/>
+      <c r="H82" s="112"/>
+      <c r="I82" s="112"/>
+      <c r="J82" s="112"/>
+      <c r="K82" s="112"/>
+      <c r="L82" s="112"/>
+      <c r="M82" s="112"/>
+      <c r="N82" s="112"/>
+      <c r="O82" s="112"/>
+      <c r="P82" s="112"/>
+      <c r="Q82" s="112"/>
+      <c r="R82" s="112"/>
+      <c r="S82" s="112"/>
+      <c r="T82" s="112"/>
+      <c r="U82" s="112"/>
+      <c r="V82" s="112"/>
+      <c r="W82" s="112"/>
+      <c r="X82" s="112"/>
+      <c r="Y82" s="112"/>
+      <c r="Z82" s="112"/>
+      <c r="AA82" s="112"/>
+      <c r="AB82" s="112"/>
+      <c r="AC82" s="112"/>
+      <c r="AD82" s="112"/>
+      <c r="AE82" s="112"/>
+      <c r="AF82" s="112"/>
+      <c r="AG82" s="112"/>
+      <c r="AH82" s="112"/>
+      <c r="AI82" s="112"/>
+      <c r="AJ82" s="112"/>
+      <c r="AK82" s="112"/>
+      <c r="AL82" s="112"/>
+      <c r="AM82" s="112"/>
+      <c r="AN82" s="112"/>
+      <c r="AO82" s="112"/>
+      <c r="AP82" s="112"/>
+      <c r="AQ82" s="112"/>
+      <c r="AR82" s="112"/>
+      <c r="AS82" s="112"/>
+      <c r="AT82" s="113"/>
     </row>
     <row r="83" spans="1:46" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A83" s="158"/>
-      <c r="B83" s="159"/>
-      <c r="C83" s="159"/>
-      <c r="D83" s="159"/>
-      <c r="E83" s="159"/>
-      <c r="F83" s="159"/>
-      <c r="G83" s="159"/>
-      <c r="H83" s="159"/>
-      <c r="I83" s="159"/>
-      <c r="J83" s="159"/>
-      <c r="K83" s="159"/>
-      <c r="L83" s="159"/>
-      <c r="M83" s="159"/>
-      <c r="N83" s="159"/>
-      <c r="O83" s="159"/>
-      <c r="P83" s="159"/>
-      <c r="Q83" s="159"/>
-      <c r="R83" s="159"/>
-      <c r="S83" s="159"/>
-      <c r="T83" s="159"/>
-      <c r="U83" s="159"/>
-      <c r="V83" s="159"/>
-      <c r="W83" s="159"/>
-      <c r="X83" s="159"/>
-      <c r="Y83" s="159"/>
-      <c r="Z83" s="159"/>
-      <c r="AA83" s="159"/>
-      <c r="AB83" s="159"/>
-      <c r="AC83" s="159"/>
-      <c r="AD83" s="159"/>
-      <c r="AE83" s="159"/>
-      <c r="AF83" s="159"/>
-      <c r="AG83" s="159"/>
-      <c r="AH83" s="159"/>
-      <c r="AI83" s="159"/>
-      <c r="AJ83" s="159"/>
-      <c r="AK83" s="159"/>
-      <c r="AL83" s="159"/>
-      <c r="AM83" s="159"/>
-      <c r="AN83" s="159"/>
-      <c r="AO83" s="159"/>
-      <c r="AP83" s="159"/>
-      <c r="AQ83" s="159"/>
-      <c r="AR83" s="159"/>
-      <c r="AS83" s="159"/>
-      <c r="AT83" s="160"/>
+      <c r="A83" s="111"/>
+      <c r="B83" s="112"/>
+      <c r="C83" s="112"/>
+      <c r="D83" s="112"/>
+      <c r="E83" s="112"/>
+      <c r="F83" s="112"/>
+      <c r="G83" s="112"/>
+      <c r="H83" s="112"/>
+      <c r="I83" s="112"/>
+      <c r="J83" s="112"/>
+      <c r="K83" s="112"/>
+      <c r="L83" s="112"/>
+      <c r="M83" s="112"/>
+      <c r="N83" s="112"/>
+      <c r="O83" s="112"/>
+      <c r="P83" s="112"/>
+      <c r="Q83" s="112"/>
+      <c r="R83" s="112"/>
+      <c r="S83" s="112"/>
+      <c r="T83" s="112"/>
+      <c r="U83" s="112"/>
+      <c r="V83" s="112"/>
+      <c r="W83" s="112"/>
+      <c r="X83" s="112"/>
+      <c r="Y83" s="112"/>
+      <c r="Z83" s="112"/>
+      <c r="AA83" s="112"/>
+      <c r="AB83" s="112"/>
+      <c r="AC83" s="112"/>
+      <c r="AD83" s="112"/>
+      <c r="AE83" s="112"/>
+      <c r="AF83" s="112"/>
+      <c r="AG83" s="112"/>
+      <c r="AH83" s="112"/>
+      <c r="AI83" s="112"/>
+      <c r="AJ83" s="112"/>
+      <c r="AK83" s="112"/>
+      <c r="AL83" s="112"/>
+      <c r="AM83" s="112"/>
+      <c r="AN83" s="112"/>
+      <c r="AO83" s="112"/>
+      <c r="AP83" s="112"/>
+      <c r="AQ83" s="112"/>
+      <c r="AR83" s="112"/>
+      <c r="AS83" s="112"/>
+      <c r="AT83" s="113"/>
     </row>
     <row r="84" spans="1:46" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="74"/>
@@ -6621,10 +6621,10 @@
       <c r="L85" s="21"/>
       <c r="M85" s="21"/>
       <c r="N85" s="21"/>
-      <c r="Q85" s="155" t="s">
+      <c r="Q85" s="108" t="s">
         <v>18</v>
       </c>
-      <c r="R85" s="155"/>
+      <c r="R85" s="108"/>
       <c r="S85" s="76"/>
       <c r="T85" s="76"/>
       <c r="U85" s="77"/>
@@ -6955,99 +6955,99 @@
     <row r="93" spans="1:46" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" s="88"/>
       <c r="B93" s="90"/>
-      <c r="C93" s="135" t="s">
+      <c r="C93" s="144" t="s">
         <v>73</v>
       </c>
-      <c r="D93" s="135"/>
-      <c r="E93" s="135"/>
-      <c r="F93" s="135"/>
-      <c r="G93" s="135"/>
-      <c r="H93" s="135"/>
-      <c r="I93" s="135"/>
-      <c r="J93" s="135"/>
-      <c r="K93" s="135"/>
-      <c r="L93" s="135"/>
-      <c r="M93" s="135"/>
-      <c r="N93" s="135"/>
-      <c r="O93" s="135"/>
-      <c r="P93" s="135"/>
-      <c r="Q93" s="135"/>
-      <c r="R93" s="135"/>
-      <c r="S93" s="135"/>
-      <c r="T93" s="135"/>
-      <c r="U93" s="135"/>
-      <c r="V93" s="135"/>
-      <c r="W93" s="135"/>
-      <c r="X93" s="135"/>
-      <c r="Y93" s="135"/>
-      <c r="Z93" s="135"/>
-      <c r="AA93" s="135"/>
-      <c r="AB93" s="135"/>
-      <c r="AC93" s="135"/>
-      <c r="AD93" s="135"/>
-      <c r="AE93" s="135"/>
-      <c r="AF93" s="135"/>
-      <c r="AG93" s="135"/>
-      <c r="AH93" s="135"/>
-      <c r="AI93" s="135"/>
-      <c r="AJ93" s="135"/>
-      <c r="AK93" s="135"/>
-      <c r="AL93" s="135"/>
-      <c r="AM93" s="135"/>
-      <c r="AN93" s="135"/>
-      <c r="AO93" s="135"/>
-      <c r="AP93" s="135"/>
-      <c r="AQ93" s="135"/>
-      <c r="AR93" s="135"/>
-      <c r="AS93" s="135"/>
+      <c r="D93" s="144"/>
+      <c r="E93" s="144"/>
+      <c r="F93" s="144"/>
+      <c r="G93" s="144"/>
+      <c r="H93" s="144"/>
+      <c r="I93" s="144"/>
+      <c r="J93" s="144"/>
+      <c r="K93" s="144"/>
+      <c r="L93" s="144"/>
+      <c r="M93" s="144"/>
+      <c r="N93" s="144"/>
+      <c r="O93" s="144"/>
+      <c r="P93" s="144"/>
+      <c r="Q93" s="144"/>
+      <c r="R93" s="144"/>
+      <c r="S93" s="144"/>
+      <c r="T93" s="144"/>
+      <c r="U93" s="144"/>
+      <c r="V93" s="144"/>
+      <c r="W93" s="144"/>
+      <c r="X93" s="144"/>
+      <c r="Y93" s="144"/>
+      <c r="Z93" s="144"/>
+      <c r="AA93" s="144"/>
+      <c r="AB93" s="144"/>
+      <c r="AC93" s="144"/>
+      <c r="AD93" s="144"/>
+      <c r="AE93" s="144"/>
+      <c r="AF93" s="144"/>
+      <c r="AG93" s="144"/>
+      <c r="AH93" s="144"/>
+      <c r="AI93" s="144"/>
+      <c r="AJ93" s="144"/>
+      <c r="AK93" s="144"/>
+      <c r="AL93" s="144"/>
+      <c r="AM93" s="144"/>
+      <c r="AN93" s="144"/>
+      <c r="AO93" s="144"/>
+      <c r="AP93" s="144"/>
+      <c r="AQ93" s="144"/>
+      <c r="AR93" s="144"/>
+      <c r="AS93" s="144"/>
       <c r="AT93" s="46"/>
     </row>
     <row r="94" spans="1:46" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A94" s="88"/>
       <c r="B94" s="89"/>
-      <c r="C94" s="135"/>
-      <c r="D94" s="135"/>
-      <c r="E94" s="135"/>
-      <c r="F94" s="135"/>
-      <c r="G94" s="135"/>
-      <c r="H94" s="135"/>
-      <c r="I94" s="135"/>
-      <c r="J94" s="135"/>
-      <c r="K94" s="135"/>
-      <c r="L94" s="135"/>
-      <c r="M94" s="135"/>
-      <c r="N94" s="135"/>
-      <c r="O94" s="135"/>
-      <c r="P94" s="135"/>
-      <c r="Q94" s="135"/>
-      <c r="R94" s="135"/>
-      <c r="S94" s="135"/>
-      <c r="T94" s="135"/>
-      <c r="U94" s="135"/>
-      <c r="V94" s="135"/>
-      <c r="W94" s="135"/>
-      <c r="X94" s="135"/>
-      <c r="Y94" s="135"/>
-      <c r="Z94" s="135"/>
-      <c r="AA94" s="135"/>
-      <c r="AB94" s="135"/>
-      <c r="AC94" s="135"/>
-      <c r="AD94" s="135"/>
-      <c r="AE94" s="135"/>
-      <c r="AF94" s="135"/>
-      <c r="AG94" s="135"/>
-      <c r="AH94" s="135"/>
-      <c r="AI94" s="135"/>
-      <c r="AJ94" s="135"/>
-      <c r="AK94" s="135"/>
-      <c r="AL94" s="135"/>
-      <c r="AM94" s="135"/>
-      <c r="AN94" s="135"/>
-      <c r="AO94" s="135"/>
-      <c r="AP94" s="135"/>
-      <c r="AQ94" s="135"/>
-      <c r="AR94" s="135"/>
-      <c r="AS94" s="135"/>
+      <c r="C94" s="144"/>
+      <c r="D94" s="144"/>
+      <c r="E94" s="144"/>
+      <c r="F94" s="144"/>
+      <c r="G94" s="144"/>
+      <c r="H94" s="144"/>
+      <c r="I94" s="144"/>
+      <c r="J94" s="144"/>
+      <c r="K94" s="144"/>
+      <c r="L94" s="144"/>
+      <c r="M94" s="144"/>
+      <c r="N94" s="144"/>
+      <c r="O94" s="144"/>
+      <c r="P94" s="144"/>
+      <c r="Q94" s="144"/>
+      <c r="R94" s="144"/>
+      <c r="S94" s="144"/>
+      <c r="T94" s="144"/>
+      <c r="U94" s="144"/>
+      <c r="V94" s="144"/>
+      <c r="W94" s="144"/>
+      <c r="X94" s="144"/>
+      <c r="Y94" s="144"/>
+      <c r="Z94" s="144"/>
+      <c r="AA94" s="144"/>
+      <c r="AB94" s="144"/>
+      <c r="AC94" s="144"/>
+      <c r="AD94" s="144"/>
+      <c r="AE94" s="144"/>
+      <c r="AF94" s="144"/>
+      <c r="AG94" s="144"/>
+      <c r="AH94" s="144"/>
+      <c r="AI94" s="144"/>
+      <c r="AJ94" s="144"/>
+      <c r="AK94" s="144"/>
+      <c r="AL94" s="144"/>
+      <c r="AM94" s="144"/>
+      <c r="AN94" s="144"/>
+      <c r="AO94" s="144"/>
+      <c r="AP94" s="144"/>
+      <c r="AQ94" s="144"/>
+      <c r="AR94" s="144"/>
+      <c r="AS94" s="144"/>
       <c r="AT94" s="46"/>
     </row>
     <row r="95" spans="1:46" ht="12.75" x14ac:dyDescent="0.2">
@@ -7100,99 +7100,99 @@
     <row r="96" spans="1:46" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" s="88"/>
       <c r="B96" s="89"/>
-      <c r="C96" s="134" t="s">
+      <c r="C96" s="143" t="s">
         <v>74</v>
       </c>
-      <c r="D96" s="134"/>
-      <c r="E96" s="134"/>
-      <c r="F96" s="134"/>
-      <c r="G96" s="134"/>
-      <c r="H96" s="134"/>
-      <c r="I96" s="134"/>
-      <c r="J96" s="134"/>
-      <c r="K96" s="134"/>
-      <c r="L96" s="134"/>
-      <c r="M96" s="134"/>
-      <c r="N96" s="134"/>
-      <c r="O96" s="134"/>
-      <c r="P96" s="134"/>
-      <c r="Q96" s="134"/>
-      <c r="R96" s="134"/>
-      <c r="S96" s="134"/>
-      <c r="T96" s="134"/>
-      <c r="U96" s="134"/>
-      <c r="V96" s="134"/>
-      <c r="W96" s="134"/>
-      <c r="X96" s="134"/>
-      <c r="Y96" s="134"/>
-      <c r="Z96" s="134"/>
-      <c r="AA96" s="134"/>
-      <c r="AB96" s="134"/>
-      <c r="AC96" s="134"/>
-      <c r="AD96" s="134"/>
-      <c r="AE96" s="134"/>
-      <c r="AF96" s="134"/>
-      <c r="AG96" s="134"/>
-      <c r="AH96" s="134"/>
-      <c r="AI96" s="134"/>
-      <c r="AJ96" s="134"/>
-      <c r="AK96" s="134"/>
-      <c r="AL96" s="134"/>
-      <c r="AM96" s="134"/>
-      <c r="AN96" s="134"/>
-      <c r="AO96" s="134"/>
-      <c r="AP96" s="134"/>
-      <c r="AQ96" s="134"/>
-      <c r="AR96" s="134"/>
-      <c r="AS96" s="134"/>
+      <c r="D96" s="143"/>
+      <c r="E96" s="143"/>
+      <c r="F96" s="143"/>
+      <c r="G96" s="143"/>
+      <c r="H96" s="143"/>
+      <c r="I96" s="143"/>
+      <c r="J96" s="143"/>
+      <c r="K96" s="143"/>
+      <c r="L96" s="143"/>
+      <c r="M96" s="143"/>
+      <c r="N96" s="143"/>
+      <c r="O96" s="143"/>
+      <c r="P96" s="143"/>
+      <c r="Q96" s="143"/>
+      <c r="R96" s="143"/>
+      <c r="S96" s="143"/>
+      <c r="T96" s="143"/>
+      <c r="U96" s="143"/>
+      <c r="V96" s="143"/>
+      <c r="W96" s="143"/>
+      <c r="X96" s="143"/>
+      <c r="Y96" s="143"/>
+      <c r="Z96" s="143"/>
+      <c r="AA96" s="143"/>
+      <c r="AB96" s="143"/>
+      <c r="AC96" s="143"/>
+      <c r="AD96" s="143"/>
+      <c r="AE96" s="143"/>
+      <c r="AF96" s="143"/>
+      <c r="AG96" s="143"/>
+      <c r="AH96" s="143"/>
+      <c r="AI96" s="143"/>
+      <c r="AJ96" s="143"/>
+      <c r="AK96" s="143"/>
+      <c r="AL96" s="143"/>
+      <c r="AM96" s="143"/>
+      <c r="AN96" s="143"/>
+      <c r="AO96" s="143"/>
+      <c r="AP96" s="143"/>
+      <c r="AQ96" s="143"/>
+      <c r="AR96" s="143"/>
+      <c r="AS96" s="143"/>
       <c r="AT96" s="46"/>
     </row>
     <row r="97" spans="1:46" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A97" s="88"/>
       <c r="B97" s="89"/>
-      <c r="C97" s="134"/>
-      <c r="D97" s="134"/>
-      <c r="E97" s="134"/>
-      <c r="F97" s="134"/>
-      <c r="G97" s="134"/>
-      <c r="H97" s="134"/>
-      <c r="I97" s="134"/>
-      <c r="J97" s="134"/>
-      <c r="K97" s="134"/>
-      <c r="L97" s="134"/>
-      <c r="M97" s="134"/>
-      <c r="N97" s="134"/>
-      <c r="O97" s="134"/>
-      <c r="P97" s="134"/>
-      <c r="Q97" s="134"/>
-      <c r="R97" s="134"/>
-      <c r="S97" s="134"/>
-      <c r="T97" s="134"/>
-      <c r="U97" s="134"/>
-      <c r="V97" s="134"/>
-      <c r="W97" s="134"/>
-      <c r="X97" s="134"/>
-      <c r="Y97" s="134"/>
-      <c r="Z97" s="134"/>
-      <c r="AA97" s="134"/>
-      <c r="AB97" s="134"/>
-      <c r="AC97" s="134"/>
-      <c r="AD97" s="134"/>
-      <c r="AE97" s="134"/>
-      <c r="AF97" s="134"/>
-      <c r="AG97" s="134"/>
-      <c r="AH97" s="134"/>
-      <c r="AI97" s="134"/>
-      <c r="AJ97" s="134"/>
-      <c r="AK97" s="134"/>
-      <c r="AL97" s="134"/>
-      <c r="AM97" s="134"/>
-      <c r="AN97" s="134"/>
-      <c r="AO97" s="134"/>
-      <c r="AP97" s="134"/>
-      <c r="AQ97" s="134"/>
-      <c r="AR97" s="134"/>
-      <c r="AS97" s="134"/>
+      <c r="C97" s="143"/>
+      <c r="D97" s="143"/>
+      <c r="E97" s="143"/>
+      <c r="F97" s="143"/>
+      <c r="G97" s="143"/>
+      <c r="H97" s="143"/>
+      <c r="I97" s="143"/>
+      <c r="J97" s="143"/>
+      <c r="K97" s="143"/>
+      <c r="L97" s="143"/>
+      <c r="M97" s="143"/>
+      <c r="N97" s="143"/>
+      <c r="O97" s="143"/>
+      <c r="P97" s="143"/>
+      <c r="Q97" s="143"/>
+      <c r="R97" s="143"/>
+      <c r="S97" s="143"/>
+      <c r="T97" s="143"/>
+      <c r="U97" s="143"/>
+      <c r="V97" s="143"/>
+      <c r="W97" s="143"/>
+      <c r="X97" s="143"/>
+      <c r="Y97" s="143"/>
+      <c r="Z97" s="143"/>
+      <c r="AA97" s="143"/>
+      <c r="AB97" s="143"/>
+      <c r="AC97" s="143"/>
+      <c r="AD97" s="143"/>
+      <c r="AE97" s="143"/>
+      <c r="AF97" s="143"/>
+      <c r="AG97" s="143"/>
+      <c r="AH97" s="143"/>
+      <c r="AI97" s="143"/>
+      <c r="AJ97" s="143"/>
+      <c r="AK97" s="143"/>
+      <c r="AL97" s="143"/>
+      <c r="AM97" s="143"/>
+      <c r="AN97" s="143"/>
+      <c r="AO97" s="143"/>
+      <c r="AP97" s="143"/>
+      <c r="AQ97" s="143"/>
+      <c r="AR97" s="143"/>
+      <c r="AS97" s="143"/>
       <c r="AT97" s="46"/>
     </row>
     <row r="98" spans="1:46" ht="12.75" x14ac:dyDescent="0.2">
@@ -7245,99 +7245,99 @@
     <row r="99" spans="1:46" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" s="88"/>
       <c r="B99" s="90"/>
-      <c r="C99" s="134" t="s">
+      <c r="C99" s="143" t="s">
         <v>87</v>
       </c>
-      <c r="D99" s="134"/>
-      <c r="E99" s="134"/>
-      <c r="F99" s="134"/>
-      <c r="G99" s="134"/>
-      <c r="H99" s="134"/>
-      <c r="I99" s="134"/>
-      <c r="J99" s="134"/>
-      <c r="K99" s="134"/>
-      <c r="L99" s="134"/>
-      <c r="M99" s="134"/>
-      <c r="N99" s="134"/>
-      <c r="O99" s="134"/>
-      <c r="P99" s="134"/>
-      <c r="Q99" s="134"/>
-      <c r="R99" s="134"/>
-      <c r="S99" s="134"/>
-      <c r="T99" s="134"/>
-      <c r="U99" s="134"/>
-      <c r="V99" s="134"/>
-      <c r="W99" s="134"/>
-      <c r="X99" s="134"/>
-      <c r="Y99" s="134"/>
-      <c r="Z99" s="134"/>
-      <c r="AA99" s="134"/>
-      <c r="AB99" s="134"/>
-      <c r="AC99" s="134"/>
-      <c r="AD99" s="134"/>
-      <c r="AE99" s="134"/>
-      <c r="AF99" s="134"/>
-      <c r="AG99" s="134"/>
-      <c r="AH99" s="134"/>
-      <c r="AI99" s="134"/>
-      <c r="AJ99" s="134"/>
-      <c r="AK99" s="134"/>
-      <c r="AL99" s="134"/>
-      <c r="AM99" s="134"/>
-      <c r="AN99" s="134"/>
-      <c r="AO99" s="134"/>
-      <c r="AP99" s="134"/>
-      <c r="AQ99" s="134"/>
-      <c r="AR99" s="134"/>
-      <c r="AS99" s="134"/>
+      <c r="D99" s="143"/>
+      <c r="E99" s="143"/>
+      <c r="F99" s="143"/>
+      <c r="G99" s="143"/>
+      <c r="H99" s="143"/>
+      <c r="I99" s="143"/>
+      <c r="J99" s="143"/>
+      <c r="K99" s="143"/>
+      <c r="L99" s="143"/>
+      <c r="M99" s="143"/>
+      <c r="N99" s="143"/>
+      <c r="O99" s="143"/>
+      <c r="P99" s="143"/>
+      <c r="Q99" s="143"/>
+      <c r="R99" s="143"/>
+      <c r="S99" s="143"/>
+      <c r="T99" s="143"/>
+      <c r="U99" s="143"/>
+      <c r="V99" s="143"/>
+      <c r="W99" s="143"/>
+      <c r="X99" s="143"/>
+      <c r="Y99" s="143"/>
+      <c r="Z99" s="143"/>
+      <c r="AA99" s="143"/>
+      <c r="AB99" s="143"/>
+      <c r="AC99" s="143"/>
+      <c r="AD99" s="143"/>
+      <c r="AE99" s="143"/>
+      <c r="AF99" s="143"/>
+      <c r="AG99" s="143"/>
+      <c r="AH99" s="143"/>
+      <c r="AI99" s="143"/>
+      <c r="AJ99" s="143"/>
+      <c r="AK99" s="143"/>
+      <c r="AL99" s="143"/>
+      <c r="AM99" s="143"/>
+      <c r="AN99" s="143"/>
+      <c r="AO99" s="143"/>
+      <c r="AP99" s="143"/>
+      <c r="AQ99" s="143"/>
+      <c r="AR99" s="143"/>
+      <c r="AS99" s="143"/>
       <c r="AT99" s="46"/>
     </row>
     <row r="100" spans="1:46" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A100" s="88"/>
       <c r="B100" s="89"/>
-      <c r="C100" s="134"/>
-      <c r="D100" s="134"/>
-      <c r="E100" s="134"/>
-      <c r="F100" s="134"/>
-      <c r="G100" s="134"/>
-      <c r="H100" s="134"/>
-      <c r="I100" s="134"/>
-      <c r="J100" s="134"/>
-      <c r="K100" s="134"/>
-      <c r="L100" s="134"/>
-      <c r="M100" s="134"/>
-      <c r="N100" s="134"/>
-      <c r="O100" s="134"/>
-      <c r="P100" s="134"/>
-      <c r="Q100" s="134"/>
-      <c r="R100" s="134"/>
-      <c r="S100" s="134"/>
-      <c r="T100" s="134"/>
-      <c r="U100" s="134"/>
-      <c r="V100" s="134"/>
-      <c r="W100" s="134"/>
-      <c r="X100" s="134"/>
-      <c r="Y100" s="134"/>
-      <c r="Z100" s="134"/>
-      <c r="AA100" s="134"/>
-      <c r="AB100" s="134"/>
-      <c r="AC100" s="134"/>
-      <c r="AD100" s="134"/>
-      <c r="AE100" s="134"/>
-      <c r="AF100" s="134"/>
-      <c r="AG100" s="134"/>
-      <c r="AH100" s="134"/>
-      <c r="AI100" s="134"/>
-      <c r="AJ100" s="134"/>
-      <c r="AK100" s="134"/>
-      <c r="AL100" s="134"/>
-      <c r="AM100" s="134"/>
-      <c r="AN100" s="134"/>
-      <c r="AO100" s="134"/>
-      <c r="AP100" s="134"/>
-      <c r="AQ100" s="134"/>
-      <c r="AR100" s="134"/>
-      <c r="AS100" s="134"/>
+      <c r="C100" s="143"/>
+      <c r="D100" s="143"/>
+      <c r="E100" s="143"/>
+      <c r="F100" s="143"/>
+      <c r="G100" s="143"/>
+      <c r="H100" s="143"/>
+      <c r="I100" s="143"/>
+      <c r="J100" s="143"/>
+      <c r="K100" s="143"/>
+      <c r="L100" s="143"/>
+      <c r="M100" s="143"/>
+      <c r="N100" s="143"/>
+      <c r="O100" s="143"/>
+      <c r="P100" s="143"/>
+      <c r="Q100" s="143"/>
+      <c r="R100" s="143"/>
+      <c r="S100" s="143"/>
+      <c r="T100" s="143"/>
+      <c r="U100" s="143"/>
+      <c r="V100" s="143"/>
+      <c r="W100" s="143"/>
+      <c r="X100" s="143"/>
+      <c r="Y100" s="143"/>
+      <c r="Z100" s="143"/>
+      <c r="AA100" s="143"/>
+      <c r="AB100" s="143"/>
+      <c r="AC100" s="143"/>
+      <c r="AD100" s="143"/>
+      <c r="AE100" s="143"/>
+      <c r="AF100" s="143"/>
+      <c r="AG100" s="143"/>
+      <c r="AH100" s="143"/>
+      <c r="AI100" s="143"/>
+      <c r="AJ100" s="143"/>
+      <c r="AK100" s="143"/>
+      <c r="AL100" s="143"/>
+      <c r="AM100" s="143"/>
+      <c r="AN100" s="143"/>
+      <c r="AO100" s="143"/>
+      <c r="AP100" s="143"/>
+      <c r="AQ100" s="143"/>
+      <c r="AR100" s="143"/>
+      <c r="AS100" s="143"/>
       <c r="AT100" s="46"/>
     </row>
     <row r="101" spans="1:46" ht="5.85" customHeight="1" x14ac:dyDescent="0.2">
@@ -7774,96 +7774,96 @@
     <row r="110" spans="1:46" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A110" s="88"/>
       <c r="B110" s="90"/>
-      <c r="C110" s="134" t="s">
+      <c r="C110" s="143" t="s">
         <v>79</v>
       </c>
-      <c r="D110" s="134"/>
-      <c r="E110" s="134"/>
-      <c r="F110" s="134"/>
-      <c r="G110" s="134"/>
-      <c r="H110" s="134"/>
-      <c r="I110" s="134"/>
-      <c r="J110" s="134"/>
-      <c r="K110" s="134"/>
-      <c r="L110" s="134"/>
-      <c r="M110" s="134"/>
-      <c r="N110" s="134"/>
-      <c r="O110" s="134"/>
-      <c r="P110" s="134"/>
-      <c r="Q110" s="134"/>
-      <c r="R110" s="134"/>
-      <c r="S110" s="134"/>
-      <c r="T110" s="134"/>
-      <c r="U110" s="134"/>
-      <c r="V110" s="134"/>
-      <c r="W110" s="134"/>
-      <c r="X110" s="134"/>
-      <c r="Y110" s="134"/>
-      <c r="Z110" s="134"/>
-      <c r="AA110" s="134"/>
-      <c r="AB110" s="134"/>
-      <c r="AC110" s="134"/>
-      <c r="AD110" s="134"/>
-      <c r="AE110" s="134"/>
-      <c r="AF110" s="134"/>
-      <c r="AG110" s="134"/>
-      <c r="AH110" s="134"/>
-      <c r="AI110" s="134"/>
-      <c r="AJ110" s="134"/>
-      <c r="AK110" s="134"/>
-      <c r="AL110" s="134"/>
-      <c r="AM110" s="134"/>
-      <c r="AN110" s="134"/>
-      <c r="AO110" s="134"/>
-      <c r="AP110" s="134"/>
-      <c r="AQ110" s="134"/>
+      <c r="D110" s="143"/>
+      <c r="E110" s="143"/>
+      <c r="F110" s="143"/>
+      <c r="G110" s="143"/>
+      <c r="H110" s="143"/>
+      <c r="I110" s="143"/>
+      <c r="J110" s="143"/>
+      <c r="K110" s="143"/>
+      <c r="L110" s="143"/>
+      <c r="M110" s="143"/>
+      <c r="N110" s="143"/>
+      <c r="O110" s="143"/>
+      <c r="P110" s="143"/>
+      <c r="Q110" s="143"/>
+      <c r="R110" s="143"/>
+      <c r="S110" s="143"/>
+      <c r="T110" s="143"/>
+      <c r="U110" s="143"/>
+      <c r="V110" s="143"/>
+      <c r="W110" s="143"/>
+      <c r="X110" s="143"/>
+      <c r="Y110" s="143"/>
+      <c r="Z110" s="143"/>
+      <c r="AA110" s="143"/>
+      <c r="AB110" s="143"/>
+      <c r="AC110" s="143"/>
+      <c r="AD110" s="143"/>
+      <c r="AE110" s="143"/>
+      <c r="AF110" s="143"/>
+      <c r="AG110" s="143"/>
+      <c r="AH110" s="143"/>
+      <c r="AI110" s="143"/>
+      <c r="AJ110" s="143"/>
+      <c r="AK110" s="143"/>
+      <c r="AL110" s="143"/>
+      <c r="AM110" s="143"/>
+      <c r="AN110" s="143"/>
+      <c r="AO110" s="143"/>
+      <c r="AP110" s="143"/>
+      <c r="AQ110" s="143"/>
       <c r="AR110" s="89"/>
       <c r="AT110" s="46"/>
     </row>
     <row r="111" spans="1:46" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A111" s="88"/>
       <c r="B111" s="93"/>
-      <c r="C111" s="134"/>
-      <c r="D111" s="134"/>
-      <c r="E111" s="134"/>
-      <c r="F111" s="134"/>
-      <c r="G111" s="134"/>
-      <c r="H111" s="134"/>
-      <c r="I111" s="134"/>
-      <c r="J111" s="134"/>
-      <c r="K111" s="134"/>
-      <c r="L111" s="134"/>
-      <c r="M111" s="134"/>
-      <c r="N111" s="134"/>
-      <c r="O111" s="134"/>
-      <c r="P111" s="134"/>
-      <c r="Q111" s="134"/>
-      <c r="R111" s="134"/>
-      <c r="S111" s="134"/>
-      <c r="T111" s="134"/>
-      <c r="U111" s="134"/>
-      <c r="V111" s="134"/>
-      <c r="W111" s="134"/>
-      <c r="X111" s="134"/>
-      <c r="Y111" s="134"/>
-      <c r="Z111" s="134"/>
-      <c r="AA111" s="134"/>
-      <c r="AB111" s="134"/>
-      <c r="AC111" s="134"/>
-      <c r="AD111" s="134"/>
-      <c r="AE111" s="134"/>
-      <c r="AF111" s="134"/>
-      <c r="AG111" s="134"/>
-      <c r="AH111" s="134"/>
-      <c r="AI111" s="134"/>
-      <c r="AJ111" s="134"/>
-      <c r="AK111" s="134"/>
-      <c r="AL111" s="134"/>
-      <c r="AM111" s="134"/>
-      <c r="AN111" s="134"/>
-      <c r="AO111" s="134"/>
-      <c r="AP111" s="134"/>
-      <c r="AQ111" s="134"/>
+      <c r="C111" s="143"/>
+      <c r="D111" s="143"/>
+      <c r="E111" s="143"/>
+      <c r="F111" s="143"/>
+      <c r="G111" s="143"/>
+      <c r="H111" s="143"/>
+      <c r="I111" s="143"/>
+      <c r="J111" s="143"/>
+      <c r="K111" s="143"/>
+      <c r="L111" s="143"/>
+      <c r="M111" s="143"/>
+      <c r="N111" s="143"/>
+      <c r="O111" s="143"/>
+      <c r="P111" s="143"/>
+      <c r="Q111" s="143"/>
+      <c r="R111" s="143"/>
+      <c r="S111" s="143"/>
+      <c r="T111" s="143"/>
+      <c r="U111" s="143"/>
+      <c r="V111" s="143"/>
+      <c r="W111" s="143"/>
+      <c r="X111" s="143"/>
+      <c r="Y111" s="143"/>
+      <c r="Z111" s="143"/>
+      <c r="AA111" s="143"/>
+      <c r="AB111" s="143"/>
+      <c r="AC111" s="143"/>
+      <c r="AD111" s="143"/>
+      <c r="AE111" s="143"/>
+      <c r="AF111" s="143"/>
+      <c r="AG111" s="143"/>
+      <c r="AH111" s="143"/>
+      <c r="AI111" s="143"/>
+      <c r="AJ111" s="143"/>
+      <c r="AK111" s="143"/>
+      <c r="AL111" s="143"/>
+      <c r="AM111" s="143"/>
+      <c r="AN111" s="143"/>
+      <c r="AO111" s="143"/>
+      <c r="AP111" s="143"/>
+      <c r="AQ111" s="143"/>
       <c r="AR111" s="89"/>
       <c r="AT111" s="46"/>
     </row>
@@ -7917,144 +7917,144 @@
     <row r="113" spans="1:46" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A113" s="88"/>
       <c r="B113" s="90"/>
-      <c r="C113" s="133" t="s">
+      <c r="C113" s="142" t="s">
         <v>80</v>
       </c>
-      <c r="D113" s="133"/>
-      <c r="E113" s="133"/>
-      <c r="F113" s="133"/>
-      <c r="G113" s="133"/>
-      <c r="H113" s="133"/>
-      <c r="I113" s="133"/>
-      <c r="J113" s="133"/>
-      <c r="K113" s="133"/>
-      <c r="L113" s="133"/>
-      <c r="M113" s="133"/>
-      <c r="N113" s="133"/>
-      <c r="O113" s="133"/>
-      <c r="P113" s="133"/>
-      <c r="Q113" s="133"/>
-      <c r="R113" s="133"/>
-      <c r="S113" s="133"/>
-      <c r="T113" s="133"/>
-      <c r="U113" s="133"/>
-      <c r="V113" s="133"/>
-      <c r="W113" s="133"/>
-      <c r="X113" s="133"/>
-      <c r="Y113" s="133"/>
-      <c r="Z113" s="133"/>
-      <c r="AA113" s="133"/>
-      <c r="AB113" s="133"/>
-      <c r="AC113" s="133"/>
-      <c r="AD113" s="133"/>
-      <c r="AE113" s="133"/>
-      <c r="AF113" s="133"/>
-      <c r="AG113" s="133"/>
-      <c r="AH113" s="133"/>
-      <c r="AI113" s="133"/>
-      <c r="AJ113" s="133"/>
-      <c r="AK113" s="133"/>
-      <c r="AL113" s="133"/>
-      <c r="AM113" s="133"/>
-      <c r="AN113" s="133"/>
-      <c r="AO113" s="133"/>
-      <c r="AP113" s="133"/>
-      <c r="AQ113" s="133"/>
-      <c r="AR113" s="133"/>
+      <c r="D113" s="142"/>
+      <c r="E113" s="142"/>
+      <c r="F113" s="142"/>
+      <c r="G113" s="142"/>
+      <c r="H113" s="142"/>
+      <c r="I113" s="142"/>
+      <c r="J113" s="142"/>
+      <c r="K113" s="142"/>
+      <c r="L113" s="142"/>
+      <c r="M113" s="142"/>
+      <c r="N113" s="142"/>
+      <c r="O113" s="142"/>
+      <c r="P113" s="142"/>
+      <c r="Q113" s="142"/>
+      <c r="R113" s="142"/>
+      <c r="S113" s="142"/>
+      <c r="T113" s="142"/>
+      <c r="U113" s="142"/>
+      <c r="V113" s="142"/>
+      <c r="W113" s="142"/>
+      <c r="X113" s="142"/>
+      <c r="Y113" s="142"/>
+      <c r="Z113" s="142"/>
+      <c r="AA113" s="142"/>
+      <c r="AB113" s="142"/>
+      <c r="AC113" s="142"/>
+      <c r="AD113" s="142"/>
+      <c r="AE113" s="142"/>
+      <c r="AF113" s="142"/>
+      <c r="AG113" s="142"/>
+      <c r="AH113" s="142"/>
+      <c r="AI113" s="142"/>
+      <c r="AJ113" s="142"/>
+      <c r="AK113" s="142"/>
+      <c r="AL113" s="142"/>
+      <c r="AM113" s="142"/>
+      <c r="AN113" s="142"/>
+      <c r="AO113" s="142"/>
+      <c r="AP113" s="142"/>
+      <c r="AQ113" s="142"/>
+      <c r="AR113" s="142"/>
       <c r="AT113" s="46"/>
     </row>
     <row r="114" spans="1:46" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A114" s="88"/>
       <c r="B114" s="93"/>
-      <c r="C114" s="133"/>
-      <c r="D114" s="133"/>
-      <c r="E114" s="133"/>
-      <c r="F114" s="133"/>
-      <c r="G114" s="133"/>
-      <c r="H114" s="133"/>
-      <c r="I114" s="133"/>
-      <c r="J114" s="133"/>
-      <c r="K114" s="133"/>
-      <c r="L114" s="133"/>
-      <c r="M114" s="133"/>
-      <c r="N114" s="133"/>
-      <c r="O114" s="133"/>
-      <c r="P114" s="133"/>
-      <c r="Q114" s="133"/>
-      <c r="R114" s="133"/>
-      <c r="S114" s="133"/>
-      <c r="T114" s="133"/>
-      <c r="U114" s="133"/>
-      <c r="V114" s="133"/>
-      <c r="W114" s="133"/>
-      <c r="X114" s="133"/>
-      <c r="Y114" s="133"/>
-      <c r="Z114" s="133"/>
-      <c r="AA114" s="133"/>
-      <c r="AB114" s="133"/>
-      <c r="AC114" s="133"/>
-      <c r="AD114" s="133"/>
-      <c r="AE114" s="133"/>
-      <c r="AF114" s="133"/>
-      <c r="AG114" s="133"/>
-      <c r="AH114" s="133"/>
-      <c r="AI114" s="133"/>
-      <c r="AJ114" s="133"/>
-      <c r="AK114" s="133"/>
-      <c r="AL114" s="133"/>
-      <c r="AM114" s="133"/>
-      <c r="AN114" s="133"/>
-      <c r="AO114" s="133"/>
-      <c r="AP114" s="133"/>
-      <c r="AQ114" s="133"/>
-      <c r="AR114" s="133"/>
+      <c r="C114" s="142"/>
+      <c r="D114" s="142"/>
+      <c r="E114" s="142"/>
+      <c r="F114" s="142"/>
+      <c r="G114" s="142"/>
+      <c r="H114" s="142"/>
+      <c r="I114" s="142"/>
+      <c r="J114" s="142"/>
+      <c r="K114" s="142"/>
+      <c r="L114" s="142"/>
+      <c r="M114" s="142"/>
+      <c r="N114" s="142"/>
+      <c r="O114" s="142"/>
+      <c r="P114" s="142"/>
+      <c r="Q114" s="142"/>
+      <c r="R114" s="142"/>
+      <c r="S114" s="142"/>
+      <c r="T114" s="142"/>
+      <c r="U114" s="142"/>
+      <c r="V114" s="142"/>
+      <c r="W114" s="142"/>
+      <c r="X114" s="142"/>
+      <c r="Y114" s="142"/>
+      <c r="Z114" s="142"/>
+      <c r="AA114" s="142"/>
+      <c r="AB114" s="142"/>
+      <c r="AC114" s="142"/>
+      <c r="AD114" s="142"/>
+      <c r="AE114" s="142"/>
+      <c r="AF114" s="142"/>
+      <c r="AG114" s="142"/>
+      <c r="AH114" s="142"/>
+      <c r="AI114" s="142"/>
+      <c r="AJ114" s="142"/>
+      <c r="AK114" s="142"/>
+      <c r="AL114" s="142"/>
+      <c r="AM114" s="142"/>
+      <c r="AN114" s="142"/>
+      <c r="AO114" s="142"/>
+      <c r="AP114" s="142"/>
+      <c r="AQ114" s="142"/>
+      <c r="AR114" s="142"/>
       <c r="AT114" s="46"/>
     </row>
     <row r="115" spans="1:46" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A115" s="88"/>
       <c r="B115" s="93"/>
-      <c r="C115" s="133"/>
-      <c r="D115" s="133"/>
-      <c r="E115" s="133"/>
-      <c r="F115" s="133"/>
-      <c r="G115" s="133"/>
-      <c r="H115" s="133"/>
-      <c r="I115" s="133"/>
-      <c r="J115" s="133"/>
-      <c r="K115" s="133"/>
-      <c r="L115" s="133"/>
-      <c r="M115" s="133"/>
-      <c r="N115" s="133"/>
-      <c r="O115" s="133"/>
-      <c r="P115" s="133"/>
-      <c r="Q115" s="133"/>
-      <c r="R115" s="133"/>
-      <c r="S115" s="133"/>
-      <c r="T115" s="133"/>
-      <c r="U115" s="133"/>
-      <c r="V115" s="133"/>
-      <c r="W115" s="133"/>
-      <c r="X115" s="133"/>
-      <c r="Y115" s="133"/>
-      <c r="Z115" s="133"/>
-      <c r="AA115" s="133"/>
-      <c r="AB115" s="133"/>
-      <c r="AC115" s="133"/>
-      <c r="AD115" s="133"/>
-      <c r="AE115" s="133"/>
-      <c r="AF115" s="133"/>
-      <c r="AG115" s="133"/>
-      <c r="AH115" s="133"/>
-      <c r="AI115" s="133"/>
-      <c r="AJ115" s="133"/>
-      <c r="AK115" s="133"/>
-      <c r="AL115" s="133"/>
-      <c r="AM115" s="133"/>
-      <c r="AN115" s="133"/>
-      <c r="AO115" s="133"/>
-      <c r="AP115" s="133"/>
-      <c r="AQ115" s="133"/>
-      <c r="AR115" s="133"/>
+      <c r="C115" s="142"/>
+      <c r="D115" s="142"/>
+      <c r="E115" s="142"/>
+      <c r="F115" s="142"/>
+      <c r="G115" s="142"/>
+      <c r="H115" s="142"/>
+      <c r="I115" s="142"/>
+      <c r="J115" s="142"/>
+      <c r="K115" s="142"/>
+      <c r="L115" s="142"/>
+      <c r="M115" s="142"/>
+      <c r="N115" s="142"/>
+      <c r="O115" s="142"/>
+      <c r="P115" s="142"/>
+      <c r="Q115" s="142"/>
+      <c r="R115" s="142"/>
+      <c r="S115" s="142"/>
+      <c r="T115" s="142"/>
+      <c r="U115" s="142"/>
+      <c r="V115" s="142"/>
+      <c r="W115" s="142"/>
+      <c r="X115" s="142"/>
+      <c r="Y115" s="142"/>
+      <c r="Z115" s="142"/>
+      <c r="AA115" s="142"/>
+      <c r="AB115" s="142"/>
+      <c r="AC115" s="142"/>
+      <c r="AD115" s="142"/>
+      <c r="AE115" s="142"/>
+      <c r="AF115" s="142"/>
+      <c r="AG115" s="142"/>
+      <c r="AH115" s="142"/>
+      <c r="AI115" s="142"/>
+      <c r="AJ115" s="142"/>
+      <c r="AK115" s="142"/>
+      <c r="AL115" s="142"/>
+      <c r="AM115" s="142"/>
+      <c r="AN115" s="142"/>
+      <c r="AO115" s="142"/>
+      <c r="AP115" s="142"/>
+      <c r="AQ115" s="142"/>
+      <c r="AR115" s="142"/>
       <c r="AT115" s="46"/>
     </row>
     <row r="116" spans="1:46" ht="5.85" customHeight="1" x14ac:dyDescent="0.2">
@@ -8299,99 +8299,99 @@
     <row r="121" spans="1:46" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A121" s="88"/>
       <c r="B121" s="89"/>
-      <c r="C121" s="163" t="s">
+      <c r="C121" s="117" t="s">
         <v>82</v>
       </c>
-      <c r="D121" s="163"/>
-      <c r="E121" s="163"/>
-      <c r="F121" s="163"/>
-      <c r="G121" s="163"/>
-      <c r="H121" s="163"/>
-      <c r="I121" s="163"/>
-      <c r="J121" s="163"/>
-      <c r="K121" s="163"/>
-      <c r="L121" s="163"/>
-      <c r="M121" s="163"/>
-      <c r="N121" s="163"/>
-      <c r="O121" s="163"/>
-      <c r="P121" s="163"/>
-      <c r="Q121" s="163"/>
-      <c r="R121" s="163"/>
-      <c r="S121" s="163"/>
-      <c r="T121" s="163"/>
-      <c r="U121" s="163"/>
-      <c r="V121" s="163"/>
-      <c r="W121" s="163"/>
-      <c r="X121" s="163"/>
-      <c r="Y121" s="163"/>
-      <c r="Z121" s="163"/>
-      <c r="AA121" s="163"/>
-      <c r="AB121" s="163"/>
-      <c r="AC121" s="163"/>
-      <c r="AD121" s="163"/>
-      <c r="AE121" s="163"/>
-      <c r="AF121" s="163"/>
-      <c r="AG121" s="163"/>
-      <c r="AH121" s="163"/>
-      <c r="AI121" s="163"/>
-      <c r="AJ121" s="163"/>
-      <c r="AK121" s="163"/>
-      <c r="AL121" s="163"/>
-      <c r="AM121" s="163"/>
-      <c r="AN121" s="163"/>
-      <c r="AO121" s="163"/>
-      <c r="AP121" s="163"/>
-      <c r="AQ121" s="163"/>
-      <c r="AR121" s="163"/>
-      <c r="AS121" s="163"/>
+      <c r="D121" s="117"/>
+      <c r="E121" s="117"/>
+      <c r="F121" s="117"/>
+      <c r="G121" s="117"/>
+      <c r="H121" s="117"/>
+      <c r="I121" s="117"/>
+      <c r="J121" s="117"/>
+      <c r="K121" s="117"/>
+      <c r="L121" s="117"/>
+      <c r="M121" s="117"/>
+      <c r="N121" s="117"/>
+      <c r="O121" s="117"/>
+      <c r="P121" s="117"/>
+      <c r="Q121" s="117"/>
+      <c r="R121" s="117"/>
+      <c r="S121" s="117"/>
+      <c r="T121" s="117"/>
+      <c r="U121" s="117"/>
+      <c r="V121" s="117"/>
+      <c r="W121" s="117"/>
+      <c r="X121" s="117"/>
+      <c r="Y121" s="117"/>
+      <c r="Z121" s="117"/>
+      <c r="AA121" s="117"/>
+      <c r="AB121" s="117"/>
+      <c r="AC121" s="117"/>
+      <c r="AD121" s="117"/>
+      <c r="AE121" s="117"/>
+      <c r="AF121" s="117"/>
+      <c r="AG121" s="117"/>
+      <c r="AH121" s="117"/>
+      <c r="AI121" s="117"/>
+      <c r="AJ121" s="117"/>
+      <c r="AK121" s="117"/>
+      <c r="AL121" s="117"/>
+      <c r="AM121" s="117"/>
+      <c r="AN121" s="117"/>
+      <c r="AO121" s="117"/>
+      <c r="AP121" s="117"/>
+      <c r="AQ121" s="117"/>
+      <c r="AR121" s="117"/>
+      <c r="AS121" s="117"/>
       <c r="AT121" s="46"/>
     </row>
     <row r="122" spans="1:46" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A122" s="88"/>
       <c r="B122" s="89"/>
-      <c r="C122" s="163"/>
-      <c r="D122" s="163"/>
-      <c r="E122" s="163"/>
-      <c r="F122" s="163"/>
-      <c r="G122" s="163"/>
-      <c r="H122" s="163"/>
-      <c r="I122" s="163"/>
-      <c r="J122" s="163"/>
-      <c r="K122" s="163"/>
-      <c r="L122" s="163"/>
-      <c r="M122" s="163"/>
-      <c r="N122" s="163"/>
-      <c r="O122" s="163"/>
-      <c r="P122" s="163"/>
-      <c r="Q122" s="163"/>
-      <c r="R122" s="163"/>
-      <c r="S122" s="163"/>
-      <c r="T122" s="163"/>
-      <c r="U122" s="163"/>
-      <c r="V122" s="163"/>
-      <c r="W122" s="163"/>
-      <c r="X122" s="163"/>
-      <c r="Y122" s="163"/>
-      <c r="Z122" s="163"/>
-      <c r="AA122" s="163"/>
-      <c r="AB122" s="163"/>
-      <c r="AC122" s="163"/>
-      <c r="AD122" s="163"/>
-      <c r="AE122" s="163"/>
-      <c r="AF122" s="163"/>
-      <c r="AG122" s="163"/>
-      <c r="AH122" s="163"/>
-      <c r="AI122" s="163"/>
-      <c r="AJ122" s="163"/>
-      <c r="AK122" s="163"/>
-      <c r="AL122" s="163"/>
-      <c r="AM122" s="163"/>
-      <c r="AN122" s="163"/>
-      <c r="AO122" s="163"/>
-      <c r="AP122" s="163"/>
-      <c r="AQ122" s="163"/>
-      <c r="AR122" s="163"/>
-      <c r="AS122" s="163"/>
+      <c r="C122" s="117"/>
+      <c r="D122" s="117"/>
+      <c r="E122" s="117"/>
+      <c r="F122" s="117"/>
+      <c r="G122" s="117"/>
+      <c r="H122" s="117"/>
+      <c r="I122" s="117"/>
+      <c r="J122" s="117"/>
+      <c r="K122" s="117"/>
+      <c r="L122" s="117"/>
+      <c r="M122" s="117"/>
+      <c r="N122" s="117"/>
+      <c r="O122" s="117"/>
+      <c r="P122" s="117"/>
+      <c r="Q122" s="117"/>
+      <c r="R122" s="117"/>
+      <c r="S122" s="117"/>
+      <c r="T122" s="117"/>
+      <c r="U122" s="117"/>
+      <c r="V122" s="117"/>
+      <c r="W122" s="117"/>
+      <c r="X122" s="117"/>
+      <c r="Y122" s="117"/>
+      <c r="Z122" s="117"/>
+      <c r="AA122" s="117"/>
+      <c r="AB122" s="117"/>
+      <c r="AC122" s="117"/>
+      <c r="AD122" s="117"/>
+      <c r="AE122" s="117"/>
+      <c r="AF122" s="117"/>
+      <c r="AG122" s="117"/>
+      <c r="AH122" s="117"/>
+      <c r="AI122" s="117"/>
+      <c r="AJ122" s="117"/>
+      <c r="AK122" s="117"/>
+      <c r="AL122" s="117"/>
+      <c r="AM122" s="117"/>
+      <c r="AN122" s="117"/>
+      <c r="AO122" s="117"/>
+      <c r="AP122" s="117"/>
+      <c r="AQ122" s="117"/>
+      <c r="AR122" s="117"/>
+      <c r="AS122" s="117"/>
       <c r="AT122" s="46"/>
     </row>
     <row r="123" spans="1:46" ht="12.75" x14ac:dyDescent="0.2">
@@ -8634,53 +8634,53 @@
     </row>
     <row r="128" spans="1:46" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A128" s="88"/>
-      <c r="B128" s="151" t="s">
+      <c r="B128" s="104" t="s">
         <v>84</v>
       </c>
-      <c r="C128" s="151"/>
-      <c r="D128" s="151"/>
-      <c r="E128" s="151"/>
-      <c r="F128" s="151"/>
-      <c r="G128" s="151"/>
-      <c r="H128" s="151"/>
-      <c r="I128" s="151"/>
-      <c r="J128" s="151"/>
-      <c r="K128" s="151"/>
-      <c r="L128" s="151"/>
-      <c r="M128" s="151"/>
+      <c r="C128" s="104"/>
+      <c r="D128" s="104"/>
+      <c r="E128" s="104"/>
+      <c r="F128" s="104"/>
+      <c r="G128" s="104"/>
+      <c r="H128" s="104"/>
+      <c r="I128" s="104"/>
+      <c r="J128" s="104"/>
+      <c r="K128" s="104"/>
+      <c r="L128" s="104"/>
+      <c r="M128" s="104"/>
       <c r="N128" s="89"/>
       <c r="O128" s="89"/>
-      <c r="Q128" s="151" t="s">
+      <c r="Q128" s="104" t="s">
         <v>85</v>
       </c>
-      <c r="R128" s="151"/>
-      <c r="S128" s="151"/>
-      <c r="T128" s="151"/>
-      <c r="U128" s="151"/>
-      <c r="V128" s="151"/>
-      <c r="W128" s="151"/>
-      <c r="X128" s="151"/>
-      <c r="Y128" s="151"/>
-      <c r="Z128" s="151"/>
-      <c r="AA128" s="151"/>
-      <c r="AB128" s="151"/>
-      <c r="AC128" s="151"/>
-      <c r="AD128" s="151"/>
+      <c r="R128" s="104"/>
+      <c r="S128" s="104"/>
+      <c r="T128" s="104"/>
+      <c r="U128" s="104"/>
+      <c r="V128" s="104"/>
+      <c r="W128" s="104"/>
+      <c r="X128" s="104"/>
+      <c r="Y128" s="104"/>
+      <c r="Z128" s="104"/>
+      <c r="AA128" s="104"/>
+      <c r="AB128" s="104"/>
+      <c r="AC128" s="104"/>
+      <c r="AD128" s="104"/>
       <c r="AE128" s="89"/>
-      <c r="AH128" s="151" t="s">
+      <c r="AH128" s="104" t="s">
         <v>85</v>
       </c>
-      <c r="AI128" s="151"/>
-      <c r="AJ128" s="151"/>
-      <c r="AK128" s="151"/>
-      <c r="AL128" s="151"/>
-      <c r="AM128" s="151"/>
-      <c r="AN128" s="151"/>
-      <c r="AO128" s="151"/>
-      <c r="AP128" s="151"/>
-      <c r="AQ128" s="151"/>
-      <c r="AR128" s="151"/>
-      <c r="AS128" s="151"/>
+      <c r="AI128" s="104"/>
+      <c r="AJ128" s="104"/>
+      <c r="AK128" s="104"/>
+      <c r="AL128" s="104"/>
+      <c r="AM128" s="104"/>
+      <c r="AN128" s="104"/>
+      <c r="AO128" s="104"/>
+      <c r="AP128" s="104"/>
+      <c r="AQ128" s="104"/>
+      <c r="AR128" s="104"/>
+      <c r="AS128" s="104"/>
       <c r="AT128" s="46"/>
     </row>
     <row r="129" spans="1:46" ht="12.75" x14ac:dyDescent="0.2">
@@ -8688,15 +8688,15 @@
       <c r="B129" s="100"/>
       <c r="C129" s="100"/>
       <c r="D129" s="100"/>
-      <c r="E129" s="152" t="str">
+      <c r="E129" s="105" t="str">
         <f>IFERROR(VLOOKUP($B$3,Dados!K1:M9,2,),"")</f>
         <v/>
       </c>
-      <c r="F129" s="153"/>
-      <c r="G129" s="153"/>
-      <c r="H129" s="153"/>
-      <c r="I129" s="153"/>
-      <c r="J129" s="154"/>
+      <c r="F129" s="106"/>
+      <c r="G129" s="106"/>
+      <c r="H129" s="106"/>
+      <c r="I129" s="106"/>
+      <c r="J129" s="107"/>
       <c r="K129" s="89"/>
       <c r="L129" s="89"/>
       <c r="M129" s="89"/>
@@ -8736,14 +8736,14 @@
       <c r="B130" s="100"/>
       <c r="C130" s="100"/>
       <c r="D130" s="100"/>
-      <c r="E130" s="150" t="s">
+      <c r="E130" s="103" t="s">
         <v>64</v>
       </c>
-      <c r="F130" s="150"/>
-      <c r="G130" s="150"/>
-      <c r="H130" s="150"/>
-      <c r="I130" s="150"/>
-      <c r="J130" s="150"/>
+      <c r="F130" s="103"/>
+      <c r="G130" s="103"/>
+      <c r="H130" s="103"/>
+      <c r="I130" s="103"/>
+      <c r="J130" s="103"/>
       <c r="K130" s="89"/>
       <c r="L130" s="89"/>
       <c r="M130" s="89"/>
@@ -8833,6 +8833,46 @@
   </sheetData>
   <sheetProtection selectLockedCells="1"/>
   <mergeCells count="56">
+    <mergeCell ref="C61:V62"/>
+    <mergeCell ref="C59:W60"/>
+    <mergeCell ref="C55:W57"/>
+    <mergeCell ref="AH11:AS11"/>
+    <mergeCell ref="AE21:AN21"/>
+    <mergeCell ref="AP21:AS21"/>
+    <mergeCell ref="B21:G21"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="E17:J17"/>
+    <mergeCell ref="K17:M17"/>
+    <mergeCell ref="N17:AH17"/>
+    <mergeCell ref="AL17:AS17"/>
+    <mergeCell ref="D15:AH15"/>
+    <mergeCell ref="S21:V21"/>
+    <mergeCell ref="AL15:AS15"/>
+    <mergeCell ref="C113:AR115"/>
+    <mergeCell ref="C110:AQ111"/>
+    <mergeCell ref="C99:AS100"/>
+    <mergeCell ref="C96:AS97"/>
+    <mergeCell ref="C93:AS94"/>
+    <mergeCell ref="B6:AS6"/>
+    <mergeCell ref="B11:M11"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="F3:I3"/>
+    <mergeCell ref="B8:AS8"/>
+    <mergeCell ref="Z53:AS54"/>
+    <mergeCell ref="Q46:AS49"/>
+    <mergeCell ref="B48:O48"/>
+    <mergeCell ref="D24:AS24"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="E26:J26"/>
+    <mergeCell ref="K26:M26"/>
+    <mergeCell ref="N26:AH26"/>
+    <mergeCell ref="AL26:AS26"/>
+    <mergeCell ref="F40:AS40"/>
+    <mergeCell ref="F42:AS42"/>
+    <mergeCell ref="B44:AS44"/>
+    <mergeCell ref="A42:E42"/>
+    <mergeCell ref="B24:C24"/>
     <mergeCell ref="Z55:AS56"/>
     <mergeCell ref="Z57:AS58"/>
     <mergeCell ref="Z59:AS60"/>
@@ -8849,46 +8889,6 @@
     <mergeCell ref="B78:F78"/>
     <mergeCell ref="T78:AO78"/>
     <mergeCell ref="C121:AS122"/>
-    <mergeCell ref="Z53:AS54"/>
-    <mergeCell ref="Q46:AS49"/>
-    <mergeCell ref="B48:O48"/>
-    <mergeCell ref="D24:AS24"/>
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="E26:J26"/>
-    <mergeCell ref="K26:M26"/>
-    <mergeCell ref="N26:AH26"/>
-    <mergeCell ref="AL26:AS26"/>
-    <mergeCell ref="F40:AS40"/>
-    <mergeCell ref="F42:AS42"/>
-    <mergeCell ref="B44:AS44"/>
-    <mergeCell ref="A42:E42"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B6:AS6"/>
-    <mergeCell ref="B11:M11"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="F3:I3"/>
-    <mergeCell ref="B8:AS8"/>
-    <mergeCell ref="C113:AR115"/>
-    <mergeCell ref="C110:AQ111"/>
-    <mergeCell ref="C99:AS100"/>
-    <mergeCell ref="C96:AS97"/>
-    <mergeCell ref="C93:AS94"/>
-    <mergeCell ref="C61:V62"/>
-    <mergeCell ref="C59:W60"/>
-    <mergeCell ref="C55:W57"/>
-    <mergeCell ref="AH11:AS11"/>
-    <mergeCell ref="AE21:AN21"/>
-    <mergeCell ref="AP21:AS21"/>
-    <mergeCell ref="B21:G21"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="E17:J17"/>
-    <mergeCell ref="K17:M17"/>
-    <mergeCell ref="N17:AH17"/>
-    <mergeCell ref="AL17:AS17"/>
-    <mergeCell ref="D15:AH15"/>
-    <mergeCell ref="S21:V21"/>
-    <mergeCell ref="AL15:AS15"/>
   </mergeCells>
   <conditionalFormatting sqref="A51:AT73">
     <cfRule type="expression" dxfId="5" priority="4">
@@ -8920,7 +8920,7 @@
       <formula>LEN(TRIM(B8))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="9">
+  <dataValidations count="8">
     <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Opa!!" error="Digíte somente números!!" sqref="F3" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>1</formula1>
     </dataValidation>
@@ -8928,14 +8928,13 @@
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="III - Muito Graves, aquelas em que forem verificadas duas circunstâncias agravantes;" sqref="X72" xr:uid="{00000000-0002-0000-0000-000002000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="II - Graves, aquelas em que for verificada uma circunstância agravante;" sqref="L72" xr:uid="{00000000-0002-0000-0000-000003000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="I - Leves, aquelas em que o infrator seja beneficiado por circunstâncias atenuantes;" sqref="B72" xr:uid="{00000000-0002-0000-0000-000004000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" sqref="E26:J26" xr:uid="{00000000-0002-0000-0000-000006000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" sqref="E26:J26 E17:J17" xr:uid="{00000000-0002-0000-0000-000006000000}"/>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S21:V21" xr:uid="{00000000-0002-0000-0000-000007000000}">
       <formula1>"SIM,NÃO"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="B8:AS8" xr:uid="{00000000-0002-0000-0000-000008000000}">
       <formula1>"N/A"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" sqref="E17:J17" xr:uid="{68F80EDD-65B4-466D-A5BE-1AB772BE3762}"/>
   </dataValidations>
   <pageMargins left="0.51181102362204722" right="0.51181102362204722" top="0.78740157480314965" bottom="0.78740157480314965" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="93" fitToHeight="0" orientation="portrait" r:id="rId1"/>

</xml_diff>